<commit_message>
* reverted RoleToAccessProfile changes * caseFlags working now
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.reeve/et-ccd-definitions-scotland/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jack\et-ccd-definitions-scotland\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512C7ECC-FDF7-364C-B742-DC59679EF371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A23205-63EE-4767-AAE4-18BF4D44F404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" tabRatio="500" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24450" yWindow="4455" windowWidth="35070" windowHeight="15555" tabRatio="500" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CaseRoles" sheetId="30" r:id="rId1"/>
@@ -24,24 +24,23 @@
     <sheet name="ChallengeQuestion" sheetId="31" r:id="rId9"/>
     <sheet name="ComplexTypes" sheetId="9" r:id="rId10"/>
     <sheet name="EventToComplexTypes" sheetId="32" r:id="rId11"/>
-    <sheet name="RoleToAccessProfiles" sheetId="33" r:id="rId12"/>
-    <sheet name="Scotland Scrubbed" sheetId="26" r:id="rId13"/>
-    <sheet name="SearchInputFields" sheetId="12" r:id="rId14"/>
-    <sheet name="WorkBasketInputFields" sheetId="14" r:id="rId15"/>
-    <sheet name="SearchResultFields" sheetId="13" r:id="rId16"/>
-    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId17"/>
-    <sheet name="SearchCaseResultFields" sheetId="22" r:id="rId18"/>
-    <sheet name="UserProfile" sheetId="16" r:id="rId19"/>
-    <sheet name="AuthorisationComplexType" sheetId="17" r:id="rId20"/>
-    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId21"/>
-    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId22"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId23"/>
-    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId24"/>
+    <sheet name="Scotland Scrubbed" sheetId="26" r:id="rId12"/>
+    <sheet name="SearchInputFields" sheetId="12" r:id="rId13"/>
+    <sheet name="WorkBasketInputFields" sheetId="14" r:id="rId14"/>
+    <sheet name="SearchResultFields" sheetId="13" r:id="rId15"/>
+    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId16"/>
+    <sheet name="SearchCaseResultFields" sheetId="22" r:id="rId17"/>
+    <sheet name="UserProfile" sheetId="16" r:id="rId18"/>
+    <sheet name="AuthorisationComplexType" sheetId="17" r:id="rId19"/>
+    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId20"/>
+    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId21"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId22"/>
+    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId23"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseField!$A$1:$D$517</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseField!$A$1:$D$517</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">CaseEvent!$A$3:$Z$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CaseEventToFields!$A$3:$P$231</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseField!$A$3:$U$3</definedName>
@@ -49,7 +48,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">CaseTypeTab!$A$3:$P$54</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">ComplexTypes!$A$3:$W$559</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">EventToComplexTypes!$A$3:$I$382</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Scotland Scrubbed'!$A$3:$F$646</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Scotland Scrubbed'!$A$3:$F$646</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">State!$A$3:$Q$11</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
@@ -70,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="352">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1200,27 +1199,6 @@
   </si>
   <si>
     <t>DefaultValue</t>
-  </si>
-  <si>
-    <t>RoleToAccessProfiles</t>
-  </si>
-  <si>
-    <t>RoleName</t>
-  </si>
-  <si>
-    <t>CaseAccessCategories</t>
-  </si>
-  <si>
-    <t>Authorisation</t>
-  </si>
-  <si>
-    <t>ReadOnly</t>
-  </si>
-  <si>
-    <t>AccessProfiles</t>
-  </si>
-  <si>
-    <t>Disabled</t>
   </si>
 </sst>
 </file>
@@ -2926,17 +2904,17 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" style="133" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="133" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" style="133" customWidth="1"/>
-    <col min="4" max="4" width="28.5" style="133" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" style="133" customWidth="1"/>
-    <col min="6" max="6" width="22.83203125" style="133" customWidth="1"/>
-    <col min="7" max="7" width="24.5" style="133" customWidth="1"/>
-    <col min="8" max="1025" width="8.83203125" style="133" customWidth="1"/>
-    <col min="1026" max="16384" width="8.83203125" style="133"/>
+    <col min="1" max="1" width="16.140625" style="133" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="133" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="133" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" style="133" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="133" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" style="133" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" style="133" customWidth="1"/>
+    <col min="8" max="1025" width="8.85546875" style="133" customWidth="1"/>
+    <col min="1026" max="16384" width="8.85546875" style="133"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1">
@@ -2955,7 +2933,7 @@
       <c r="E1" s="240"/>
       <c r="F1" s="240"/>
     </row>
-    <row r="2" spans="1:6" s="236" customFormat="1" ht="42">
+    <row r="2" spans="1:6" s="236" customFormat="1" ht="38.25">
       <c r="A2" s="239" t="s">
         <v>4</v>
       </c>
@@ -2975,7 +2953,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.75" customHeight="1">
+    <row r="3" spans="1:6" ht="13.7" customHeight="1">
       <c r="A3" s="233" t="s">
         <v>9</v>
       </c>
@@ -2995,28 +2973,28 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.75" customHeight="1">
+    <row r="4" spans="1:6" ht="13.7" customHeight="1">
       <c r="A4" s="232"/>
       <c r="B4" s="232"/>
     </row>
-    <row r="5" spans="1:6" ht="13.75" customHeight="1">
+    <row r="5" spans="1:6" ht="13.7" customHeight="1">
       <c r="A5" s="232"/>
       <c r="B5" s="232"/>
     </row>
-    <row r="6" spans="1:6" ht="13.75" customHeight="1">
+    <row r="6" spans="1:6" ht="13.7" customHeight="1">
       <c r="A6" s="232"/>
       <c r="B6" s="232"/>
     </row>
-    <row r="7" spans="1:6" ht="13.75" customHeight="1">
+    <row r="7" spans="1:6" ht="13.7" customHeight="1">
       <c r="A7" s="232"/>
       <c r="B7" s="232"/>
     </row>
-    <row r="8" spans="1:6" ht="13.75" customHeight="1">
+    <row r="8" spans="1:6" ht="13.7" customHeight="1">
       <c r="A8" s="232"/>
       <c r="B8" s="232"/>
     </row>
-    <row r="9" spans="1:6" ht="13.75" customHeight="1"/>
-    <row r="10" spans="1:6" ht="13.75" customHeight="1"/>
+    <row r="9" spans="1:6" ht="13.7" customHeight="1"/>
+    <row r="10" spans="1:6" ht="13.7" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3034,26 +3012,26 @@
       <selection activeCell="A4" sqref="A4:XFD559"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="31.5" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="20.5" style="52" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="41" customWidth="1"/>
-    <col min="7" max="7" width="9.5" style="41" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="52" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="41" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="41" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" style="53" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" style="53" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="53" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="53" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="28.33203125" customWidth="1"/>
-    <col min="16" max="23" width="6.33203125" customWidth="1"/>
-    <col min="24" max="1023" width="8.33203125" customWidth="1"/>
-    <col min="1024" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="15" max="15" width="28.28515625" customWidth="1"/>
+    <col min="16" max="23" width="6.28515625" customWidth="1"/>
+    <col min="24" max="1023" width="8.28515625" customWidth="1"/>
+    <col min="1024" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="18" customHeight="1">
@@ -3082,7 +3060,7 @@
       <c r="P1" s="36"/>
       <c r="Q1" s="36"/>
     </row>
-    <row r="2" spans="1:23" ht="65" customHeight="1">
+    <row r="2" spans="1:23" ht="65.099999999999994" customHeight="1">
       <c r="A2" s="25" t="s">
         <v>113</v>
       </c>
@@ -3123,7 +3101,7 @@
       <c r="P2" s="10"/>
       <c r="Q2" s="10"/>
     </row>
-    <row r="3" spans="1:23" s="2" customFormat="1" ht="33.5" customHeight="1">
+    <row r="3" spans="1:23" s="2" customFormat="1" ht="33.6" customHeight="1">
       <c r="A3" s="27" t="s">
         <v>11</v>
       </c>
@@ -5264,7 +5242,7 @@
       <c r="I278"/>
       <c r="J278"/>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:10" ht="13.5">
       <c r="B279" s="231"/>
       <c r="E279"/>
       <c r="F279" s="108"/>
@@ -6803,7 +6781,7 @@
       <c r="G488" s="219"/>
       <c r="H488" s="193"/>
     </row>
-    <row r="489" spans="1:8">
+    <row r="489" spans="1:8" ht="13.5">
       <c r="A489" s="56"/>
       <c r="B489" s="231"/>
       <c r="C489" s="56"/>
@@ -6813,7 +6791,7 @@
       <c r="G489" s="219"/>
       <c r="H489" s="193"/>
     </row>
-    <row r="490" spans="1:8">
+    <row r="490" spans="1:8" ht="13.5">
       <c r="A490" s="56"/>
       <c r="B490" s="231"/>
       <c r="C490" s="56"/>
@@ -6823,7 +6801,7 @@
       <c r="G490" s="219"/>
       <c r="H490" s="193"/>
     </row>
-    <row r="491" spans="1:8">
+    <row r="491" spans="1:8" ht="13.5">
       <c r="A491" s="56"/>
       <c r="B491" s="231"/>
       <c r="C491" s="56"/>
@@ -7653,21 +7631,21 @@
       <selection pane="bottomLeft" activeCell="E369" sqref="E369"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.5" customWidth="1"/>
-    <col min="6" max="6" width="50.1640625" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
-    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.42578125" customWidth="1"/>
+    <col min="6" max="6" width="50.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="40" customHeight="1">
+    <row r="1" spans="1:11" ht="39.950000000000003" customHeight="1">
       <c r="A1" s="282" t="s">
         <v>120</v>
       </c>
@@ -7686,7 +7664,7 @@
       <c r="H1" s="278"/>
       <c r="I1" s="277"/>
     </row>
-    <row r="2" spans="1:11" ht="67" customHeight="1">
+    <row r="2" spans="1:11" ht="66.95" customHeight="1">
       <c r="A2" s="275" t="s">
         <v>121</v>
       </c>
@@ -13868,89 +13846,28 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61D48D4-7617-864E-81CB-58F1828F347E}">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="143" t="s">
-        <v>352</v>
-      </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="H1" s="143"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="143"/>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="G2" s="143"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="143" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="143" t="s">
-        <v>353</v>
-      </c>
-      <c r="C3" s="143" t="s">
-        <v>354</v>
-      </c>
-      <c r="D3" s="143" t="s">
-        <v>355</v>
-      </c>
-      <c r="E3" s="143" t="s">
-        <v>356</v>
-      </c>
-      <c r="F3" s="143" t="s">
-        <v>357</v>
-      </c>
-      <c r="G3" s="143" t="s">
-        <v>358</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEDE50F-3952-214F-9597-838D9D10B1E0}">
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
   <dimension ref="A1:K650"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD650"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" style="151" customWidth="1"/>
-    <col min="2" max="2" width="61.6640625" style="171" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" style="151" customWidth="1"/>
+    <col min="2" max="2" width="61.7109375" style="171" customWidth="1"/>
     <col min="3" max="3" width="65" style="151" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="151" customWidth="1"/>
-    <col min="5" max="6" width="8.6640625" style="151"/>
+    <col min="4" max="4" width="14.7109375" style="151" customWidth="1"/>
+    <col min="5" max="6" width="8.7109375" style="151"/>
     <col min="7" max="7" width="13" style="151" customWidth="1"/>
-    <col min="8" max="8" width="11.5" style="151" customWidth="1"/>
-    <col min="9" max="12" width="8.6640625" style="151"/>
-    <col min="13" max="13" width="16.33203125" style="151" customWidth="1"/>
-    <col min="14" max="16384" width="8.6640625" style="151"/>
+    <col min="8" max="8" width="11.42578125" style="151" customWidth="1"/>
+    <col min="9" max="12" width="8.7109375" style="151"/>
+    <col min="13" max="13" width="16.28515625" style="151" customWidth="1"/>
+    <col min="14" max="16384" width="8.7109375" style="151"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18">
@@ -13967,7 +13884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="56">
+    <row r="2" spans="1:11" ht="51">
       <c r="A2" s="152" t="s">
         <v>129</v>
       </c>
@@ -16824,7 +16741,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
@@ -16832,22 +16749,22 @@
       <selection activeCell="A4" sqref="A4:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="32.5" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
-    <col min="7" max="7" width="43.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" customWidth="1"/>
-    <col min="9" max="9" width="31.5" customWidth="1"/>
-    <col min="10" max="10" width="21.6640625" customWidth="1"/>
-    <col min="11" max="11" width="6.33203125" customWidth="1"/>
-    <col min="12" max="1025" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="32.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="43.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="31.42578125" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" customWidth="1"/>
+    <col min="12" max="1025" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="19">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="36">
       <c r="A1" s="69" t="s">
         <v>134</v>
       </c>
@@ -16865,7 +16782,7 @@
       <c r="G1" s="73"/>
       <c r="H1" s="186"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="71">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="75">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
@@ -17077,6 +16994,138 @@
     <row r="37" spans="5:7">
       <c r="E37" s="1"/>
       <c r="G37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" customWidth="1"/>
+    <col min="9" max="1023" width="8.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18.75">
+      <c r="A1" s="80" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="82" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="84"/>
+    </row>
+    <row r="2" spans="1:8" ht="89.25">
+      <c r="A2" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="126" t="s">
+        <v>170</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15">
+      <c r="A3" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="74" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="74" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="127" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="127" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15">
+      <c r="D4"/>
+      <c r="E4" s="1"/>
+      <c r="G4" s="68"/>
+    </row>
+    <row r="5" spans="1:8" ht="15">
+      <c r="D5" s="111"/>
+      <c r="E5" s="1"/>
+      <c r="G5" s="68"/>
+    </row>
+    <row r="6" spans="1:8" ht="14.25">
+      <c r="D6" s="112"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="15">
+      <c r="D7"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="187"/>
+    </row>
+    <row r="8" spans="1:8" ht="14.25">
+      <c r="B8" s="108"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="B9" s="108"/>
+      <c r="D9"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="D10"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="D11"/>
+      <c r="E11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -17088,66 +17137,70 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.5" customWidth="1"/>
-    <col min="9" max="1023" width="8.5" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" customWidth="1"/>
+    <col min="8" max="1023" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="80" t="s">
-        <v>142</v>
-      </c>
-      <c r="B1" s="81" t="s">
+    <row r="1" spans="1:15" ht="36">
+      <c r="A1" s="69" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="83" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="84"/>
-    </row>
-    <row r="2" spans="1:8" ht="84">
+      <c r="E1" s="39"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+    </row>
+    <row r="2" spans="1:15" ht="90">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" s="126" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" s="123" t="s">
         <v>170</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15">
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+    </row>
+    <row r="3" spans="1:15" ht="15">
       <c r="A3" s="74" t="s">
         <v>32</v>
       </c>
@@ -17163,52 +17216,54 @@
       <c r="E3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="127" t="s">
-        <v>51</v>
+      <c r="F3" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="127" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15">
-      <c r="D4"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="E4" s="1"/>
-      <c r="G4" s="68"/>
-    </row>
-    <row r="5" spans="1:8" ht="15">
-      <c r="D5" s="111"/>
+    </row>
+    <row r="5" spans="1:15" ht="15">
       <c r="E5" s="1"/>
-      <c r="G5" s="68"/>
-    </row>
-    <row r="6" spans="1:8" ht="14">
-      <c r="D6" s="112"/>
+      <c r="F5" s="187"/>
+    </row>
+    <row r="6" spans="1:15">
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="15">
-      <c r="D7"/>
+    <row r="7" spans="1:15">
       <c r="E7" s="1"/>
-      <c r="F7" s="187"/>
-    </row>
-    <row r="8" spans="1:8" ht="14">
-      <c r="B8" s="108"/>
-      <c r="D8" s="112"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:15">
       <c r="B9" s="108"/>
-      <c r="D9"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:8">
-      <c r="D10"/>
+    <row r="10" spans="1:15">
+      <c r="B10" s="108"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:8">
-      <c r="D11"/>
+    <row r="11" spans="1:15">
+      <c r="B11" s="108"/>
       <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="E13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -17220,46 +17275,46 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:O13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD13"/>
+      <selection activeCell="A4" sqref="A4:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="32.5" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1"/>
-    <col min="8" max="1023" width="11.5"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="50" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" customWidth="1"/>
+    <col min="8" max="14" width="6.28515625" customWidth="1"/>
+    <col min="15" max="1023" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="19">
-      <c r="A1" s="69" t="s">
-        <v>138</v>
-      </c>
-      <c r="B1" s="75" t="s">
+    <row r="1" spans="1:14" ht="18">
+      <c r="A1" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-    </row>
-    <row r="2" spans="1:15" ht="80">
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+    </row>
+    <row r="2" spans="1:14" ht="105">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
@@ -17267,7 +17322,7 @@
         <v>139</v>
       </c>
       <c r="C2" s="24"/>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="113" t="s">
         <v>140</v>
       </c>
       <c r="E2" s="24" t="s">
@@ -17279,11 +17334,10 @@
       <c r="G2" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-    </row>
-    <row r="3" spans="1:15" ht="15">
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+    </row>
+    <row r="3" spans="1:14" ht="15">
       <c r="A3" s="74" t="s">
         <v>32</v>
       </c>
@@ -17293,7 +17347,7 @@
       <c r="C3" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="114" t="s">
         <v>105</v>
       </c>
       <c r="E3" s="12" t="s">
@@ -17312,41 +17366,41 @@
       <c r="L3" s="79"/>
       <c r="M3" s="79"/>
       <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
-    </row>
-    <row r="4" spans="1:15">
+    </row>
+    <row r="4" spans="1:14">
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="15">
+    <row r="5" spans="1:14">
       <c r="E5" s="1"/>
-      <c r="F5" s="187"/>
-    </row>
-    <row r="6" spans="1:15">
+    </row>
+    <row r="6" spans="1:14">
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:14">
+      <c r="D7"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:14">
+      <c r="D8"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:14">
       <c r="B9" s="108"/>
+      <c r="D9"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:14">
       <c r="B10" s="108"/>
+      <c r="D10"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:15">
-      <c r="B11" s="108"/>
+    <row r="11" spans="1:14">
+      <c r="D11"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:14">
+      <c r="D12"/>
       <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="E13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -17358,143 +17412,6 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:N12"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
-  <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="25.5" customWidth="1"/>
-    <col min="8" max="14" width="6.33203125" customWidth="1"/>
-    <col min="15" max="1023" width="8.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="18">
-      <c r="A1" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-    </row>
-    <row r="2" spans="1:14" ht="96">
-      <c r="A2" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="113" t="s">
-        <v>140</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="F2" s="123" t="s">
-        <v>170</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-    </row>
-    <row r="3" spans="1:14" ht="15">
-      <c r="A3" s="74" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="74" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="74" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" s="114" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="D7"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="D8"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="B9" s="108"/>
-      <c r="D9"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="B10" s="108"/>
-      <c r="D10"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="D11"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="D12"/>
-      <c r="E12" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E55ACB-56A8-B541-931E-FA903DDDD8CF}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -17502,18 +17419,18 @@
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="133" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" style="133" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="133" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="133" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="133" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" style="133" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" style="133" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="133" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="133" customWidth="1"/>
-    <col min="10" max="16384" width="10.6640625" style="133"/>
+    <col min="1" max="1" width="13.28515625" style="133" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="133" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="133" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="133" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="133" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="133" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="133" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="133" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="133" customWidth="1"/>
+    <col min="10" max="16384" width="10.7109375" style="133"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18">
@@ -17535,7 +17452,7 @@
       <c r="H1" s="132"/>
       <c r="I1" s="132"/>
     </row>
-    <row r="2" spans="1:9" ht="42">
+    <row r="2" spans="1:9" ht="38.25">
       <c r="A2" s="134"/>
       <c r="B2" s="134"/>
       <c r="C2" s="135" t="s">
@@ -17657,7 +17574,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -17665,14 +17582,14 @@
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="11.5"/>
-    <col min="3" max="3" width="35.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="1" max="2" width="11.42578125"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="1025" width="11.5"/>
+    <col min="7" max="1025" width="11.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18">
@@ -17696,7 +17613,7 @@
       <c r="J1" s="36"/>
       <c r="K1" s="36"/>
     </row>
-    <row r="2" spans="1:11" ht="70">
+    <row r="2" spans="1:11" ht="63.75">
       <c r="A2" s="23" t="s">
         <v>4</v>
       </c>
@@ -17719,7 +17636,7 @@
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
     </row>
-    <row r="3" spans="1:11" ht="28">
+    <row r="3" spans="1:11" ht="38.25">
       <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
@@ -17754,108 +17671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N4"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
-  <cols>
-    <col min="1" max="2" width="11.5"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
-    <col min="4" max="1024" width="11.5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="18">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:14" ht="126">
-      <c r="A2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="147" t="s">
-        <v>179</v>
-      </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="F4" s="108"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:IU148"/>
   <sheetViews>
@@ -17863,15 +17679,15 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="50.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="45.6640625" customWidth="1"/>
-    <col min="7" max="1025" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="50.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+    <col min="7" max="1025" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:255" ht="18" customHeight="1">
@@ -18139,7 +17955,7 @@
       <c r="IT1" s="36"/>
       <c r="IU1" s="36"/>
     </row>
-    <row r="2" spans="1:255" ht="196">
+    <row r="2" spans="1:255" ht="191.25">
       <c r="A2" s="23"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24" t="s">
@@ -18908,7 +18724,108 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N4"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="2" width="11.42578125"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="1024" width="11.42578125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="18">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:14" ht="127.5">
+      <c r="A2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="147" t="s">
+        <v>179</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="F4" s="108"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:IU10"/>
   <sheetViews>
@@ -18916,14 +18833,14 @@
       <selection activeCell="A4" sqref="A4:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="50.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="1" customWidth="1"/>
-    <col min="6" max="1025" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="50.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
+    <col min="6" max="1025" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:255" ht="18" customHeight="1">
@@ -19191,7 +19108,7 @@
       <c r="IT1" s="36"/>
       <c r="IU1" s="36"/>
     </row>
-    <row r="2" spans="1:255" ht="84">
+    <row r="2" spans="1:255" ht="89.25">
       <c r="A2" s="23" t="s">
         <v>4</v>
       </c>
@@ -19521,7 +19438,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:D518"/>
   <sheetViews>
@@ -19529,14 +19446,14 @@
       <selection activeCell="A4" sqref="A4:XFD518"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.5" customWidth="1"/>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" style="1" customWidth="1"/>
-    <col min="5" max="1011" width="8.33203125" customWidth="1"/>
-    <col min="1012" max="1016" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="1" customWidth="1"/>
+    <col min="5" max="1011" width="8.28515625" customWidth="1"/>
+    <col min="1012" max="1016" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -19553,7 +19470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="56">
+    <row r="2" spans="1:4" ht="51">
       <c r="A2" s="24" t="s">
         <v>153</v>
       </c>
@@ -21265,7 +21182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:D109"/>
   <sheetViews>
@@ -21273,12 +21190,12 @@
       <selection activeCell="A4" sqref="A4:XFD115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -21295,7 +21212,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="56">
+    <row r="2" spans="1:4" ht="63.75">
       <c r="A2" s="24" t="s">
         <v>160</v>
       </c>
@@ -21694,7 +21611,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -21702,12 +21619,12 @@
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="53.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="53.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -21724,7 +21641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="56">
+    <row r="2" spans="1:4" ht="51">
       <c r="A2" s="24" t="s">
         <v>153</v>
       </c>
@@ -21902,14 +21819,14 @@
       <selection activeCell="A4" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="11.5"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="1" max="2" width="11.42578125"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
     <col min="4" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="61.33203125" customWidth="1"/>
-    <col min="8" max="1025" width="11.5"/>
+    <col min="7" max="7" width="61.28515625" customWidth="1"/>
+    <col min="8" max="1025" width="11.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18">
@@ -21936,7 +21853,7 @@
       <c r="M1" s="22"/>
       <c r="N1" s="22"/>
     </row>
-    <row r="2" spans="1:19" ht="196">
+    <row r="2" spans="1:19" ht="178.5">
       <c r="A2" s="23" t="s">
         <v>4</v>
       </c>
@@ -21970,7 +21887,7 @@
       <c r="M2" s="26"/>
       <c r="N2" s="26"/>
     </row>
-    <row r="3" spans="1:19" ht="42">
+    <row r="3" spans="1:19" ht="38.25">
       <c r="A3" s="27" t="s">
         <v>9</v>
       </c>
@@ -22050,14 +21967,14 @@
       <selection activeCell="A4" sqref="A4:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.5" customWidth="1"/>
-    <col min="2" max="3" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="3" width="21.28515625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="11.5"/>
-    <col min="6" max="6" width="35.33203125" customWidth="1"/>
-    <col min="7" max="1023" width="11.5"/>
+    <col min="5" max="5" width="11.42578125"/>
+    <col min="6" max="6" width="35.28515625" customWidth="1"/>
+    <col min="7" max="1023" width="11.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18">
@@ -22082,7 +21999,7 @@
       <c r="K1" s="22"/>
       <c r="L1" s="22"/>
     </row>
-    <row r="2" spans="1:17" ht="98">
+    <row r="2" spans="1:17" ht="89.25">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
@@ -22108,7 +22025,7 @@
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
     </row>
-    <row r="3" spans="1:17" ht="28">
+    <row r="3" spans="1:17" ht="25.5">
       <c r="A3" s="28" t="s">
         <v>32</v>
       </c>
@@ -22210,19 +22127,19 @@
       <selection activeCell="A4" sqref="A4:XFD98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
     <col min="9" max="9" width="31" customWidth="1"/>
-    <col min="10" max="10" width="26.33203125" customWidth="1"/>
-    <col min="11" max="1023" width="8.6640625" customWidth="1"/>
+    <col min="10" max="10" width="26.28515625" customWidth="1"/>
+    <col min="11" max="1023" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18">
@@ -22280,7 +22197,7 @@
       <c r="K2" s="36"/>
       <c r="L2" s="36"/>
     </row>
-    <row r="3" spans="1:16" ht="42">
+    <row r="3" spans="1:16" ht="38.25">
       <c r="A3" s="40" t="s">
         <v>32</v>
       </c>
@@ -22860,29 +22777,29 @@
       <selection activeCell="A4" sqref="A4:XFD54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="42.33203125" customWidth="1"/>
-    <col min="8" max="8" width="74.6640625" customWidth="1"/>
-    <col min="9" max="9" width="83.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="79.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="88.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="23.33203125" customWidth="1"/>
-    <col min="14" max="14" width="8.5" customWidth="1"/>
-    <col min="15" max="15" width="18.5" customWidth="1"/>
-    <col min="16" max="16" width="18.5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.33203125" customWidth="1"/>
-    <col min="18" max="18" width="20.5" customWidth="1"/>
-    <col min="19" max="19" width="17.6640625" customWidth="1"/>
-    <col min="20" max="30" width="8.5" customWidth="1"/>
-    <col min="31" max="1024" width="8.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" customWidth="1"/>
+    <col min="8" max="8" width="74.7109375" customWidth="1"/>
+    <col min="9" max="9" width="83.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="88.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="23.28515625" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" customWidth="1"/>
+    <col min="18" max="18" width="20.42578125" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" customWidth="1"/>
+    <col min="20" max="30" width="8.42578125" customWidth="1"/>
+    <col min="31" max="1024" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">
@@ -22914,7 +22831,7 @@
       <c r="R1" s="39"/>
       <c r="S1" s="39"/>
     </row>
-    <row r="2" spans="1:26" ht="126">
+    <row r="2" spans="1:26" ht="127.5">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
@@ -22955,7 +22872,7 @@
       <c r="R2" s="25"/>
       <c r="S2" s="25"/>
     </row>
-    <row r="3" spans="1:26" ht="42">
+    <row r="3" spans="1:26" ht="38.25">
       <c r="A3" s="40" t="s">
         <v>32</v>
       </c>
@@ -23021,14 +22938,14 @@
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
     </row>
-    <row r="4" spans="1:26" ht="14">
+    <row r="4" spans="1:26" ht="14.25">
       <c r="I4" s="107"/>
       <c r="L4" s="36"/>
       <c r="M4" s="46"/>
       <c r="R4" s="109"/>
       <c r="S4" s="109"/>
     </row>
-    <row r="5" spans="1:26" ht="14">
+    <row r="5" spans="1:26" ht="14.25">
       <c r="F5" s="2"/>
       <c r="J5" s="107"/>
       <c r="K5" s="36"/>
@@ -23037,7 +22954,7 @@
       <c r="R5" s="109"/>
       <c r="S5" s="109"/>
     </row>
-    <row r="6" spans="1:26" ht="14">
+    <row r="6" spans="1:26" ht="14.25">
       <c r="F6" s="2"/>
       <c r="G6" s="143"/>
       <c r="I6" s="188"/>
@@ -23047,7 +22964,7 @@
       <c r="R6" s="109"/>
       <c r="S6" s="109"/>
     </row>
-    <row r="7" spans="1:26" ht="14">
+    <row r="7" spans="1:26" ht="14.25">
       <c r="F7" s="2"/>
       <c r="G7" s="218"/>
       <c r="H7" s="2"/>
@@ -23058,7 +22975,7 @@
       <c r="R7" s="109"/>
       <c r="S7" s="109"/>
     </row>
-    <row r="8" spans="1:26" ht="14">
+    <row r="8" spans="1:26" ht="14.25">
       <c r="F8" s="2"/>
       <c r="G8" s="218"/>
       <c r="H8" s="2"/>
@@ -23069,7 +22986,7 @@
       <c r="R8" s="109"/>
       <c r="S8" s="109"/>
     </row>
-    <row r="9" spans="1:26" ht="14">
+    <row r="9" spans="1:26" ht="14.25">
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -23081,7 +22998,7 @@
       <c r="R9" s="109"/>
       <c r="S9" s="109"/>
     </row>
-    <row r="10" spans="1:26" ht="14">
+    <row r="10" spans="1:26" ht="14.25">
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -23093,7 +23010,7 @@
       <c r="R10" s="109"/>
       <c r="S10" s="109"/>
     </row>
-    <row r="11" spans="1:26" ht="14">
+    <row r="11" spans="1:26" ht="14.25">
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -23105,7 +23022,7 @@
       <c r="R11" s="109"/>
       <c r="S11" s="109"/>
     </row>
-    <row r="12" spans="1:26" ht="14">
+    <row r="12" spans="1:26" ht="14.25">
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -23117,7 +23034,7 @@
       <c r="R12" s="109"/>
       <c r="S12" s="109"/>
     </row>
-    <row r="13" spans="1:26" ht="14">
+    <row r="13" spans="1:26" ht="14.25">
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -23129,7 +23046,7 @@
       <c r="R13" s="109"/>
       <c r="S13" s="109"/>
     </row>
-    <row r="14" spans="1:26" ht="14">
+    <row r="14" spans="1:26" ht="14.25">
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -23141,7 +23058,7 @@
       <c r="R14" s="109"/>
       <c r="S14" s="109"/>
     </row>
-    <row r="15" spans="1:26" ht="14">
+    <row r="15" spans="1:26" ht="14.25">
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -23153,7 +23070,7 @@
       <c r="R15" s="109"/>
       <c r="S15" s="109"/>
     </row>
-    <row r="16" spans="1:26" ht="14">
+    <row r="16" spans="1:26" ht="14.25">
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -23165,7 +23082,7 @@
       <c r="R16" s="109"/>
       <c r="S16" s="109"/>
     </row>
-    <row r="17" spans="6:19" ht="14">
+    <row r="17" spans="6:19" ht="14.25">
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -23177,7 +23094,7 @@
       <c r="R17" s="109"/>
       <c r="S17" s="109"/>
     </row>
-    <row r="18" spans="6:19" ht="14">
+    <row r="18" spans="6:19" ht="14.25">
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -23188,7 +23105,7 @@
       <c r="R18" s="109"/>
       <c r="S18" s="109"/>
     </row>
-    <row r="19" spans="6:19" ht="14">
+    <row r="19" spans="6:19" ht="14.25">
       <c r="F19" s="2"/>
       <c r="I19" s="115"/>
       <c r="J19" s="141"/>
@@ -23198,7 +23115,7 @@
       <c r="R19" s="109"/>
       <c r="S19" s="109"/>
     </row>
-    <row r="20" spans="6:19" ht="14">
+    <row r="20" spans="6:19" ht="14.25">
       <c r="F20" s="2"/>
       <c r="I20" s="107"/>
       <c r="J20" s="107"/>
@@ -23207,7 +23124,7 @@
       <c r="R20" s="109"/>
       <c r="S20" s="109"/>
     </row>
-    <row r="21" spans="6:19" ht="14">
+    <row r="21" spans="6:19" ht="14.25">
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -23218,7 +23135,7 @@
       <c r="R21" s="109"/>
       <c r="S21" s="109"/>
     </row>
-    <row r="22" spans="6:19" ht="14">
+    <row r="22" spans="6:19" ht="14.25">
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -23230,7 +23147,7 @@
       <c r="R22" s="109"/>
       <c r="S22" s="109"/>
     </row>
-    <row r="23" spans="6:19" ht="14">
+    <row r="23" spans="6:19" ht="14.25">
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -23242,7 +23159,7 @@
       <c r="R23" s="109"/>
       <c r="S23" s="109"/>
     </row>
-    <row r="24" spans="6:19" ht="14">
+    <row r="24" spans="6:19" ht="14.25">
       <c r="J24" s="33"/>
       <c r="L24" s="36"/>
       <c r="M24" s="46"/>
@@ -23250,7 +23167,7 @@
       <c r="R24" s="109"/>
       <c r="S24" s="109"/>
     </row>
-    <row r="25" spans="6:19" ht="14">
+    <row r="25" spans="6:19" ht="14.25">
       <c r="F25" s="2"/>
       <c r="I25" s="107"/>
       <c r="J25" s="107"/>
@@ -23261,7 +23178,7 @@
       <c r="R25" s="109"/>
       <c r="S25" s="109"/>
     </row>
-    <row r="26" spans="6:19" ht="14">
+    <row r="26" spans="6:19" ht="14.25">
       <c r="F26" s="2"/>
       <c r="J26" s="107"/>
       <c r="K26" s="107"/>
@@ -23271,7 +23188,7 @@
       <c r="R26" s="109"/>
       <c r="S26" s="109"/>
     </row>
-    <row r="27" spans="6:19" ht="14">
+    <row r="27" spans="6:19" ht="14.25">
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="I27" s="107"/>
@@ -23282,7 +23199,7 @@
       <c r="R27" s="109"/>
       <c r="S27" s="109"/>
     </row>
-    <row r="28" spans="6:19" ht="14">
+    <row r="28" spans="6:19" ht="14.25">
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="I28" s="107"/>
@@ -23293,7 +23210,7 @@
       <c r="R28" s="109"/>
       <c r="S28" s="109"/>
     </row>
-    <row r="29" spans="6:19" ht="14">
+    <row r="29" spans="6:19" ht="14.25">
       <c r="F29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="107"/>
@@ -23304,7 +23221,7 @@
       <c r="R29" s="109"/>
       <c r="S29" s="109"/>
     </row>
-    <row r="30" spans="6:19" ht="14">
+    <row r="30" spans="6:19" ht="14.25">
       <c r="G30" s="2"/>
       <c r="I30" s="188"/>
       <c r="J30" s="107"/>
@@ -23314,7 +23231,7 @@
       <c r="R30" s="109"/>
       <c r="S30" s="109"/>
     </row>
-    <row r="31" spans="6:19" ht="14">
+    <row r="31" spans="6:19" ht="14.25">
       <c r="J31" s="107"/>
       <c r="K31" s="107"/>
       <c r="L31" s="36"/>
@@ -23323,7 +23240,7 @@
       <c r="R31" s="109"/>
       <c r="S31" s="109"/>
     </row>
-    <row r="32" spans="6:19" ht="14">
+    <row r="32" spans="6:19" ht="14.25">
       <c r="G32" s="2"/>
       <c r="J32" s="107"/>
       <c r="K32" s="107"/>
@@ -23333,7 +23250,7 @@
       <c r="R32" s="109"/>
       <c r="S32" s="109"/>
     </row>
-    <row r="33" spans="1:19" ht="14">
+    <row r="33" spans="1:19" ht="14.25">
       <c r="H33" s="145"/>
       <c r="I33" s="107"/>
       <c r="J33" s="110"/>
@@ -23343,7 +23260,7 @@
       <c r="R33" s="36"/>
       <c r="S33" s="36"/>
     </row>
-    <row r="34" spans="1:19" ht="14">
+    <row r="34" spans="1:19" ht="14.25">
       <c r="I34" s="107"/>
       <c r="J34" s="107"/>
       <c r="L34" s="36"/>
@@ -23447,7 +23364,7 @@
       <c r="R45" s="109"/>
       <c r="S45" s="32"/>
     </row>
-    <row r="46" spans="1:19" ht="14">
+    <row r="46" spans="1:19" ht="14.25">
       <c r="A46" s="120"/>
       <c r="F46" s="111"/>
       <c r="I46" s="107"/>
@@ -23542,20 +23459,20 @@
       <selection activeCell="A4" sqref="A4:XFD240"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="7" width="8.6640625" customWidth="1"/>
-    <col min="8" max="8" width="28.6640625" customWidth="1"/>
+    <col min="5" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="90.33203125" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" customWidth="1"/>
-    <col min="14" max="1010" width="8.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="90.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+    <col min="14" max="1010" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18">
@@ -23632,7 +23549,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="56">
+    <row r="3" spans="1:16" ht="51">
       <c r="A3" s="28" t="s">
         <v>32</v>
       </c>
@@ -25616,22 +25533,22 @@
       <selection activeCell="A4" sqref="A4:XFD206"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.6640625" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="26.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.33203125" style="1" customWidth="1"/>
-    <col min="12" max="17" width="8.5" customWidth="1"/>
-    <col min="18" max="21" width="6.33203125" customWidth="1"/>
-    <col min="22" max="1023" width="8.33203125" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" style="1" customWidth="1"/>
+    <col min="12" max="17" width="8.42578125" customWidth="1"/>
+    <col min="18" max="21" width="6.28515625" customWidth="1"/>
+    <col min="22" max="1023" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18">
@@ -26854,20 +26771,20 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" style="246" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="246"/>
-    <col min="3" max="3" width="54.6640625" style="246" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" style="246" customWidth="1"/>
-    <col min="5" max="6" width="12.6640625" style="246" customWidth="1"/>
-    <col min="7" max="7" width="44.33203125" style="246" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" style="246" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" style="246" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="246"/>
+    <col min="3" max="3" width="54.7109375" style="246" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="246" customWidth="1"/>
+    <col min="5" max="6" width="12.7109375" style="246" customWidth="1"/>
+    <col min="7" max="7" width="44.28515625" style="246" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="246" customWidth="1"/>
     <col min="9" max="9" width="37" style="246" customWidth="1"/>
-    <col min="10" max="10" width="43.6640625" style="246" customWidth="1"/>
-    <col min="11" max="11" width="19.1640625" style="246" customWidth="1"/>
-    <col min="12" max="1025" width="10.83203125" style="246"/>
-    <col min="1026" max="16384" width="10.83203125" style="245"/>
+    <col min="10" max="10" width="43.7109375" style="246" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" style="246" customWidth="1"/>
+    <col min="12" max="1025" width="10.85546875" style="246"/>
+    <col min="1026" max="16384" width="10.85546875" style="245"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18">
@@ -26893,7 +26810,7 @@
       <c r="L1" s="247"/>
       <c r="M1" s="247"/>
     </row>
-    <row r="2" spans="1:13" ht="56">
+    <row r="2" spans="1:13" ht="63.75">
       <c r="A2" s="258" t="s">
         <v>4</v>
       </c>
@@ -26928,7 +26845,7 @@
       <c r="L2" s="254"/>
       <c r="M2" s="254"/>
     </row>
-    <row r="3" spans="1:13" ht="16">
+    <row r="3" spans="1:13" ht="15.75">
       <c r="A3" s="253" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Consolidate template columns and tabs
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judgem\Documents\Scotland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9474332B-A8A5-44AD-AB4C-139D012E58CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FD542F-E05E-412B-98A2-66829B25C94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4470" yWindow="-21720" windowWidth="38640" windowHeight="21240" tabRatio="855" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4470" yWindow="-21720" windowWidth="38640" windowHeight="21240" tabRatio="855" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CaseRoles" sheetId="30" r:id="rId1"/>
@@ -24,23 +24,24 @@
     <sheet name="ChallengeQuestion" sheetId="31" r:id="rId9"/>
     <sheet name="ComplexTypes" sheetId="9" r:id="rId10"/>
     <sheet name="EventToComplexTypes" sheetId="32" r:id="rId11"/>
-    <sheet name="Scotland Scrubbed" sheetId="26" r:id="rId12"/>
-    <sheet name="SearchInputFields" sheetId="12" r:id="rId13"/>
-    <sheet name="WorkBasketInputFields" sheetId="14" r:id="rId14"/>
-    <sheet name="SearchResultFields" sheetId="13" r:id="rId15"/>
-    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId16"/>
-    <sheet name="SearchCaseResultFields" sheetId="22" r:id="rId17"/>
-    <sheet name="UserProfile" sheetId="16" r:id="rId18"/>
-    <sheet name="AuthorisationComplexType" sheetId="17" r:id="rId19"/>
-    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId20"/>
-    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId21"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId22"/>
-    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId23"/>
+    <sheet name="RoleToAccessProfiles" sheetId="33" r:id="rId12"/>
+    <sheet name="Scotland Scrubbed" sheetId="26" r:id="rId13"/>
+    <sheet name="SearchInputFields" sheetId="12" r:id="rId14"/>
+    <sheet name="WorkBasketInputFields" sheetId="14" r:id="rId15"/>
+    <sheet name="SearchResultFields" sheetId="13" r:id="rId16"/>
+    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId17"/>
+    <sheet name="SearchCaseResultFields" sheetId="22" r:id="rId18"/>
+    <sheet name="UserProfile" sheetId="16" r:id="rId19"/>
+    <sheet name="AuthorisationComplexType" sheetId="17" r:id="rId20"/>
+    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId21"/>
+    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId22"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId23"/>
+    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId24"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseField!$A$1:$D$517</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseField!$A$1:$D$517</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">CaseEvent!$A$3:$Z$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CaseEventToFields!$A$3:$Q$231</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseField!$A$3:$U$3</definedName>
@@ -48,7 +49,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">CaseTypeTab!$A$3:$P$54</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">ComplexTypes!$A$3:$W$559</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">EventToComplexTypes!$A$3:$I$382</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Scotland Scrubbed'!$A$3:$F$646</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Scotland Scrubbed'!$A$3:$F$646</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">State!$A$3:$Q$11</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="359">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1205,6 +1206,21 @@
   </si>
   <si>
     <t>Boolean value to say if an event can be published</t>
+  </si>
+  <si>
+    <t>AccessProfiles</t>
+  </si>
+  <si>
+    <t>ReadOnly</t>
+  </si>
+  <si>
+    <t>RoleName</t>
+  </si>
+  <si>
+    <t>RoleToAccessProfiles</t>
+  </si>
+  <si>
+    <t>A comma-separated list of AccessProfiles that should be assigned to the user if their RoleName, ReadOnly value (and optional Authorisations) match.</t>
   </si>
 </sst>
 </file>
@@ -1860,7 +1876,7 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="283">
+  <cellXfs count="284">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2411,6 +2427,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -7631,7 +7648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E7B8F4-5285-46EC-BCE1-BF8FCCDC20D1}">
   <dimension ref="A1:L402"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D14" sqref="D14"/>
       <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
@@ -13858,6 +13875,809 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0B9A54-A710-4970-B170-413E5E0036C4}">
+  <dimension ref="A1:E249"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18">
+      <c r="A1" s="35" t="s">
+        <v>357</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="169">
+      <c r="A2" s="239" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.5">
+      <c r="A3" s="233" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="74" t="s">
+        <v>356</v>
+      </c>
+      <c r="D3" s="283" t="s">
+        <v>355</v>
+      </c>
+      <c r="E3" s="283" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="15"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="15"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="15"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="15"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="15"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="15"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="15"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="15"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="15"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="15"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="15"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="15"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="15"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="15"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="15"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="15"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="15"/>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="15"/>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="15"/>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="15"/>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="15"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="15"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="15"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="15"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="15"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="15"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="15"/>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="15"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="15"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="15"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="15"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="15"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="15"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="15"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="15"/>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="15"/>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="15"/>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="15"/>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="15"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="15"/>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="15"/>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="15"/>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="15"/>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="15"/>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="15"/>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="15"/>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="15"/>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="15"/>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="15"/>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="15"/>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="15"/>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="15"/>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="15"/>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="15"/>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="15"/>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="15"/>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="15"/>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="15"/>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="15"/>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="15"/>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="15"/>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="15"/>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="15"/>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="15"/>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="15"/>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="15"/>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="15"/>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="15"/>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="15"/>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="15"/>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="15"/>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="15"/>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="15"/>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="15"/>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="15"/>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="15"/>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="15"/>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="15"/>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="15"/>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="15"/>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="15"/>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="15"/>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="15"/>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="15"/>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="15"/>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="15"/>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="15"/>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="15"/>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="15"/>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="15"/>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="15"/>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="15"/>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="15"/>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="15"/>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="15"/>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="15"/>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="15"/>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="15"/>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="15"/>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="15"/>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="15"/>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="15"/>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="15"/>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="15"/>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="15"/>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="15"/>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="15"/>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="15"/>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="15"/>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="15"/>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="15"/>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="15"/>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="15"/>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="15"/>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="15"/>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="15"/>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="15"/>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="15"/>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="15"/>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="15"/>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="15"/>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="15"/>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="15"/>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="15"/>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="15"/>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="15"/>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="15"/>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="15"/>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="15"/>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="15"/>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="15"/>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="15"/>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="15"/>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="15"/>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="15"/>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" s="15"/>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="15"/>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="15"/>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="15"/>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="15"/>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="15"/>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" s="15"/>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="15"/>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="15"/>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" s="15"/>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="15"/>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" s="15"/>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" s="15"/>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="15"/>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" s="15"/>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" s="15"/>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" s="15"/>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" s="15"/>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" s="15"/>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" s="15"/>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" s="15"/>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" s="15"/>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" s="15"/>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" s="15"/>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" s="15"/>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" s="15"/>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" s="15"/>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" s="15"/>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" s="15"/>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" s="15"/>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" s="15"/>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" s="15"/>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" s="15"/>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" s="15"/>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" s="15"/>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" s="15"/>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" s="15"/>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" s="15"/>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" s="15"/>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" s="15"/>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" s="15"/>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" s="15"/>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" s="15"/>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" s="15"/>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" s="15"/>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" s="15"/>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" s="15"/>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" s="15"/>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" s="15"/>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" s="15"/>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" s="15"/>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" s="15"/>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" s="15"/>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" s="15"/>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" s="15"/>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" s="15"/>
+    </row>
+    <row r="195" spans="1:1">
+      <c r="A195" s="15"/>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" s="15"/>
+    </row>
+    <row r="197" spans="1:1">
+      <c r="A197" s="15"/>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" s="15"/>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" s="15"/>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" s="15"/>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" s="15"/>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" s="15"/>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" s="15"/>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" s="15"/>
+    </row>
+    <row r="205" spans="1:1">
+      <c r="A205" s="15"/>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" s="15"/>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" s="15"/>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" s="15"/>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" s="15"/>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" s="15"/>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211" s="15"/>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212" s="15"/>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213" s="15"/>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214" s="15"/>
+    </row>
+    <row r="215" spans="1:1">
+      <c r="A215" s="15"/>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216" s="15"/>
+    </row>
+    <row r="217" spans="1:1">
+      <c r="A217" s="15"/>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218" s="15"/>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" s="15"/>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220" s="15"/>
+    </row>
+    <row r="221" spans="1:1">
+      <c r="A221" s="15"/>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" s="15"/>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223" s="15"/>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224" s="15"/>
+    </row>
+    <row r="225" spans="1:1">
+      <c r="A225" s="15"/>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226" s="15"/>
+    </row>
+    <row r="227" spans="1:1">
+      <c r="A227" s="15"/>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228" s="15"/>
+    </row>
+    <row r="229" spans="1:1">
+      <c r="A229" s="15"/>
+    </row>
+    <row r="230" spans="1:1">
+      <c r="A230" s="15"/>
+    </row>
+    <row r="231" spans="1:1">
+      <c r="A231" s="15"/>
+    </row>
+    <row r="232" spans="1:1">
+      <c r="A232" s="15"/>
+    </row>
+    <row r="233" spans="1:1">
+      <c r="A233" s="15"/>
+    </row>
+    <row r="234" spans="1:1">
+      <c r="A234" s="15"/>
+    </row>
+    <row r="235" spans="1:1">
+      <c r="A235" s="15"/>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236" s="15"/>
+    </row>
+    <row r="237" spans="1:1">
+      <c r="A237" s="15"/>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238" s="15"/>
+    </row>
+    <row r="239" spans="1:1">
+      <c r="A239" s="15"/>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240" s="15"/>
+    </row>
+    <row r="241" spans="1:1">
+      <c r="A241" s="15"/>
+    </row>
+    <row r="242" spans="1:1">
+      <c r="A242" s="15"/>
+    </row>
+    <row r="243" spans="1:1">
+      <c r="A243" s="15"/>
+    </row>
+    <row r="244" spans="1:1">
+      <c r="A244" s="15"/>
+    </row>
+    <row r="245" spans="1:1">
+      <c r="A245" s="15"/>
+    </row>
+    <row r="246" spans="1:1">
+      <c r="A246" s="15"/>
+    </row>
+    <row r="247" spans="1:1">
+      <c r="A247" s="15"/>
+    </row>
+    <row r="248" spans="1:1">
+      <c r="A248" s="15"/>
+    </row>
+    <row r="249" spans="1:1">
+      <c r="A249" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEDE50F-3952-214F-9597-838D9D10B1E0}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -16753,7 +17573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
@@ -17016,7 +17836,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
@@ -17148,7 +17968,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:O13"/>
   <sheetViews>
@@ -17286,7 +18106,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:N12"/>
   <sheetViews>
@@ -17423,7 +18243,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E55ACB-56A8-B541-931E-FA903DDDD8CF}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -17586,7 +18406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -17683,7 +18503,108 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N4"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="2" width="11.453125"/>
+    <col min="3" max="3" width="25.453125" customWidth="1"/>
+    <col min="4" max="1024" width="11.453125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="18">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:14" ht="130">
+      <c r="A2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="147" t="s">
+        <v>179</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+    </row>
+    <row r="3" spans="1:14" ht="13">
+      <c r="A3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="F4" s="108"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:IU148"/>
   <sheetViews>
@@ -18736,108 +19657,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N4"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5"/>
-  <cols>
-    <col min="1" max="2" width="11.453125"/>
-    <col min="3" max="3" width="25.453125" customWidth="1"/>
-    <col min="4" max="1024" width="11.453125"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="18">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:14" ht="130">
-      <c r="A2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="147" t="s">
-        <v>179</v>
-      </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-    </row>
-    <row r="3" spans="1:14" ht="13">
-      <c r="A3" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="F4" s="108"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:IU10"/>
   <sheetViews>
@@ -19450,7 +20270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:D518"/>
   <sheetViews>
@@ -21194,7 +22014,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:D109"/>
   <sheetViews>
@@ -21623,7 +22443,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -23472,7 +24292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:R240"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ret 3878 - Migrate ET from IDAM to RAS (#473)
* Add RoleToAccessProfiles

* Update AuthCaseType

* Consolidate template columns and tabs
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judgem\Documents\Scotland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9474332B-A8A5-44AD-AB4C-139D012E58CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FD542F-E05E-412B-98A2-66829B25C94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4470" yWindow="-21720" windowWidth="38640" windowHeight="21240" tabRatio="855" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4470" yWindow="-21720" windowWidth="38640" windowHeight="21240" tabRatio="855" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CaseRoles" sheetId="30" r:id="rId1"/>
@@ -24,23 +24,24 @@
     <sheet name="ChallengeQuestion" sheetId="31" r:id="rId9"/>
     <sheet name="ComplexTypes" sheetId="9" r:id="rId10"/>
     <sheet name="EventToComplexTypes" sheetId="32" r:id="rId11"/>
-    <sheet name="Scotland Scrubbed" sheetId="26" r:id="rId12"/>
-    <sheet name="SearchInputFields" sheetId="12" r:id="rId13"/>
-    <sheet name="WorkBasketInputFields" sheetId="14" r:id="rId14"/>
-    <sheet name="SearchResultFields" sheetId="13" r:id="rId15"/>
-    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId16"/>
-    <sheet name="SearchCaseResultFields" sheetId="22" r:id="rId17"/>
-    <sheet name="UserProfile" sheetId="16" r:id="rId18"/>
-    <sheet name="AuthorisationComplexType" sheetId="17" r:id="rId19"/>
-    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId20"/>
-    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId21"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId22"/>
-    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId23"/>
+    <sheet name="RoleToAccessProfiles" sheetId="33" r:id="rId12"/>
+    <sheet name="Scotland Scrubbed" sheetId="26" r:id="rId13"/>
+    <sheet name="SearchInputFields" sheetId="12" r:id="rId14"/>
+    <sheet name="WorkBasketInputFields" sheetId="14" r:id="rId15"/>
+    <sheet name="SearchResultFields" sheetId="13" r:id="rId16"/>
+    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId17"/>
+    <sheet name="SearchCaseResultFields" sheetId="22" r:id="rId18"/>
+    <sheet name="UserProfile" sheetId="16" r:id="rId19"/>
+    <sheet name="AuthorisationComplexType" sheetId="17" r:id="rId20"/>
+    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId21"/>
+    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId22"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId23"/>
+    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId24"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseField!$A$1:$D$517</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseField!$A$1:$D$517</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">CaseEvent!$A$3:$Z$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CaseEventToFields!$A$3:$Q$231</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseField!$A$3:$U$3</definedName>
@@ -48,7 +49,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">CaseTypeTab!$A$3:$P$54</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">ComplexTypes!$A$3:$W$559</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">EventToComplexTypes!$A$3:$I$382</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Scotland Scrubbed'!$A$3:$F$646</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Scotland Scrubbed'!$A$3:$F$646</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">State!$A$3:$Q$11</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="359">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1205,6 +1206,21 @@
   </si>
   <si>
     <t>Boolean value to say if an event can be published</t>
+  </si>
+  <si>
+    <t>AccessProfiles</t>
+  </si>
+  <si>
+    <t>ReadOnly</t>
+  </si>
+  <si>
+    <t>RoleName</t>
+  </si>
+  <si>
+    <t>RoleToAccessProfiles</t>
+  </si>
+  <si>
+    <t>A comma-separated list of AccessProfiles that should be assigned to the user if their RoleName, ReadOnly value (and optional Authorisations) match.</t>
   </si>
 </sst>
 </file>
@@ -1860,7 +1876,7 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="283">
+  <cellXfs count="284">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2411,6 +2427,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -7631,7 +7648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E7B8F4-5285-46EC-BCE1-BF8FCCDC20D1}">
   <dimension ref="A1:L402"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D14" sqref="D14"/>
       <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
@@ -13858,6 +13875,809 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0B9A54-A710-4970-B170-413E5E0036C4}">
+  <dimension ref="A1:E249"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="1" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18">
+      <c r="A1" s="35" t="s">
+        <v>357</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="169">
+      <c r="A2" s="239" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14.5">
+      <c r="A3" s="233" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="74" t="s">
+        <v>356</v>
+      </c>
+      <c r="D3" s="283" t="s">
+        <v>355</v>
+      </c>
+      <c r="E3" s="283" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="15"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="15"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="15"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="15"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="15"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="15"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="15"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="15"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="15"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="15"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="15"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="15"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="15"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="15"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="15"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="15"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="15"/>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="15"/>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="15"/>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="15"/>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="15"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="15"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="15"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="15"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="15"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="15"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="15"/>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="15"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="15"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="15"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="15"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="15"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="15"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="15"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="15"/>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="15"/>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="15"/>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="15"/>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="15"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="15"/>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="15"/>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="15"/>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="15"/>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="15"/>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="15"/>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="15"/>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="15"/>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="15"/>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="15"/>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="15"/>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="15"/>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="15"/>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="15"/>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="15"/>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="15"/>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="15"/>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="15"/>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="15"/>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="15"/>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="15"/>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="15"/>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="15"/>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="15"/>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="15"/>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="15"/>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="15"/>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="15"/>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="15"/>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="15"/>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="15"/>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="15"/>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="15"/>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="15"/>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="15"/>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="15"/>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="15"/>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="15"/>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="15"/>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="15"/>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="15"/>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="15"/>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="15"/>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="15"/>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="15"/>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="15"/>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="15"/>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="15"/>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="15"/>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="15"/>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="15"/>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="15"/>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="15"/>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="15"/>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="15"/>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="15"/>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="15"/>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="15"/>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="15"/>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="15"/>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="15"/>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="15"/>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="15"/>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="15"/>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="15"/>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="15"/>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="15"/>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="15"/>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="15"/>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="15"/>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="15"/>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="15"/>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="15"/>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="15"/>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="15"/>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="15"/>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="15"/>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="15"/>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="15"/>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="15"/>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="15"/>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="15"/>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="15"/>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="15"/>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="15"/>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="15"/>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="15"/>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="15"/>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="15"/>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="15"/>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="15"/>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="15"/>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="15"/>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="15"/>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="15"/>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="15"/>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" s="15"/>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="15"/>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="15"/>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="15"/>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="15"/>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="15"/>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" s="15"/>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="15"/>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="15"/>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" s="15"/>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="15"/>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" s="15"/>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" s="15"/>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="15"/>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" s="15"/>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" s="15"/>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" s="15"/>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" s="15"/>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" s="15"/>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" s="15"/>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" s="15"/>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" s="15"/>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" s="15"/>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" s="15"/>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" s="15"/>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" s="15"/>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" s="15"/>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" s="15"/>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" s="15"/>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" s="15"/>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" s="15"/>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" s="15"/>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" s="15"/>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" s="15"/>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" s="15"/>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" s="15"/>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" s="15"/>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" s="15"/>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" s="15"/>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" s="15"/>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" s="15"/>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" s="15"/>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" s="15"/>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" s="15"/>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" s="15"/>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" s="15"/>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" s="15"/>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" s="15"/>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" s="15"/>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" s="15"/>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" s="15"/>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" s="15"/>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" s="15"/>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" s="15"/>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" s="15"/>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" s="15"/>
+    </row>
+    <row r="195" spans="1:1">
+      <c r="A195" s="15"/>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" s="15"/>
+    </row>
+    <row r="197" spans="1:1">
+      <c r="A197" s="15"/>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" s="15"/>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" s="15"/>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" s="15"/>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" s="15"/>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" s="15"/>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" s="15"/>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" s="15"/>
+    </row>
+    <row r="205" spans="1:1">
+      <c r="A205" s="15"/>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" s="15"/>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" s="15"/>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" s="15"/>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" s="15"/>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" s="15"/>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211" s="15"/>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212" s="15"/>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213" s="15"/>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214" s="15"/>
+    </row>
+    <row r="215" spans="1:1">
+      <c r="A215" s="15"/>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216" s="15"/>
+    </row>
+    <row r="217" spans="1:1">
+      <c r="A217" s="15"/>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218" s="15"/>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" s="15"/>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220" s="15"/>
+    </row>
+    <row r="221" spans="1:1">
+      <c r="A221" s="15"/>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" s="15"/>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223" s="15"/>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224" s="15"/>
+    </row>
+    <row r="225" spans="1:1">
+      <c r="A225" s="15"/>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226" s="15"/>
+    </row>
+    <row r="227" spans="1:1">
+      <c r="A227" s="15"/>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228" s="15"/>
+    </row>
+    <row r="229" spans="1:1">
+      <c r="A229" s="15"/>
+    </row>
+    <row r="230" spans="1:1">
+      <c r="A230" s="15"/>
+    </row>
+    <row r="231" spans="1:1">
+      <c r="A231" s="15"/>
+    </row>
+    <row r="232" spans="1:1">
+      <c r="A232" s="15"/>
+    </row>
+    <row r="233" spans="1:1">
+      <c r="A233" s="15"/>
+    </row>
+    <row r="234" spans="1:1">
+      <c r="A234" s="15"/>
+    </row>
+    <row r="235" spans="1:1">
+      <c r="A235" s="15"/>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236" s="15"/>
+    </row>
+    <row r="237" spans="1:1">
+      <c r="A237" s="15"/>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238" s="15"/>
+    </row>
+    <row r="239" spans="1:1">
+      <c r="A239" s="15"/>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240" s="15"/>
+    </row>
+    <row r="241" spans="1:1">
+      <c r="A241" s="15"/>
+    </row>
+    <row r="242" spans="1:1">
+      <c r="A242" s="15"/>
+    </row>
+    <row r="243" spans="1:1">
+      <c r="A243" s="15"/>
+    </row>
+    <row r="244" spans="1:1">
+      <c r="A244" s="15"/>
+    </row>
+    <row r="245" spans="1:1">
+      <c r="A245" s="15"/>
+    </row>
+    <row r="246" spans="1:1">
+      <c r="A246" s="15"/>
+    </row>
+    <row r="247" spans="1:1">
+      <c r="A247" s="15"/>
+    </row>
+    <row r="248" spans="1:1">
+      <c r="A248" s="15"/>
+    </row>
+    <row r="249" spans="1:1">
+      <c r="A249" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEDE50F-3952-214F-9597-838D9D10B1E0}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -16753,7 +17573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
@@ -17016,7 +17836,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
@@ -17148,7 +17968,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:O13"/>
   <sheetViews>
@@ -17286,7 +18106,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:N12"/>
   <sheetViews>
@@ -17423,7 +18243,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E55ACB-56A8-B541-931E-FA903DDDD8CF}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -17586,7 +18406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -17683,7 +18503,108 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N4"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5"/>
+  <cols>
+    <col min="1" max="2" width="11.453125"/>
+    <col min="3" max="3" width="25.453125" customWidth="1"/>
+    <col min="4" max="1024" width="11.453125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="18">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:14" ht="130">
+      <c r="A2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="147" t="s">
+        <v>179</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+    </row>
+    <row r="3" spans="1:14" ht="13">
+      <c r="A3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="F4" s="108"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:IU148"/>
   <sheetViews>
@@ -18736,108 +19657,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N4"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5"/>
-  <cols>
-    <col min="1" max="2" width="11.453125"/>
-    <col min="3" max="3" width="25.453125" customWidth="1"/>
-    <col min="4" max="1024" width="11.453125"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="18">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:14" ht="130">
-      <c r="A2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="147" t="s">
-        <v>179</v>
-      </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-    </row>
-    <row r="3" spans="1:14" ht="13">
-      <c r="A3" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="F4" s="108"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:IU10"/>
   <sheetViews>
@@ -19450,7 +20270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:D518"/>
   <sheetViews>
@@ -21194,7 +22014,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:D109"/>
   <sheetViews>
@@ -21623,7 +22443,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -23472,7 +24292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:R240"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
RET-2462: Add RoleToAccessProfile (temp remove GS_Profile to allow import)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharmendrakumar/development/moj/et/et-ccd-definitions-scotland/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\fergusoshea\et-ccd-definitions-scotland\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0921C5D-5E2E-9946-98FA-BC2EB12568DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40113A3E-F1C4-4437-8CDB-1D8BB5FCD4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20625" tabRatio="500" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchParty" sheetId="36" r:id="rId1"/>
@@ -26,23 +26,24 @@
     <sheet name="ChallengeQuestion" sheetId="31" r:id="rId11"/>
     <sheet name="ComplexTypes" sheetId="9" r:id="rId12"/>
     <sheet name="EventToComplexTypes" sheetId="32" r:id="rId13"/>
-    <sheet name="Scotland Scrubbed" sheetId="26" r:id="rId14"/>
-    <sheet name="SearchInputFields" sheetId="12" r:id="rId15"/>
-    <sheet name="WorkBasketInputFields" sheetId="14" r:id="rId16"/>
-    <sheet name="SearchResultFields" sheetId="13" r:id="rId17"/>
-    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId18"/>
-    <sheet name="SearchCaseResultFields" sheetId="22" r:id="rId19"/>
-    <sheet name="UserProfile" sheetId="16" r:id="rId20"/>
-    <sheet name="AuthorisationComplexType" sheetId="17" r:id="rId21"/>
-    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId22"/>
-    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId23"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId24"/>
-    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId25"/>
+    <sheet name="RoleToAccessProfiles" sheetId="37" r:id="rId14"/>
+    <sheet name="Scotland Scrubbed" sheetId="26" r:id="rId15"/>
+    <sheet name="SearchInputFields" sheetId="12" r:id="rId16"/>
+    <sheet name="WorkBasketInputFields" sheetId="14" r:id="rId17"/>
+    <sheet name="SearchResultFields" sheetId="13" r:id="rId18"/>
+    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId19"/>
+    <sheet name="SearchCaseResultFields" sheetId="22" r:id="rId20"/>
+    <sheet name="UserProfile" sheetId="16" r:id="rId21"/>
+    <sheet name="AuthorisationComplexType" sheetId="17" r:id="rId22"/>
+    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId23"/>
+    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId24"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId25"/>
+    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId26"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseField!$A$1:$D$517</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">AuthorisationCaseField!$A$1:$D$517</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="25" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEvent!$A$3:$Z$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseEventToFields!$A$3:$P$231</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">CaseField!$A$3:$U$3</definedName>
@@ -50,7 +51,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CaseTypeTab!$A$3:$P$54</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">ComplexTypes!$A$3:$W$559</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">EventToComplexTypes!$A$3:$I$382</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'Scotland Scrubbed'!$A$3:$F$646</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'Scotland Scrubbed'!$A$3:$F$646</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">State!$A$3:$Q$11</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="377">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1269,6 +1270,21 @@
   <si>
     <t>A comma separated list of fields or elements or complex types that make use the party's name.  Spaces will be inserted by CCD between the values of each field. Used to make up the party name for the given SearchPartyID
 Max Length: 200</t>
+  </si>
+  <si>
+    <t>RoleToAccessProfiles</t>
+  </si>
+  <si>
+    <t>A comma-separated list of AccessProfiles that should be assigned to the user if their RoleName, ReadOnly value (and optional Authorisations) match.</t>
+  </si>
+  <si>
+    <t>RoleName</t>
+  </si>
+  <si>
+    <t>ReadOnly</t>
+  </si>
+  <si>
+    <t>AccessProfiles</t>
   </si>
 </sst>
 </file>
@@ -2001,7 +2017,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -2017,8 +2033,9 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="300">
+  <cellXfs count="303">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2600,8 +2617,15 @@
     </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="18" xfId="13" applyBorder="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="20" xfId="13" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="16">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Excel Built-in Explanatory Text 1" xfId="4" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Excel Built-in Explanatory Text 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -2614,6 +2638,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="5" xr:uid="{2B00B115-41E4-DC4C-9D19-EA97F2E3C2B5}"/>
     <cellStyle name="Normal 2 2" xfId="7" xr:uid="{FE050982-89CB-CB47-B347-F33481D0E4EA}"/>
+    <cellStyle name="Normal 2 2 2" xfId="15" xr:uid="{6D8BBEB4-E03F-466C-905A-0333309E2DE2}"/>
     <cellStyle name="Normal 2 4" xfId="9" xr:uid="{B0AE22DF-3912-4A1A-AFFC-B4DD9404E3FC}"/>
     <cellStyle name="Normal 3" xfId="8" xr:uid="{CD9D10AF-0097-42A0-9715-FA166A90F092}"/>
     <cellStyle name="Normal 4" xfId="13" xr:uid="{128380BE-A59E-BF42-970E-A4A85023A104}"/>
@@ -3097,15 +3122,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{652CD649-9CF9-A24F-8AFE-A9F7C5D8EE93}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="10.6640625" style="291" customWidth="1"/>
-    <col min="3" max="1025" width="11.1640625" style="287" customWidth="1"/>
-    <col min="1026" max="16384" width="8.83203125" style="287"/>
+    <col min="1" max="2" width="10.7109375" style="291" customWidth="1"/>
+    <col min="3" max="1025" width="11.140625" style="287" customWidth="1"/>
+    <col min="1026" max="16384" width="8.85546875" style="287"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18">
@@ -3122,7 +3147,7 @@
       <c r="I1" s="299"/>
       <c r="J1" s="298"/>
     </row>
-    <row r="2" spans="1:10" ht="409.6">
+    <row r="2" spans="1:10" ht="409.5">
       <c r="A2" s="296" t="s">
         <v>353</v>
       </c>
@@ -3200,22 +3225,22 @@
       <selection activeCell="A4" sqref="A4:XFD206"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.6640625" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="26.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.33203125" style="1" customWidth="1"/>
-    <col min="12" max="17" width="8.5" customWidth="1"/>
-    <col min="18" max="21" width="6.33203125" customWidth="1"/>
-    <col min="22" max="1023" width="8.33203125" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" style="1" customWidth="1"/>
+    <col min="12" max="17" width="8.42578125" customWidth="1"/>
+    <col min="18" max="21" width="6.28515625" customWidth="1"/>
+    <col min="22" max="1023" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18">
@@ -4438,20 +4463,20 @@
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" style="246" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="246"/>
-    <col min="3" max="3" width="54.6640625" style="246" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" style="246" customWidth="1"/>
-    <col min="5" max="6" width="12.6640625" style="246" customWidth="1"/>
-    <col min="7" max="7" width="44.33203125" style="246" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" style="246" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" style="246" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="246"/>
+    <col min="3" max="3" width="54.7109375" style="246" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="246" customWidth="1"/>
+    <col min="5" max="6" width="12.7109375" style="246" customWidth="1"/>
+    <col min="7" max="7" width="44.28515625" style="246" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="246" customWidth="1"/>
     <col min="9" max="9" width="37" style="246" customWidth="1"/>
-    <col min="10" max="10" width="43.6640625" style="246" customWidth="1"/>
-    <col min="11" max="11" width="19.1640625" style="246" customWidth="1"/>
-    <col min="12" max="1025" width="10.83203125" style="246"/>
-    <col min="1026" max="16384" width="10.83203125" style="245"/>
+    <col min="10" max="10" width="43.7109375" style="246" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" style="246" customWidth="1"/>
+    <col min="12" max="1025" width="10.85546875" style="246"/>
+    <col min="1026" max="16384" width="10.85546875" style="245"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18">
@@ -4477,7 +4502,7 @@
       <c r="L1" s="247"/>
       <c r="M1" s="247"/>
     </row>
-    <row r="2" spans="1:13" ht="56">
+    <row r="2" spans="1:13" ht="63.75">
       <c r="A2" s="258" t="s">
         <v>4</v>
       </c>
@@ -4512,7 +4537,7 @@
       <c r="L2" s="254"/>
       <c r="M2" s="254"/>
     </row>
-    <row r="3" spans="1:13" ht="16">
+    <row r="3" spans="1:13" ht="15.75">
       <c r="A3" s="253" t="s">
         <v>9</v>
       </c>
@@ -4637,26 +4662,26 @@
       <selection activeCell="A4" sqref="A4:XFD559"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="31.5" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="20.5" style="52" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="41" customWidth="1"/>
-    <col min="7" max="7" width="9.5" style="41" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="52" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="41" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="41" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" style="53" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" style="53" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="53" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="53" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="28.33203125" customWidth="1"/>
-    <col min="16" max="23" width="6.33203125" customWidth="1"/>
-    <col min="24" max="1023" width="8.33203125" customWidth="1"/>
-    <col min="1024" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="15" max="15" width="28.28515625" customWidth="1"/>
+    <col min="16" max="23" width="6.28515625" customWidth="1"/>
+    <col min="24" max="1023" width="8.28515625" customWidth="1"/>
+    <col min="1024" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="18" customHeight="1">
@@ -4685,7 +4710,7 @@
       <c r="P1" s="36"/>
       <c r="Q1" s="36"/>
     </row>
-    <row r="2" spans="1:23" ht="65" customHeight="1">
+    <row r="2" spans="1:23" ht="65.099999999999994" customHeight="1">
       <c r="A2" s="25" t="s">
         <v>113</v>
       </c>
@@ -4726,7 +4751,7 @@
       <c r="P2" s="10"/>
       <c r="Q2" s="10"/>
     </row>
-    <row r="3" spans="1:23" s="2" customFormat="1" ht="33.5" customHeight="1">
+    <row r="3" spans="1:23" s="2" customFormat="1" ht="33.6" customHeight="1">
       <c r="A3" s="27" t="s">
         <v>11</v>
       </c>
@@ -6867,7 +6892,7 @@
       <c r="I278"/>
       <c r="J278"/>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:10" ht="13.5">
       <c r="B279" s="231"/>
       <c r="E279"/>
       <c r="F279" s="108"/>
@@ -8406,7 +8431,7 @@
       <c r="G488" s="219"/>
       <c r="H488" s="193"/>
     </row>
-    <row r="489" spans="1:8">
+    <row r="489" spans="1:8" ht="13.5">
       <c r="A489" s="56"/>
       <c r="B489" s="231"/>
       <c r="C489" s="56"/>
@@ -8416,7 +8441,7 @@
       <c r="G489" s="219"/>
       <c r="H489" s="193"/>
     </row>
-    <row r="490" spans="1:8">
+    <row r="490" spans="1:8" ht="13.5">
       <c r="A490" s="56"/>
       <c r="B490" s="231"/>
       <c r="C490" s="56"/>
@@ -8426,7 +8451,7 @@
       <c r="G490" s="219"/>
       <c r="H490" s="193"/>
     </row>
-    <row r="491" spans="1:8">
+    <row r="491" spans="1:8" ht="13.5">
       <c r="A491" s="56"/>
       <c r="B491" s="231"/>
       <c r="C491" s="56"/>
@@ -9256,21 +9281,21 @@
       <selection pane="bottomLeft" activeCell="E369" sqref="E369"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.5" customWidth="1"/>
-    <col min="6" max="6" width="50.1640625" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
-    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.42578125" customWidth="1"/>
+    <col min="6" max="6" width="50.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="40" customHeight="1">
+    <row r="1" spans="1:11" ht="39.950000000000003" customHeight="1">
       <c r="A1" s="282" t="s">
         <v>120</v>
       </c>
@@ -9289,7 +9314,7 @@
       <c r="H1" s="278"/>
       <c r="I1" s="277"/>
     </row>
-    <row r="2" spans="1:11" ht="67" customHeight="1">
+    <row r="2" spans="1:11" ht="66.95" customHeight="1">
       <c r="A2" s="275" t="s">
         <v>121</v>
       </c>
@@ -15471,6 +15496,808 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C4F7720-24EC-4BC8-BFE2-934342B17442}">
+  <dimension ref="A1:E249"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18">
+      <c r="A1" s="35" t="s">
+        <v>372</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="165.75">
+      <c r="A2" s="300" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15">
+      <c r="A3" s="301" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="74" t="s">
+        <v>374</v>
+      </c>
+      <c r="D3" s="302" t="s">
+        <v>375</v>
+      </c>
+      <c r="E3" s="302" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="15"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="15"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="15"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="15"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="15"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="15"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="15"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="15"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="15"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="15"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="15"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="15"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="15"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="15"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="15"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="15"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="15"/>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="15"/>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="15"/>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="15"/>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="15"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="15"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="15"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="15"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="15"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="15"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="15"/>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="15"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="15"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="15"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="15"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="15"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="15"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="15"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="15"/>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="15"/>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="15"/>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="15"/>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="15"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="15"/>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="15"/>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="15"/>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="15"/>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="15"/>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="15"/>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="15"/>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="15"/>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="15"/>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="15"/>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="15"/>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="15"/>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="15"/>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="15"/>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="15"/>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="15"/>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="15"/>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="15"/>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="15"/>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="15"/>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="15"/>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="15"/>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="15"/>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="15"/>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="15"/>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="15"/>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="15"/>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="15"/>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="15"/>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="15"/>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="15"/>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="15"/>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="15"/>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="15"/>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="15"/>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="15"/>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="15"/>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="15"/>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="15"/>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="15"/>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="15"/>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="15"/>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="15"/>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="15"/>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="15"/>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="15"/>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="15"/>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="15"/>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="15"/>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="15"/>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="15"/>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="15"/>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="15"/>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="15"/>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="15"/>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="15"/>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="15"/>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="15"/>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="15"/>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="15"/>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="15"/>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="15"/>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="15"/>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="15"/>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="15"/>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="15"/>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="15"/>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="15"/>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="15"/>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="15"/>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="15"/>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="15"/>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="15"/>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="15"/>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="15"/>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="15"/>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="15"/>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="15"/>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="15"/>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="15"/>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="15"/>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="15"/>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="15"/>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="15"/>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="15"/>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="15"/>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="15"/>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="15"/>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="15"/>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="15"/>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="15"/>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="15"/>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="15"/>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="15"/>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="15"/>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="15"/>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" s="15"/>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="15"/>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="15"/>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="15"/>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="15"/>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="15"/>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" s="15"/>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="15"/>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="15"/>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" s="15"/>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="15"/>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" s="15"/>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" s="15"/>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="15"/>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" s="15"/>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" s="15"/>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" s="15"/>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" s="15"/>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" s="15"/>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" s="15"/>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" s="15"/>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" s="15"/>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" s="15"/>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" s="15"/>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" s="15"/>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" s="15"/>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" s="15"/>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" s="15"/>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" s="15"/>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" s="15"/>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" s="15"/>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" s="15"/>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" s="15"/>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" s="15"/>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" s="15"/>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" s="15"/>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" s="15"/>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" s="15"/>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" s="15"/>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" s="15"/>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" s="15"/>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" s="15"/>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" s="15"/>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" s="15"/>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" s="15"/>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" s="15"/>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" s="15"/>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" s="15"/>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" s="15"/>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" s="15"/>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" s="15"/>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" s="15"/>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" s="15"/>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" s="15"/>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" s="15"/>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" s="15"/>
+    </row>
+    <row r="195" spans="1:1">
+      <c r="A195" s="15"/>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" s="15"/>
+    </row>
+    <row r="197" spans="1:1">
+      <c r="A197" s="15"/>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" s="15"/>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" s="15"/>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" s="15"/>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" s="15"/>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" s="15"/>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" s="15"/>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" s="15"/>
+    </row>
+    <row r="205" spans="1:1">
+      <c r="A205" s="15"/>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" s="15"/>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" s="15"/>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" s="15"/>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" s="15"/>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" s="15"/>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211" s="15"/>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212" s="15"/>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213" s="15"/>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214" s="15"/>
+    </row>
+    <row r="215" spans="1:1">
+      <c r="A215" s="15"/>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216" s="15"/>
+    </row>
+    <row r="217" spans="1:1">
+      <c r="A217" s="15"/>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218" s="15"/>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" s="15"/>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220" s="15"/>
+    </row>
+    <row r="221" spans="1:1">
+      <c r="A221" s="15"/>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" s="15"/>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223" s="15"/>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224" s="15"/>
+    </row>
+    <row r="225" spans="1:1">
+      <c r="A225" s="15"/>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226" s="15"/>
+    </row>
+    <row r="227" spans="1:1">
+      <c r="A227" s="15"/>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228" s="15"/>
+    </row>
+    <row r="229" spans="1:1">
+      <c r="A229" s="15"/>
+    </row>
+    <row r="230" spans="1:1">
+      <c r="A230" s="15"/>
+    </row>
+    <row r="231" spans="1:1">
+      <c r="A231" s="15"/>
+    </row>
+    <row r="232" spans="1:1">
+      <c r="A232" s="15"/>
+    </row>
+    <row r="233" spans="1:1">
+      <c r="A233" s="15"/>
+    </row>
+    <row r="234" spans="1:1">
+      <c r="A234" s="15"/>
+    </row>
+    <row r="235" spans="1:1">
+      <c r="A235" s="15"/>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236" s="15"/>
+    </row>
+    <row r="237" spans="1:1">
+      <c r="A237" s="15"/>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238" s="15"/>
+    </row>
+    <row r="239" spans="1:1">
+      <c r="A239" s="15"/>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240" s="15"/>
+    </row>
+    <row r="241" spans="1:1">
+      <c r="A241" s="15"/>
+    </row>
+    <row r="242" spans="1:1">
+      <c r="A242" s="15"/>
+    </row>
+    <row r="243" spans="1:1">
+      <c r="A243" s="15"/>
+    </row>
+    <row r="244" spans="1:1">
+      <c r="A244" s="15"/>
+    </row>
+    <row r="245" spans="1:1">
+      <c r="A245" s="15"/>
+    </row>
+    <row r="246" spans="1:1">
+      <c r="A246" s="15"/>
+    </row>
+    <row r="247" spans="1:1">
+      <c r="A247" s="15"/>
+    </row>
+    <row r="248" spans="1:1">
+      <c r="A248" s="15"/>
+    </row>
+    <row r="249" spans="1:1">
+      <c r="A249" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEDE50F-3952-214F-9597-838D9D10B1E0}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -15481,18 +16308,18 @@
       <selection activeCell="A4" sqref="A4:XFD650"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" style="151" customWidth="1"/>
-    <col min="2" max="2" width="61.6640625" style="171" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" style="151" customWidth="1"/>
+    <col min="2" max="2" width="61.7109375" style="171" customWidth="1"/>
     <col min="3" max="3" width="65" style="151" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="151" customWidth="1"/>
-    <col min="5" max="6" width="8.6640625" style="151"/>
+    <col min="4" max="4" width="14.7109375" style="151" customWidth="1"/>
+    <col min="5" max="6" width="8.7109375" style="151"/>
     <col min="7" max="7" width="13" style="151" customWidth="1"/>
-    <col min="8" max="8" width="11.5" style="151" customWidth="1"/>
-    <col min="9" max="12" width="8.6640625" style="151"/>
-    <col min="13" max="13" width="16.33203125" style="151" customWidth="1"/>
-    <col min="14" max="16384" width="8.6640625" style="151"/>
+    <col min="8" max="8" width="11.42578125" style="151" customWidth="1"/>
+    <col min="9" max="12" width="8.7109375" style="151"/>
+    <col min="13" max="13" width="16.28515625" style="151" customWidth="1"/>
+    <col min="14" max="16384" width="8.7109375" style="151"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18">
@@ -15509,7 +16336,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="56">
+    <row r="2" spans="1:11" ht="51">
       <c r="A2" s="152" t="s">
         <v>129</v>
       </c>
@@ -18366,7 +19193,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
@@ -18374,22 +19201,22 @@
       <selection activeCell="A4" sqref="A4:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="32.5" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
-    <col min="7" max="7" width="43.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" customWidth="1"/>
-    <col min="9" max="9" width="31.5" customWidth="1"/>
-    <col min="10" max="10" width="21.6640625" customWidth="1"/>
-    <col min="11" max="11" width="6.33203125" customWidth="1"/>
-    <col min="12" max="1025" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="32.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="43.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="31.42578125" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" customWidth="1"/>
+    <col min="12" max="1025" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="19">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="36">
       <c r="A1" s="69" t="s">
         <v>134</v>
       </c>
@@ -18407,7 +19234,7 @@
       <c r="G1" s="73"/>
       <c r="H1" s="186"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="71">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="75">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
@@ -18619,138 +19446,6 @@
     <row r="37" spans="5:7">
       <c r="E37" s="1"/>
       <c r="G37"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
-  <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.5" customWidth="1"/>
-    <col min="9" max="1023" width="8.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="80" t="s">
-        <v>142</v>
-      </c>
-      <c r="B1" s="81" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="82" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="83" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="84"/>
-    </row>
-    <row r="2" spans="1:8" ht="84">
-      <c r="A2" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" s="126" t="s">
-        <v>170</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15">
-      <c r="A3" s="74" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="74" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="74" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="127" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="127" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15">
-      <c r="D4"/>
-      <c r="E4" s="1"/>
-      <c r="G4" s="68"/>
-    </row>
-    <row r="5" spans="1:8" ht="15">
-      <c r="D5" s="111"/>
-      <c r="E5" s="1"/>
-      <c r="G5" s="68"/>
-    </row>
-    <row r="6" spans="1:8" ht="14">
-      <c r="D6" s="112"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="15">
-      <c r="D7"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="187"/>
-    </row>
-    <row r="8" spans="1:8" ht="14">
-      <c r="B8" s="108"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="B9" s="108"/>
-      <c r="D9"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="D10"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="D11"/>
-      <c r="E11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -18762,70 +19457,66 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:O13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD13"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="32.5" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1"/>
-    <col min="8" max="1023" width="11.5"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" customWidth="1"/>
+    <col min="9" max="1023" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="19">
-      <c r="A1" s="69" t="s">
-        <v>138</v>
-      </c>
-      <c r="B1" s="75" t="s">
+    <row r="1" spans="1:8" ht="18.75">
+      <c r="A1" s="80" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-    </row>
-    <row r="2" spans="1:15" ht="80">
+      <c r="E1" s="84"/>
+    </row>
+    <row r="2" spans="1:8" ht="89.25">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="F2" s="123" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="126" t="s">
         <v>170</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-    </row>
-    <row r="3" spans="1:15" ht="15">
+    </row>
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="74" t="s">
         <v>32</v>
       </c>
@@ -18841,54 +19532,52 @@
       <c r="E3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="127" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="127" t="s">
         <v>157</v>
       </c>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
-    </row>
-    <row r="4" spans="1:15">
+    </row>
+    <row r="4" spans="1:8" ht="15">
+      <c r="D4"/>
       <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" ht="15">
+      <c r="G4" s="68"/>
+    </row>
+    <row r="5" spans="1:8" ht="15">
+      <c r="D5" s="111"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="187"/>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="G5" s="68"/>
+    </row>
+    <row r="6" spans="1:8" ht="14.25">
+      <c r="D6" s="112"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:8" ht="15">
+      <c r="D7"/>
       <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="F7" s="187"/>
+    </row>
+    <row r="8" spans="1:8" ht="14.25">
+      <c r="B8" s="108"/>
+      <c r="D8" s="112"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:8">
       <c r="B9" s="108"/>
+      <c r="D9"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:15">
-      <c r="B10" s="108"/>
+    <row r="10" spans="1:8">
+      <c r="D10"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:15">
-      <c r="B11" s="108"/>
+    <row r="11" spans="1:8">
+      <c r="D11"/>
       <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="E13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -18900,46 +19589,46 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:N12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD12"/>
+      <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="25.5" customWidth="1"/>
-    <col min="8" max="14" width="6.33203125" customWidth="1"/>
-    <col min="15" max="1023" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" customWidth="1"/>
+    <col min="8" max="1023" width="11.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18">
-      <c r="A1" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="B1" s="17" t="s">
+    <row r="1" spans="1:15" ht="36">
+      <c r="A1" s="69" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-    </row>
-    <row r="2" spans="1:14" ht="96">
+      <c r="E1" s="39"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+    </row>
+    <row r="2" spans="1:15" ht="90">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
@@ -18947,7 +19636,7 @@
         <v>139</v>
       </c>
       <c r="C2" s="24"/>
-      <c r="D2" s="113" t="s">
+      <c r="D2" s="24" t="s">
         <v>140</v>
       </c>
       <c r="E2" s="24" t="s">
@@ -18959,10 +19648,11 @@
       <c r="G2" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-    </row>
-    <row r="3" spans="1:14" ht="15">
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+    </row>
+    <row r="3" spans="1:15" ht="15">
       <c r="A3" s="74" t="s">
         <v>32</v>
       </c>
@@ -18972,7 +19662,7 @@
       <c r="C3" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="114" t="s">
+      <c r="D3" s="12" t="s">
         <v>105</v>
       </c>
       <c r="E3" s="12" t="s">
@@ -18991,41 +19681,41 @@
       <c r="L3" s="79"/>
       <c r="M3" s="79"/>
       <c r="N3" s="79"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3" s="79"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15" ht="15">
       <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="F5" s="187"/>
+    </row>
+    <row r="6" spans="1:15">
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:14">
-      <c r="D7"/>
+    <row r="7" spans="1:15">
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:14">
-      <c r="D8"/>
+    <row r="8" spans="1:15">
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="B9" s="108"/>
-      <c r="D9"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="B10" s="108"/>
-      <c r="D10"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:14">
-      <c r="D11"/>
+    <row r="11" spans="1:15">
+      <c r="B11" s="108"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:14">
-      <c r="D12"/>
+    <row r="12" spans="1:15">
       <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="E13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -19037,162 +19727,136 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E55ACB-56A8-B541-931E-FA903DDDD8CF}">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="133" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" style="133" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="133" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="133" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="133" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" style="133" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" style="133" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="133" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="133" customWidth="1"/>
-    <col min="10" max="16384" width="10.6640625" style="133"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="50" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" customWidth="1"/>
+    <col min="8" max="14" width="6.28515625" customWidth="1"/>
+    <col min="15" max="1023" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
-      <c r="A1" s="128" t="s">
-        <v>172</v>
-      </c>
-      <c r="B1" s="129" t="s">
+    <row r="1" spans="1:14" ht="18">
+      <c r="A1" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="130" t="s">
+      <c r="C1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="131" t="s">
+      <c r="D1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-    </row>
-    <row r="2" spans="1:9" ht="42">
-      <c r="A2" s="134"/>
-      <c r="B2" s="134"/>
-      <c r="C2" s="135" t="s">
-        <v>173</v>
-      </c>
-      <c r="D2" s="135" t="s">
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+    </row>
+    <row r="2" spans="1:14" ht="105">
+      <c r="A2" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="135" t="s">
-        <v>174</v>
-      </c>
-      <c r="F2" s="134" t="s">
-        <v>175</v>
-      </c>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-    </row>
-    <row r="3" spans="1:9" ht="15">
-      <c r="A3" s="136" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="136" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="137" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="113" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" s="123" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+    </row>
+    <row r="3" spans="1:14" ht="15">
+      <c r="A3" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="137" t="s">
+      <c r="B3" s="74" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="136" t="s">
+      <c r="C3" s="74" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="114" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="136" t="s">
+      <c r="E3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="136" t="s">
+      <c r="F3" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="136" t="s">
-        <v>176</v>
-      </c>
-      <c r="I3" s="136" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15">
-      <c r="A4" s="138"/>
-      <c r="B4" s="139"/>
-      <c r="C4" s="132"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="139"/>
-      <c r="F4" s="139"/>
-      <c r="G4" s="139"/>
-      <c r="H4" s="139"/>
-      <c r="I4" s="139"/>
-    </row>
-    <row r="5" spans="1:9" ht="15">
-      <c r="A5" s="138"/>
-      <c r="B5" s="139"/>
-      <c r="C5" s="132"/>
-      <c r="D5" s="132"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="132"/>
-      <c r="H5" s="132"/>
-      <c r="I5" s="139"/>
-    </row>
-    <row r="6" spans="1:9" ht="15">
-      <c r="A6" s="138"/>
-      <c r="B6" s="139"/>
-      <c r="C6" s="132"/>
-      <c r="D6" s="132"/>
-      <c r="E6" s="139"/>
-      <c r="F6" s="139"/>
-      <c r="G6" s="132"/>
-      <c r="H6" s="132"/>
-      <c r="I6" s="139"/>
-    </row>
-    <row r="7" spans="1:9" ht="15">
-      <c r="A7" s="138"/>
-      <c r="B7" s="139"/>
-      <c r="C7" s="132"/>
-      <c r="D7" s="132"/>
-      <c r="E7" s="139"/>
-      <c r="F7" s="139"/>
-      <c r="G7" s="132"/>
-      <c r="H7" s="132"/>
-      <c r="I7" s="139"/>
-    </row>
-    <row r="8" spans="1:9" ht="15">
-      <c r="A8" s="138"/>
-      <c r="B8" s="139"/>
-      <c r="C8" s="132"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="139"/>
-      <c r="F8" s="139"/>
-      <c r="G8" s="132"/>
-      <c r="H8" s="132"/>
-      <c r="I8" s="139"/>
-    </row>
-    <row r="9" spans="1:9" ht="15">
-      <c r="A9" s="138"/>
-      <c r="B9" s="139"/>
-      <c r="C9" s="132"/>
-      <c r="D9" s="132"/>
-      <c r="E9" s="139"/>
-      <c r="F9" s="139"/>
-      <c r="G9" s="132"/>
-      <c r="H9" s="132"/>
-      <c r="I9" s="139"/>
+      <c r="G3" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="D7"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="D8"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="B9" s="108"/>
+      <c r="D9"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="B10" s="108"/>
+      <c r="D10"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="D11"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="D12"/>
+      <c r="E12" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
   </headerFooter>
@@ -19207,11 +19871,11 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="10.6640625" style="291" customWidth="1"/>
-    <col min="3" max="1025" width="11.1640625" style="287" customWidth="1"/>
-    <col min="1026" max="16384" width="8.83203125" style="287"/>
+    <col min="1" max="2" width="10.7109375" style="291" customWidth="1"/>
+    <col min="3" max="1025" width="11.140625" style="287" customWidth="1"/>
+    <col min="1026" max="16384" width="8.85546875" style="287"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -19222,7 +19886,7 @@
       <c r="C1" s="285"/>
       <c r="D1" s="286"/>
     </row>
-    <row r="2" spans="1:4" ht="99">
+    <row r="2" spans="1:4" ht="102.75">
       <c r="A2" s="288" t="s">
         <v>353</v>
       </c>
@@ -19260,6 +19924,169 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E55ACB-56A8-B541-931E-FA903DDDD8CF}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" style="133" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="133" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="133" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="133" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="133" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="133" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="133" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="133" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="133" customWidth="1"/>
+    <col min="10" max="16384" width="10.7109375" style="133"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18">
+      <c r="A1" s="128" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="129" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="130" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="131" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
+      <c r="I1" s="132"/>
+    </row>
+    <row r="2" spans="1:9" ht="38.25">
+      <c r="A2" s="134"/>
+      <c r="B2" s="134"/>
+      <c r="C2" s="135" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="135" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="135" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" s="134" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+    </row>
+    <row r="3" spans="1:9" ht="15">
+      <c r="A3" s="136" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="136" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="137" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="137" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="136" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="136" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="136" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="136" t="s">
+        <v>176</v>
+      </c>
+      <c r="I3" s="136" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15">
+      <c r="A4" s="138"/>
+      <c r="B4" s="139"/>
+      <c r="C4" s="132"/>
+      <c r="D4" s="132"/>
+      <c r="E4" s="139"/>
+      <c r="F4" s="139"/>
+      <c r="G4" s="139"/>
+      <c r="H4" s="139"/>
+      <c r="I4" s="139"/>
+    </row>
+    <row r="5" spans="1:9" ht="15">
+      <c r="A5" s="138"/>
+      <c r="B5" s="139"/>
+      <c r="C5" s="132"/>
+      <c r="D5" s="132"/>
+      <c r="E5" s="139"/>
+      <c r="F5" s="139"/>
+      <c r="G5" s="132"/>
+      <c r="H5" s="132"/>
+      <c r="I5" s="139"/>
+    </row>
+    <row r="6" spans="1:9" ht="15">
+      <c r="A6" s="138"/>
+      <c r="B6" s="139"/>
+      <c r="C6" s="132"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="139"/>
+      <c r="F6" s="139"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="132"/>
+      <c r="I6" s="139"/>
+    </row>
+    <row r="7" spans="1:9" ht="15">
+      <c r="A7" s="138"/>
+      <c r="B7" s="139"/>
+      <c r="C7" s="132"/>
+      <c r="D7" s="132"/>
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="132"/>
+      <c r="H7" s="132"/>
+      <c r="I7" s="139"/>
+    </row>
+    <row r="8" spans="1:9" ht="15">
+      <c r="A8" s="138"/>
+      <c r="B8" s="139"/>
+      <c r="C8" s="132"/>
+      <c r="D8" s="132"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="139"/>
+      <c r="G8" s="132"/>
+      <c r="H8" s="132"/>
+      <c r="I8" s="139"/>
+    </row>
+    <row r="9" spans="1:9" ht="15">
+      <c r="A9" s="138"/>
+      <c r="B9" s="139"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132"/>
+      <c r="E9" s="139"/>
+      <c r="F9" s="139"/>
+      <c r="G9" s="132"/>
+      <c r="H9" s="132"/>
+      <c r="I9" s="139"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -19267,14 +20094,14 @@
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="11.5"/>
-    <col min="3" max="3" width="35.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="1" max="2" width="11.42578125"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="1025" width="11.5"/>
+    <col min="7" max="1025" width="11.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18">
@@ -19298,7 +20125,7 @@
       <c r="J1" s="36"/>
       <c r="K1" s="36"/>
     </row>
-    <row r="2" spans="1:11" ht="70">
+    <row r="2" spans="1:11" ht="63.75">
       <c r="A2" s="23" t="s">
         <v>4</v>
       </c>
@@ -19321,7 +20148,7 @@
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
     </row>
-    <row r="3" spans="1:11" ht="28">
+    <row r="3" spans="1:11" ht="38.25">
       <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
@@ -19356,7 +20183,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:IU148"/>
   <sheetViews>
@@ -19364,15 +20191,15 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="50.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="45.6640625" customWidth="1"/>
-    <col min="7" max="1025" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="50.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
+    <col min="7" max="1025" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:255" ht="18" customHeight="1">
@@ -19640,7 +20467,7 @@
       <c r="IT1" s="36"/>
       <c r="IU1" s="36"/>
     </row>
-    <row r="2" spans="1:255" ht="196">
+    <row r="2" spans="1:255" ht="191.25">
       <c r="A2" s="23"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24" t="s">
@@ -20409,7 +21236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:IU10"/>
   <sheetViews>
@@ -20417,14 +21244,14 @@
       <selection activeCell="A4" sqref="A4:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="50.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="1" customWidth="1"/>
-    <col min="6" max="1025" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="50.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
+    <col min="6" max="1025" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:255" ht="18" customHeight="1">
@@ -20692,7 +21519,7 @@
       <c r="IT1" s="36"/>
       <c r="IU1" s="36"/>
     </row>
-    <row r="2" spans="1:255" ht="84">
+    <row r="2" spans="1:255" ht="89.25">
       <c r="A2" s="23" t="s">
         <v>4</v>
       </c>
@@ -21022,7 +21849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:D518"/>
   <sheetViews>
@@ -21030,14 +21857,14 @@
       <selection activeCell="A4" sqref="A4:XFD518"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.5" customWidth="1"/>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" style="1" customWidth="1"/>
-    <col min="5" max="1011" width="8.33203125" customWidth="1"/>
-    <col min="1012" max="1016" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="1" customWidth="1"/>
+    <col min="5" max="1011" width="8.28515625" customWidth="1"/>
+    <col min="1012" max="1016" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -21054,7 +21881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="56">
+    <row r="2" spans="1:4" ht="51">
       <c r="A2" s="24" t="s">
         <v>153</v>
       </c>
@@ -22766,7 +23593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:D109"/>
   <sheetViews>
@@ -22774,12 +23601,12 @@
       <selection activeCell="A4" sqref="A4:XFD115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -22796,7 +23623,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="56">
+    <row r="2" spans="1:4" ht="63.75">
       <c r="A2" s="24" t="s">
         <v>160</v>
       </c>
@@ -23195,7 +24022,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -23203,12 +24030,12 @@
       <selection activeCell="A4" sqref="A4:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="53.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="53.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -23225,7 +24052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="56">
+    <row r="2" spans="1:4" ht="51">
       <c r="A2" s="24" t="s">
         <v>153</v>
       </c>
@@ -23403,17 +24230,17 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" style="133" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="133" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" style="133" customWidth="1"/>
-    <col min="4" max="4" width="28.5" style="133" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" style="133" customWidth="1"/>
-    <col min="6" max="6" width="22.83203125" style="133" customWidth="1"/>
-    <col min="7" max="7" width="24.5" style="133" customWidth="1"/>
-    <col min="8" max="1025" width="8.83203125" style="133" customWidth="1"/>
-    <col min="1026" max="16384" width="8.83203125" style="133"/>
+    <col min="1" max="1" width="16.140625" style="133" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="133" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="133" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" style="133" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="133" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" style="133" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" style="133" customWidth="1"/>
+    <col min="8" max="1025" width="8.85546875" style="133" customWidth="1"/>
+    <col min="1026" max="16384" width="8.85546875" style="133"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1">
@@ -23432,7 +24259,7 @@
       <c r="E1" s="240"/>
       <c r="F1" s="240"/>
     </row>
-    <row r="2" spans="1:6" s="236" customFormat="1" ht="42">
+    <row r="2" spans="1:6" s="236" customFormat="1" ht="38.25">
       <c r="A2" s="239" t="s">
         <v>4</v>
       </c>
@@ -23452,7 +24279,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.75" customHeight="1">
+    <row r="3" spans="1:6" ht="13.7" customHeight="1">
       <c r="A3" s="233" t="s">
         <v>9</v>
       </c>
@@ -23472,28 +24299,28 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.75" customHeight="1">
+    <row r="4" spans="1:6" ht="13.7" customHeight="1">
       <c r="A4" s="232"/>
       <c r="B4" s="232"/>
     </row>
-    <row r="5" spans="1:6" ht="13.75" customHeight="1">
+    <row r="5" spans="1:6" ht="13.7" customHeight="1">
       <c r="A5" s="232"/>
       <c r="B5" s="232"/>
     </row>
-    <row r="6" spans="1:6" ht="13.75" customHeight="1">
+    <row r="6" spans="1:6" ht="13.7" customHeight="1">
       <c r="A6" s="232"/>
       <c r="B6" s="232"/>
     </row>
-    <row r="7" spans="1:6" ht="13.75" customHeight="1">
+    <row r="7" spans="1:6" ht="13.7" customHeight="1">
       <c r="A7" s="232"/>
       <c r="B7" s="232"/>
     </row>
-    <row r="8" spans="1:6" ht="13.75" customHeight="1">
+    <row r="8" spans="1:6" ht="13.7" customHeight="1">
       <c r="A8" s="232"/>
       <c r="B8" s="232"/>
     </row>
-    <row r="9" spans="1:6" ht="13.75" customHeight="1"/>
-    <row r="10" spans="1:6" ht="13.75" customHeight="1"/>
+    <row r="9" spans="1:6" ht="13.7" customHeight="1"/>
+    <row r="10" spans="1:6" ht="13.7" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -23511,11 +24338,11 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="11.5"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
-    <col min="4" max="1024" width="11.5"/>
+    <col min="1" max="2" width="11.42578125"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="1024" width="11.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18">
@@ -23533,7 +24360,7 @@
       </c>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:14" ht="126">
+    <row r="2" spans="1:14" ht="127.5">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -23612,14 +24439,14 @@
       <selection activeCell="A4" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="11.5"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="1" max="2" width="11.42578125"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
     <col min="4" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="61.33203125" customWidth="1"/>
-    <col min="8" max="1025" width="11.5"/>
+    <col min="7" max="7" width="61.28515625" customWidth="1"/>
+    <col min="8" max="1025" width="11.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18">
@@ -23646,7 +24473,7 @@
       <c r="M1" s="22"/>
       <c r="N1" s="22"/>
     </row>
-    <row r="2" spans="1:19" ht="196">
+    <row r="2" spans="1:19" ht="178.5">
       <c r="A2" s="23" t="s">
         <v>4</v>
       </c>
@@ -23680,7 +24507,7 @@
       <c r="M2" s="26"/>
       <c r="N2" s="26"/>
     </row>
-    <row r="3" spans="1:19" ht="42">
+    <row r="3" spans="1:19" ht="38.25">
       <c r="A3" s="27" t="s">
         <v>9</v>
       </c>
@@ -23760,14 +24587,14 @@
       <selection activeCell="A4" sqref="A4:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.5" customWidth="1"/>
-    <col min="2" max="3" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="3" width="21.28515625" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="11.5"/>
-    <col min="6" max="6" width="35.33203125" customWidth="1"/>
-    <col min="7" max="1023" width="11.5"/>
+    <col min="5" max="5" width="11.42578125"/>
+    <col min="6" max="6" width="35.28515625" customWidth="1"/>
+    <col min="7" max="1023" width="11.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18">
@@ -23792,7 +24619,7 @@
       <c r="K1" s="22"/>
       <c r="L1" s="22"/>
     </row>
-    <row r="2" spans="1:17" ht="98">
+    <row r="2" spans="1:17" ht="89.25">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
@@ -23818,7 +24645,7 @@
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
     </row>
-    <row r="3" spans="1:17" ht="28">
+    <row r="3" spans="1:17" ht="25.5">
       <c r="A3" s="28" t="s">
         <v>32</v>
       </c>
@@ -23920,19 +24747,19 @@
       <selection activeCell="A4" sqref="A4:XFD98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
     <col min="9" max="9" width="31" customWidth="1"/>
-    <col min="10" max="10" width="26.33203125" customWidth="1"/>
-    <col min="11" max="1023" width="8.6640625" customWidth="1"/>
+    <col min="10" max="10" width="26.28515625" customWidth="1"/>
+    <col min="11" max="1023" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18">
@@ -23990,7 +24817,7 @@
       <c r="K2" s="36"/>
       <c r="L2" s="36"/>
     </row>
-    <row r="3" spans="1:16" ht="42">
+    <row r="3" spans="1:16" ht="38.25">
       <c r="A3" s="40" t="s">
         <v>32</v>
       </c>
@@ -24570,29 +25397,29 @@
       <selection activeCell="A4" sqref="A4:XFD54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="42.33203125" customWidth="1"/>
-    <col min="8" max="8" width="74.6640625" customWidth="1"/>
-    <col min="9" max="9" width="83.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="79.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="88.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="23.33203125" customWidth="1"/>
-    <col min="14" max="14" width="8.5" customWidth="1"/>
-    <col min="15" max="15" width="18.5" customWidth="1"/>
-    <col min="16" max="16" width="18.5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.33203125" customWidth="1"/>
-    <col min="18" max="18" width="20.5" customWidth="1"/>
-    <col min="19" max="19" width="17.6640625" customWidth="1"/>
-    <col min="20" max="30" width="8.5" customWidth="1"/>
-    <col min="31" max="1024" width="8.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" customWidth="1"/>
+    <col min="8" max="8" width="74.7109375" customWidth="1"/>
+    <col min="9" max="9" width="83.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="88.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="23.28515625" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" customWidth="1"/>
+    <col min="18" max="18" width="20.42578125" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" customWidth="1"/>
+    <col min="20" max="30" width="8.42578125" customWidth="1"/>
+    <col min="31" max="1024" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">
@@ -24624,7 +25451,7 @@
       <c r="R1" s="39"/>
       <c r="S1" s="39"/>
     </row>
-    <row r="2" spans="1:26" ht="126">
+    <row r="2" spans="1:26" ht="127.5">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
@@ -24665,7 +25492,7 @@
       <c r="R2" s="25"/>
       <c r="S2" s="25"/>
     </row>
-    <row r="3" spans="1:26" ht="42">
+    <row r="3" spans="1:26" ht="38.25">
       <c r="A3" s="40" t="s">
         <v>32</v>
       </c>
@@ -24731,14 +25558,14 @@
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
     </row>
-    <row r="4" spans="1:26" ht="14">
+    <row r="4" spans="1:26" ht="14.25">
       <c r="I4" s="107"/>
       <c r="L4" s="36"/>
       <c r="M4" s="46"/>
       <c r="R4" s="109"/>
       <c r="S4" s="109"/>
     </row>
-    <row r="5" spans="1:26" ht="14">
+    <row r="5" spans="1:26" ht="14.25">
       <c r="F5" s="2"/>
       <c r="J5" s="107"/>
       <c r="K5" s="36"/>
@@ -24747,7 +25574,7 @@
       <c r="R5" s="109"/>
       <c r="S5" s="109"/>
     </row>
-    <row r="6" spans="1:26" ht="14">
+    <row r="6" spans="1:26" ht="14.25">
       <c r="F6" s="2"/>
       <c r="G6" s="143"/>
       <c r="I6" s="188"/>
@@ -24757,7 +25584,7 @@
       <c r="R6" s="109"/>
       <c r="S6" s="109"/>
     </row>
-    <row r="7" spans="1:26" ht="14">
+    <row r="7" spans="1:26" ht="14.25">
       <c r="F7" s="2"/>
       <c r="G7" s="218"/>
       <c r="H7" s="2"/>
@@ -24768,7 +25595,7 @@
       <c r="R7" s="109"/>
       <c r="S7" s="109"/>
     </row>
-    <row r="8" spans="1:26" ht="14">
+    <row r="8" spans="1:26" ht="14.25">
       <c r="F8" s="2"/>
       <c r="G8" s="218"/>
       <c r="H8" s="2"/>
@@ -24779,7 +25606,7 @@
       <c r="R8" s="109"/>
       <c r="S8" s="109"/>
     </row>
-    <row r="9" spans="1:26" ht="14">
+    <row r="9" spans="1:26" ht="14.25">
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -24791,7 +25618,7 @@
       <c r="R9" s="109"/>
       <c r="S9" s="109"/>
     </row>
-    <row r="10" spans="1:26" ht="14">
+    <row r="10" spans="1:26" ht="14.25">
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -24803,7 +25630,7 @@
       <c r="R10" s="109"/>
       <c r="S10" s="109"/>
     </row>
-    <row r="11" spans="1:26" ht="14">
+    <row r="11" spans="1:26" ht="14.25">
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -24815,7 +25642,7 @@
       <c r="R11" s="109"/>
       <c r="S11" s="109"/>
     </row>
-    <row r="12" spans="1:26" ht="14">
+    <row r="12" spans="1:26" ht="14.25">
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -24827,7 +25654,7 @@
       <c r="R12" s="109"/>
       <c r="S12" s="109"/>
     </row>
-    <row r="13" spans="1:26" ht="14">
+    <row r="13" spans="1:26" ht="14.25">
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -24839,7 +25666,7 @@
       <c r="R13" s="109"/>
       <c r="S13" s="109"/>
     </row>
-    <row r="14" spans="1:26" ht="14">
+    <row r="14" spans="1:26" ht="14.25">
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -24851,7 +25678,7 @@
       <c r="R14" s="109"/>
       <c r="S14" s="109"/>
     </row>
-    <row r="15" spans="1:26" ht="14">
+    <row r="15" spans="1:26" ht="14.25">
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -24863,7 +25690,7 @@
       <c r="R15" s="109"/>
       <c r="S15" s="109"/>
     </row>
-    <row r="16" spans="1:26" ht="14">
+    <row r="16" spans="1:26" ht="14.25">
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -24875,7 +25702,7 @@
       <c r="R16" s="109"/>
       <c r="S16" s="109"/>
     </row>
-    <row r="17" spans="6:19" ht="14">
+    <row r="17" spans="6:19" ht="14.25">
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -24887,7 +25714,7 @@
       <c r="R17" s="109"/>
       <c r="S17" s="109"/>
     </row>
-    <row r="18" spans="6:19" ht="14">
+    <row r="18" spans="6:19" ht="14.25">
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -24898,7 +25725,7 @@
       <c r="R18" s="109"/>
       <c r="S18" s="109"/>
     </row>
-    <row r="19" spans="6:19" ht="14">
+    <row r="19" spans="6:19" ht="14.25">
       <c r="F19" s="2"/>
       <c r="I19" s="115"/>
       <c r="J19" s="141"/>
@@ -24908,7 +25735,7 @@
       <c r="R19" s="109"/>
       <c r="S19" s="109"/>
     </row>
-    <row r="20" spans="6:19" ht="14">
+    <row r="20" spans="6:19" ht="14.25">
       <c r="F20" s="2"/>
       <c r="I20" s="107"/>
       <c r="J20" s="107"/>
@@ -24917,7 +25744,7 @@
       <c r="R20" s="109"/>
       <c r="S20" s="109"/>
     </row>
-    <row r="21" spans="6:19" ht="14">
+    <row r="21" spans="6:19" ht="14.25">
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -24928,7 +25755,7 @@
       <c r="R21" s="109"/>
       <c r="S21" s="109"/>
     </row>
-    <row r="22" spans="6:19" ht="14">
+    <row r="22" spans="6:19" ht="14.25">
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -24940,7 +25767,7 @@
       <c r="R22" s="109"/>
       <c r="S22" s="109"/>
     </row>
-    <row r="23" spans="6:19" ht="14">
+    <row r="23" spans="6:19" ht="14.25">
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -24952,7 +25779,7 @@
       <c r="R23" s="109"/>
       <c r="S23" s="109"/>
     </row>
-    <row r="24" spans="6:19" ht="14">
+    <row r="24" spans="6:19" ht="14.25">
       <c r="J24" s="33"/>
       <c r="L24" s="36"/>
       <c r="M24" s="46"/>
@@ -24960,7 +25787,7 @@
       <c r="R24" s="109"/>
       <c r="S24" s="109"/>
     </row>
-    <row r="25" spans="6:19" ht="14">
+    <row r="25" spans="6:19" ht="14.25">
       <c r="F25" s="2"/>
       <c r="I25" s="107"/>
       <c r="J25" s="107"/>
@@ -24971,7 +25798,7 @@
       <c r="R25" s="109"/>
       <c r="S25" s="109"/>
     </row>
-    <row r="26" spans="6:19" ht="14">
+    <row r="26" spans="6:19" ht="14.25">
       <c r="F26" s="2"/>
       <c r="J26" s="107"/>
       <c r="K26" s="107"/>
@@ -24981,7 +25808,7 @@
       <c r="R26" s="109"/>
       <c r="S26" s="109"/>
     </row>
-    <row r="27" spans="6:19" ht="14">
+    <row r="27" spans="6:19" ht="14.25">
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="I27" s="107"/>
@@ -24992,7 +25819,7 @@
       <c r="R27" s="109"/>
       <c r="S27" s="109"/>
     </row>
-    <row r="28" spans="6:19" ht="14">
+    <row r="28" spans="6:19" ht="14.25">
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="I28" s="107"/>
@@ -25003,7 +25830,7 @@
       <c r="R28" s="109"/>
       <c r="S28" s="109"/>
     </row>
-    <row r="29" spans="6:19" ht="14">
+    <row r="29" spans="6:19" ht="14.25">
       <c r="F29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="107"/>
@@ -25014,7 +25841,7 @@
       <c r="R29" s="109"/>
       <c r="S29" s="109"/>
     </row>
-    <row r="30" spans="6:19" ht="14">
+    <row r="30" spans="6:19" ht="14.25">
       <c r="G30" s="2"/>
       <c r="I30" s="188"/>
       <c r="J30" s="107"/>
@@ -25024,7 +25851,7 @@
       <c r="R30" s="109"/>
       <c r="S30" s="109"/>
     </row>
-    <row r="31" spans="6:19" ht="14">
+    <row r="31" spans="6:19" ht="14.25">
       <c r="J31" s="107"/>
       <c r="K31" s="107"/>
       <c r="L31" s="36"/>
@@ -25033,7 +25860,7 @@
       <c r="R31" s="109"/>
       <c r="S31" s="109"/>
     </row>
-    <row r="32" spans="6:19" ht="14">
+    <row r="32" spans="6:19" ht="14.25">
       <c r="G32" s="2"/>
       <c r="J32" s="107"/>
       <c r="K32" s="107"/>
@@ -25043,7 +25870,7 @@
       <c r="R32" s="109"/>
       <c r="S32" s="109"/>
     </row>
-    <row r="33" spans="1:19" ht="14">
+    <row r="33" spans="1:19" ht="14.25">
       <c r="H33" s="145"/>
       <c r="I33" s="107"/>
       <c r="J33" s="110"/>
@@ -25053,7 +25880,7 @@
       <c r="R33" s="36"/>
       <c r="S33" s="36"/>
     </row>
-    <row r="34" spans="1:19" ht="14">
+    <row r="34" spans="1:19" ht="14.25">
       <c r="I34" s="107"/>
       <c r="J34" s="107"/>
       <c r="L34" s="36"/>
@@ -25157,7 +25984,7 @@
       <c r="R45" s="109"/>
       <c r="S45" s="32"/>
     </row>
-    <row r="46" spans="1:19" ht="14">
+    <row r="46" spans="1:19" ht="14.25">
       <c r="A46" s="120"/>
       <c r="F46" s="111"/>
       <c r="I46" s="107"/>
@@ -25252,20 +26079,20 @@
       <selection activeCell="A4" sqref="A4:XFD240"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="7" width="8.6640625" customWidth="1"/>
-    <col min="8" max="8" width="28.6640625" customWidth="1"/>
+    <col min="5" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="90.33203125" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" customWidth="1"/>
-    <col min="14" max="1010" width="8.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="90.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
+    <col min="14" max="1010" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18">
@@ -25342,7 +26169,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="56">
+    <row r="3" spans="1:16" ht="51">
       <c r="A3" s="28" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
RET-4288: nonprod.json support and CaseFlags nonprod.json example (#551)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\fergusoshea\et-ccd-definitions-scotland\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jack\et-ccd-definitions-scotland\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40113A3E-F1C4-4437-8CDB-1D8BB5FCD4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7823E5-6906-4F5C-88DC-64D3D65975D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20625" tabRatio="500" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="36660" windowHeight="19395" tabRatio="500" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchParty" sheetId="36" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">AuthorisationCaseField!$A$1:$D$517</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="25" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEvent!$A$3:$Z$31</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseEventToFields!$A$3:$P$231</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseEventToFields!$A$3:$Q$231</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">CaseField!$A$3:$U$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CaseRoles!$A$3:$F$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CaseTypeTab!$A$3:$P$54</definedName>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="377">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -15499,7 +15499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C4F7720-24EC-4BC8-BFE2-934342B17442}">
   <dimension ref="A1:E249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -26073,10 +26073,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:P240"/>
+  <dimension ref="A1:Q240"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD240"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
@@ -26084,18 +26084,18 @@
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="33.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="90.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" customWidth="1"/>
-    <col min="14" max="1010" width="8.7109375" customWidth="1"/>
+    <col min="4" max="5" width="18" customWidth="1"/>
+    <col min="6" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="90.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" customWidth="1"/>
+    <col min="15" max="1011" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18">
+    <row r="1" spans="1:17" ht="18">
       <c r="A1" s="35" t="s">
         <v>71</v>
       </c>
@@ -26106,22 +26106,23 @@
         <v>2</v>
       </c>
       <c r="D1" s="36"/>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="36"/>
+      <c r="F1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="36"/>
       <c r="G1" s="36"/>
       <c r="H1" s="36"/>
       <c r="I1" s="36"/>
       <c r="J1" s="36"/>
       <c r="K1" s="36"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="39"/>
       <c r="N1" s="36"/>
       <c r="O1" s="36"/>
-      <c r="P1" s="39"/>
-    </row>
-    <row r="2" spans="1:16" ht="144" customHeight="1">
+      <c r="P1" s="36"/>
+      <c r="Q1" s="39"/>
+    </row>
+    <row r="2" spans="1:17" ht="144" customHeight="1">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
@@ -26134,42 +26135,43 @@
       <c r="D2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="24"/>
+      <c r="F2" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="G2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="H2" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="I2" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="J2" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="23"/>
+      <c r="L2" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="M2" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="23" t="s">
+      <c r="N2" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="O2" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="23" t="s">
+      <c r="P2" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="P2" s="25" t="s">
+      <c r="Q2" s="25" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="51">
+    <row r="3" spans="1:17" ht="51">
       <c r="A3" s="28" t="s">
         <v>32</v>
       </c>
@@ -26182,1960 +26184,1981 @@
       <c r="D3" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="G3" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="H3" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="I3" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="J3" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="K3" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="L3" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="M3" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="M3" s="49" t="s">
+      <c r="N3" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="N3" s="27" t="s">
+      <c r="O3" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="O3" s="27" t="s">
+      <c r="P3" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="P3" s="27" t="s">
+      <c r="Q3" s="27" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
-      <c r="E4" s="1"/>
+    <row r="4" spans="1:17">
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="E5" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:17">
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="E6" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:17">
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="E7" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:17">
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="E8" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:17">
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="E9" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:17">
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="E10" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="N9" s="50"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:17">
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="E11" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:17">
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="E12" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:17">
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="E13" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:17">
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="E14" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:17">
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="E15" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:17">
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="E16" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:17">
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="5:14">
-      <c r="E17" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="6:15">
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="5:14">
-      <c r="E18" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="6:15">
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="33"/>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="5:14">
-      <c r="E19" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="33"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="6:15">
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="1"/>
-    </row>
-    <row r="20" spans="5:14">
-      <c r="E20" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="N19" s="50"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="6:15">
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="5:14">
-      <c r="E21" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="N20" s="50"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="6:15">
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="M21" s="50"/>
-      <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="5:14">
-      <c r="E22" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="6:15">
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="1"/>
-    </row>
-    <row r="23" spans="5:14">
-      <c r="E23" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="6:15">
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="5:14">
-      <c r="E24" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="6:15">
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="M24" s="50"/>
-      <c r="N24" s="1"/>
-    </row>
-    <row r="25" spans="5:14">
-      <c r="E25" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="6:15">
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="1"/>
-    </row>
-    <row r="26" spans="5:14">
-      <c r="E26" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="6:15">
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="M26" s="50"/>
-      <c r="N26" s="1"/>
-    </row>
-    <row r="27" spans="5:14">
-      <c r="E27" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="6:15">
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="M27" s="50"/>
-      <c r="N27" s="1"/>
-    </row>
-    <row r="28" spans="5:14">
-      <c r="E28" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="6:15">
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="M28" s="50"/>
-      <c r="N28" s="1"/>
-    </row>
-    <row r="29" spans="5:14">
-      <c r="E29" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="6:15">
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="M29" s="50"/>
-      <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="5:14">
-      <c r="E30" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="1"/>
+    </row>
+    <row r="30" spans="6:15">
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="107"/>
-      <c r="M30" s="50"/>
-      <c r="N30" s="1"/>
-    </row>
-    <row r="31" spans="5:14">
-      <c r="E31" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="107"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="1"/>
+    </row>
+    <row r="31" spans="6:15">
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="M31" s="50"/>
-      <c r="N31" s="1"/>
-    </row>
-    <row r="32" spans="5:14">
-      <c r="E32" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="N31" s="50"/>
+      <c r="O31" s="1"/>
+    </row>
+    <row r="32" spans="6:15">
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="107"/>
-      <c r="M32" s="50"/>
-      <c r="N32" s="1"/>
-    </row>
-    <row r="33" spans="5:14">
-      <c r="E33" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="107"/>
+      <c r="N32" s="50"/>
+      <c r="O32" s="1"/>
+    </row>
+    <row r="33" spans="6:15">
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="107"/>
-      <c r="M33" s="50"/>
-      <c r="N33" s="1"/>
-    </row>
-    <row r="34" spans="5:14">
-      <c r="E34" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="107"/>
+      <c r="N33" s="50"/>
+      <c r="O33" s="1"/>
+    </row>
+    <row r="34" spans="6:15">
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="107"/>
-      <c r="M34" s="50"/>
-      <c r="N34" s="1"/>
-    </row>
-    <row r="35" spans="5:14">
-      <c r="E35" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="107"/>
+      <c r="N34" s="50"/>
+      <c r="O34" s="1"/>
+    </row>
+    <row r="35" spans="6:15">
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="M35" s="50"/>
-      <c r="N35" s="1"/>
-    </row>
-    <row r="36" spans="5:14">
-      <c r="E36" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="N35" s="50"/>
+      <c r="O35" s="1"/>
+    </row>
+    <row r="36" spans="6:15">
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="M36" s="50"/>
-      <c r="N36" s="1"/>
-    </row>
-    <row r="37" spans="5:14">
-      <c r="E37" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="N36" s="50"/>
+      <c r="O36" s="1"/>
+    </row>
+    <row r="37" spans="6:15">
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="M37" s="50"/>
-      <c r="N37" s="1"/>
-    </row>
-    <row r="38" spans="5:14">
-      <c r="E38" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="N37" s="50"/>
+      <c r="O37" s="1"/>
+    </row>
+    <row r="38" spans="6:15">
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="M38" s="50"/>
-      <c r="N38" s="1"/>
-    </row>
-    <row r="39" spans="5:14">
-      <c r="E39" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="N38" s="50"/>
+      <c r="O38" s="1"/>
+    </row>
+    <row r="39" spans="6:15">
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="M39" s="50"/>
-      <c r="N39" s="1"/>
-    </row>
-    <row r="40" spans="5:14">
-      <c r="E40" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="N39" s="50"/>
+      <c r="O39" s="1"/>
+    </row>
+    <row r="40" spans="6:15">
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="M40" s="50"/>
-      <c r="N40" s="1"/>
-    </row>
-    <row r="41" spans="5:14">
-      <c r="E41" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="N40" s="50"/>
+      <c r="O40" s="1"/>
+    </row>
+    <row r="41" spans="6:15">
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="M41" s="50"/>
-      <c r="N41" s="1"/>
-    </row>
-    <row r="42" spans="5:14">
-      <c r="E42" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="N41" s="50"/>
+      <c r="O41" s="1"/>
+    </row>
+    <row r="42" spans="6:15">
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="M42" s="50"/>
-      <c r="N42" s="1"/>
-    </row>
-    <row r="43" spans="5:14">
-      <c r="E43" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="N42" s="50"/>
+      <c r="O42" s="1"/>
+    </row>
+    <row r="43" spans="6:15">
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="M43" s="50"/>
-      <c r="N43" s="1"/>
-    </row>
-    <row r="44" spans="5:14">
-      <c r="E44" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="N43" s="50"/>
+      <c r="O43" s="1"/>
+    </row>
+    <row r="44" spans="6:15">
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="M44" s="50"/>
-      <c r="N44" s="1"/>
-    </row>
-    <row r="45" spans="5:14">
-      <c r="E45" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="N44" s="50"/>
+      <c r="O44" s="1"/>
+    </row>
+    <row r="45" spans="6:15">
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="M45" s="50"/>
-      <c r="N45" s="1"/>
-    </row>
-    <row r="46" spans="5:14">
-      <c r="E46" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="N45" s="50"/>
+      <c r="O45" s="1"/>
+    </row>
+    <row r="46" spans="6:15">
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="M46" s="50"/>
-      <c r="N46" s="1"/>
-    </row>
-    <row r="47" spans="5:14">
-      <c r="E47" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="N46" s="50"/>
+      <c r="O46" s="1"/>
+    </row>
+    <row r="47" spans="6:15">
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="M47" s="50"/>
-      <c r="N47" s="1"/>
-    </row>
-    <row r="48" spans="5:14">
-      <c r="E48" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="N47" s="50"/>
+      <c r="O47" s="1"/>
+    </row>
+    <row r="48" spans="6:15">
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="M48" s="50"/>
-      <c r="N48" s="1"/>
-    </row>
-    <row r="49" spans="5:14">
-      <c r="E49" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="N48" s="50"/>
+      <c r="O48" s="1"/>
+    </row>
+    <row r="49" spans="6:15">
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="M49" s="50"/>
-      <c r="N49" s="1"/>
-    </row>
-    <row r="50" spans="5:14">
-      <c r="E50" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="N49" s="50"/>
+      <c r="O49" s="1"/>
+    </row>
+    <row r="50" spans="6:15">
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="107"/>
-      <c r="M50" s="50"/>
-      <c r="N50" s="1"/>
-    </row>
-    <row r="51" spans="5:14">
-      <c r="E51" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="107"/>
+      <c r="N50" s="50"/>
+      <c r="O50" s="1"/>
+    </row>
+    <row r="51" spans="6:15">
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="107"/>
-      <c r="M51" s="50"/>
-      <c r="N51" s="1"/>
-    </row>
-    <row r="52" spans="5:14">
-      <c r="E52" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="107"/>
+      <c r="N51" s="50"/>
+      <c r="O51" s="1"/>
+    </row>
+    <row r="52" spans="6:15">
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="M52" s="50"/>
-      <c r="N52" s="1"/>
-    </row>
-    <row r="53" spans="5:14">
-      <c r="E53" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="N52" s="50"/>
+      <c r="O52" s="1"/>
+    </row>
+    <row r="53" spans="6:15">
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="M53" s="50"/>
-      <c r="N53" s="1"/>
-    </row>
-    <row r="54" spans="5:14">
-      <c r="E54" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="N53" s="50"/>
+      <c r="O53" s="1"/>
+    </row>
+    <row r="54" spans="6:15">
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="M54" s="50"/>
-      <c r="N54" s="1"/>
-    </row>
-    <row r="55" spans="5:14">
-      <c r="E55" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="N54" s="50"/>
+      <c r="O54" s="1"/>
+    </row>
+    <row r="55" spans="6:15">
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="M55" s="50"/>
-      <c r="N55" s="1"/>
-    </row>
-    <row r="56" spans="5:14">
-      <c r="E56" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="N55" s="50"/>
+      <c r="O55" s="1"/>
+    </row>
+    <row r="56" spans="6:15">
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="M56" s="50"/>
-      <c r="N56" s="1"/>
-    </row>
-    <row r="57" spans="5:14">
-      <c r="E57" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="N56" s="50"/>
+      <c r="O56" s="1"/>
+    </row>
+    <row r="57" spans="6:15">
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
-      <c r="K57" s="1"/>
-      <c r="M57" s="50"/>
-      <c r="N57" s="1"/>
-    </row>
-    <row r="58" spans="5:14">
-      <c r="E58" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="N57" s="50"/>
+      <c r="O57" s="1"/>
+    </row>
+    <row r="58" spans="6:15">
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="M58" s="50"/>
-      <c r="N58" s="1"/>
-    </row>
-    <row r="59" spans="5:14">
-      <c r="E59" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="N58" s="50"/>
+      <c r="O58" s="1"/>
+    </row>
+    <row r="59" spans="6:15">
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
-      <c r="K59" s="1"/>
-      <c r="M59" s="50"/>
-      <c r="N59" s="1"/>
-    </row>
-    <row r="60" spans="5:14">
-      <c r="E60" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="N59" s="50"/>
+      <c r="O59" s="1"/>
+    </row>
+    <row r="60" spans="6:15">
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
-      <c r="K60" s="1"/>
-      <c r="M60" s="50"/>
-      <c r="N60" s="1"/>
-    </row>
-    <row r="61" spans="5:14">
-      <c r="E61" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="N60" s="50"/>
+      <c r="O60" s="1"/>
+    </row>
+    <row r="61" spans="6:15">
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="M61" s="50"/>
-      <c r="N61" s="1"/>
-    </row>
-    <row r="62" spans="5:14">
-      <c r="E62" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="N61" s="50"/>
+      <c r="O61" s="1"/>
+    </row>
+    <row r="62" spans="6:15">
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
-      <c r="K62" s="1"/>
-      <c r="M62" s="50"/>
-      <c r="N62" s="1"/>
-    </row>
-    <row r="63" spans="5:14">
-      <c r="E63" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="N62" s="50"/>
+      <c r="O62" s="1"/>
+    </row>
+    <row r="63" spans="6:15">
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="M63" s="50"/>
-      <c r="N63" s="1"/>
-    </row>
-    <row r="64" spans="5:14">
-      <c r="E64" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="N63" s="50"/>
+      <c r="O63" s="1"/>
+    </row>
+    <row r="64" spans="6:15">
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="M64" s="50"/>
-      <c r="N64" s="1"/>
-    </row>
-    <row r="65" spans="5:14">
-      <c r="E65" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="N64" s="50"/>
+      <c r="O64" s="1"/>
+    </row>
+    <row r="65" spans="6:15">
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="M65" s="50"/>
-      <c r="N65" s="1"/>
-    </row>
-    <row r="66" spans="5:14">
-      <c r="E66" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="N65" s="50"/>
+      <c r="O65" s="1"/>
+    </row>
+    <row r="66" spans="6:15">
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
-      <c r="K66" s="1"/>
-      <c r="M66" s="50"/>
-      <c r="N66" s="1"/>
-    </row>
-    <row r="67" spans="5:14">
-      <c r="E67" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="N66" s="50"/>
+      <c r="O66" s="1"/>
+    </row>
+    <row r="67" spans="6:15">
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
-      <c r="K67" s="1"/>
-      <c r="M67" s="50"/>
-      <c r="N67" s="1"/>
-    </row>
-    <row r="68" spans="5:14">
-      <c r="E68" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="N67" s="50"/>
+      <c r="O67" s="1"/>
+    </row>
+    <row r="68" spans="6:15">
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
-      <c r="K68" s="1"/>
-      <c r="M68" s="50"/>
-      <c r="N68" s="1"/>
-    </row>
-    <row r="69" spans="5:14">
-      <c r="E69" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="N68" s="50"/>
+      <c r="O68" s="1"/>
+    </row>
+    <row r="69" spans="6:15">
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="M69" s="50"/>
-      <c r="N69" s="1"/>
-    </row>
-    <row r="70" spans="5:14">
-      <c r="E70" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="N69" s="50"/>
+      <c r="O69" s="1"/>
+    </row>
+    <row r="70" spans="6:15">
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="M70" s="50"/>
-      <c r="N70" s="1"/>
-    </row>
-    <row r="71" spans="5:14">
-      <c r="E71" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="N70" s="50"/>
+      <c r="O70" s="1"/>
+    </row>
+    <row r="71" spans="6:15">
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
-      <c r="K71" s="1"/>
-      <c r="M71" s="50"/>
-      <c r="N71" s="1"/>
-    </row>
-    <row r="72" spans="5:14">
-      <c r="E72" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="N71" s="50"/>
+      <c r="O71" s="1"/>
+    </row>
+    <row r="72" spans="6:15">
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
-      <c r="K72" s="1"/>
-      <c r="M72" s="50"/>
-      <c r="N72" s="1"/>
-    </row>
-    <row r="73" spans="5:14">
-      <c r="E73" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="N72" s="50"/>
+      <c r="O72" s="1"/>
+    </row>
+    <row r="73" spans="6:15">
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
-      <c r="K73" s="1"/>
-      <c r="M73" s="50"/>
-      <c r="N73" s="1"/>
-    </row>
-    <row r="74" spans="5:14">
-      <c r="E74" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="N73" s="50"/>
+      <c r="O73" s="1"/>
+    </row>
+    <row r="74" spans="6:15">
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="M74" s="50"/>
-      <c r="N74" s="1"/>
-    </row>
-    <row r="75" spans="5:14">
-      <c r="E75" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="N74" s="50"/>
+      <c r="O74" s="1"/>
+    </row>
+    <row r="75" spans="6:15">
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
-      <c r="K75" s="1"/>
-      <c r="M75" s="50"/>
-      <c r="N75" s="1"/>
-    </row>
-    <row r="76" spans="5:14">
-      <c r="E76" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="N75" s="50"/>
+      <c r="O75" s="1"/>
+    </row>
+    <row r="76" spans="6:15">
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
-      <c r="K76" s="1"/>
-      <c r="M76" s="50"/>
-      <c r="N76" s="1"/>
-    </row>
-    <row r="77" spans="5:14">
-      <c r="E77" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="N76" s="50"/>
+      <c r="O76" s="1"/>
+    </row>
+    <row r="77" spans="6:15">
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
-      <c r="K77" s="1"/>
-      <c r="L77" s="33"/>
-      <c r="M77" s="50"/>
-      <c r="N77" s="1"/>
-    </row>
-    <row r="78" spans="5:14">
-      <c r="E78" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="33"/>
+      <c r="N77" s="50"/>
+      <c r="O77" s="1"/>
+    </row>
+    <row r="78" spans="6:15">
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
-      <c r="K78" s="1"/>
-      <c r="M78" s="50"/>
-      <c r="N78" s="1"/>
-    </row>
-    <row r="79" spans="5:14">
-      <c r="E79" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="N78" s="50"/>
+      <c r="O78" s="1"/>
+    </row>
+    <row r="79" spans="6:15">
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
-      <c r="K79" s="1"/>
-      <c r="M79" s="50"/>
-      <c r="N79" s="1"/>
-    </row>
-    <row r="80" spans="5:14">
-      <c r="E80" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="L79" s="1"/>
+      <c r="N79" s="50"/>
+      <c r="O79" s="1"/>
+    </row>
+    <row r="80" spans="6:15">
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
-      <c r="K80" s="1"/>
-      <c r="L80" s="107"/>
-      <c r="M80" s="50"/>
-      <c r="N80" s="1"/>
-    </row>
-    <row r="81" spans="3:14">
-      <c r="E81" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="L80" s="1"/>
+      <c r="M80" s="107"/>
+      <c r="N80" s="50"/>
+      <c r="O80" s="1"/>
+    </row>
+    <row r="81" spans="3:15">
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
-      <c r="K81" s="1"/>
-      <c r="L81" s="107"/>
-      <c r="M81" s="50"/>
-      <c r="N81" s="1"/>
-    </row>
-    <row r="82" spans="3:14">
-      <c r="E82" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="L81" s="1"/>
+      <c r="M81" s="107"/>
+      <c r="N81" s="50"/>
+      <c r="O81" s="1"/>
+    </row>
+    <row r="82" spans="3:15">
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
-      <c r="K82" s="1"/>
-      <c r="L82" s="107"/>
-      <c r="M82" s="50"/>
-      <c r="N82" s="1"/>
-    </row>
-    <row r="83" spans="3:14">
-      <c r="E83" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="L82" s="1"/>
+      <c r="M82" s="107"/>
+      <c r="N82" s="50"/>
+      <c r="O82" s="1"/>
+    </row>
+    <row r="83" spans="3:15">
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
-      <c r="K83" s="1"/>
-      <c r="L83" s="107"/>
-      <c r="M83" s="50"/>
-      <c r="N83" s="1"/>
-    </row>
-    <row r="84" spans="3:14">
-      <c r="E84" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="L83" s="1"/>
+      <c r="M83" s="107"/>
+      <c r="N83" s="50"/>
+      <c r="O83" s="1"/>
+    </row>
+    <row r="84" spans="3:15">
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
-      <c r="K84" s="1"/>
-      <c r="L84" s="107"/>
-      <c r="M84" s="50"/>
-      <c r="N84" s="1"/>
-    </row>
-    <row r="85" spans="3:14">
-      <c r="E85" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="L84" s="1"/>
+      <c r="M84" s="107"/>
+      <c r="N84" s="50"/>
+      <c r="O84" s="1"/>
+    </row>
+    <row r="85" spans="3:15">
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
-      <c r="K85" s="1"/>
-      <c r="L85" s="107"/>
-      <c r="M85" s="50"/>
-      <c r="N85" s="1"/>
-    </row>
-    <row r="86" spans="3:14">
-      <c r="E86" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="L85" s="1"/>
+      <c r="M85" s="107"/>
+      <c r="N85" s="50"/>
+      <c r="O85" s="1"/>
+    </row>
+    <row r="86" spans="3:15">
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
-      <c r="K86" s="1"/>
-      <c r="L86" s="107"/>
-      <c r="M86" s="50"/>
-      <c r="N86" s="1"/>
-    </row>
-    <row r="87" spans="3:14">
-      <c r="E87" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="L86" s="1"/>
+      <c r="M86" s="107"/>
+      <c r="N86" s="50"/>
+      <c r="O86" s="1"/>
+    </row>
+    <row r="87" spans="3:15">
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
-      <c r="K87" s="1"/>
-      <c r="L87" s="107"/>
-      <c r="M87" s="50"/>
-      <c r="N87" s="1"/>
-    </row>
-    <row r="88" spans="3:14">
-      <c r="E88" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="L87" s="1"/>
+      <c r="M87" s="107"/>
+      <c r="N87" s="50"/>
+      <c r="O87" s="1"/>
+    </row>
+    <row r="88" spans="3:15">
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
-      <c r="K88" s="1"/>
-      <c r="L88" s="107"/>
-      <c r="M88" s="50"/>
-      <c r="N88" s="1"/>
-    </row>
-    <row r="89" spans="3:14">
-      <c r="E89" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="L88" s="1"/>
+      <c r="M88" s="107"/>
+      <c r="N88" s="50"/>
+      <c r="O88" s="1"/>
+    </row>
+    <row r="89" spans="3:15">
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
-      <c r="K89" s="1"/>
-      <c r="L89" s="107"/>
-      <c r="M89" s="50"/>
-      <c r="N89" s="1"/>
-    </row>
-    <row r="90" spans="3:14">
-      <c r="E90" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="L89" s="1"/>
+      <c r="M89" s="107"/>
+      <c r="N89" s="50"/>
+      <c r="O89" s="1"/>
+    </row>
+    <row r="90" spans="3:15">
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
-      <c r="K90" s="1"/>
-      <c r="L90" s="107"/>
-      <c r="M90" s="50"/>
-      <c r="N90" s="1"/>
-    </row>
-    <row r="91" spans="3:14">
-      <c r="E91" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="L90" s="1"/>
+      <c r="M90" s="107"/>
+      <c r="N90" s="50"/>
+      <c r="O90" s="1"/>
+    </row>
+    <row r="91" spans="3:15">
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
-      <c r="K91" s="1"/>
-      <c r="L91" s="107"/>
-      <c r="M91" s="50"/>
-      <c r="N91" s="1"/>
-    </row>
-    <row r="92" spans="3:14">
-      <c r="E92" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="L91" s="1"/>
+      <c r="M91" s="107"/>
+      <c r="N91" s="50"/>
+      <c r="O91" s="1"/>
+    </row>
+    <row r="92" spans="3:15">
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
-      <c r="K92" s="1"/>
-      <c r="L92" s="107"/>
-      <c r="M92" s="50"/>
-      <c r="N92" s="1"/>
-    </row>
-    <row r="93" spans="3:14">
+      <c r="H92" s="1"/>
+      <c r="L92" s="1"/>
+      <c r="M92" s="107"/>
+      <c r="N92" s="50"/>
+      <c r="O92" s="1"/>
+    </row>
+    <row r="93" spans="3:15">
       <c r="C93" s="108"/>
-      <c r="E93" s="1"/>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
-      <c r="K93" s="1"/>
-      <c r="L93" s="107"/>
-      <c r="M93" s="50"/>
-      <c r="N93" s="1"/>
-    </row>
-    <row r="94" spans="3:14">
+      <c r="H93" s="1"/>
+      <c r="L93" s="1"/>
+      <c r="M93" s="107"/>
+      <c r="N93" s="50"/>
+      <c r="O93" s="1"/>
+    </row>
+    <row r="94" spans="3:15">
       <c r="C94" s="108"/>
-      <c r="E94" s="1"/>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
-      <c r="K94" s="1"/>
-      <c r="L94" s="107"/>
-      <c r="M94" s="50"/>
-      <c r="N94" s="1"/>
-    </row>
-    <row r="95" spans="3:14">
-      <c r="E95" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="L94" s="1"/>
+      <c r="M94" s="107"/>
+      <c r="N94" s="50"/>
+      <c r="O94" s="1"/>
+    </row>
+    <row r="95" spans="3:15">
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
-      <c r="K95" s="1"/>
-      <c r="L95" s="107"/>
-      <c r="M95" s="50"/>
-      <c r="N95" s="1"/>
-    </row>
-    <row r="96" spans="3:14">
-      <c r="E96" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="107"/>
+      <c r="N95" s="50"/>
+      <c r="O95" s="1"/>
+    </row>
+    <row r="96" spans="3:15">
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
-      <c r="K96" s="1"/>
-      <c r="L96" s="107"/>
-      <c r="M96" s="50"/>
-      <c r="N96" s="1"/>
-    </row>
-    <row r="97" spans="3:14">
-      <c r="E97" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="L96" s="1"/>
+      <c r="M96" s="107"/>
+      <c r="N96" s="50"/>
+      <c r="O96" s="1"/>
+    </row>
+    <row r="97" spans="3:15">
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
-      <c r="K97" s="1"/>
-      <c r="L97" s="107"/>
-      <c r="M97" s="50"/>
-      <c r="N97" s="1"/>
-    </row>
-    <row r="98" spans="3:14">
-      <c r="E98" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="107"/>
+      <c r="N97" s="50"/>
+      <c r="O97" s="1"/>
+    </row>
+    <row r="98" spans="3:15">
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
-      <c r="K98" s="1"/>
-      <c r="L98" s="107"/>
-      <c r="M98" s="50"/>
-      <c r="N98" s="1"/>
-    </row>
-    <row r="99" spans="3:14">
-      <c r="E99" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="107"/>
+      <c r="N98" s="50"/>
+      <c r="O98" s="1"/>
+    </row>
+    <row r="99" spans="3:15">
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
-      <c r="K99" s="1"/>
-      <c r="L99" s="107"/>
-      <c r="M99" s="50"/>
-      <c r="N99" s="1"/>
-    </row>
-    <row r="100" spans="3:14">
-      <c r="E100" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="L99" s="1"/>
+      <c r="M99" s="107"/>
+      <c r="N99" s="50"/>
+      <c r="O99" s="1"/>
+    </row>
+    <row r="100" spans="3:15">
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
-      <c r="K100" s="1"/>
-      <c r="L100" s="107"/>
-      <c r="M100" s="50"/>
-      <c r="N100" s="1"/>
-    </row>
-    <row r="101" spans="3:14">
-      <c r="E101" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="L100" s="1"/>
+      <c r="M100" s="107"/>
+      <c r="N100" s="50"/>
+      <c r="O100" s="1"/>
+    </row>
+    <row r="101" spans="3:15">
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
-      <c r="K101" s="1"/>
-      <c r="L101" s="107"/>
-      <c r="M101" s="50"/>
-      <c r="N101" s="1"/>
-    </row>
-    <row r="102" spans="3:14">
-      <c r="E102" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="L101" s="1"/>
+      <c r="M101" s="107"/>
+      <c r="N101" s="50"/>
+      <c r="O101" s="1"/>
+    </row>
+    <row r="102" spans="3:15">
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
-      <c r="K102" s="1"/>
-      <c r="L102" s="107"/>
-      <c r="M102" s="50"/>
-      <c r="N102" s="1"/>
-    </row>
-    <row r="103" spans="3:14">
-      <c r="E103" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="L102" s="1"/>
+      <c r="M102" s="107"/>
+      <c r="N102" s="50"/>
+      <c r="O102" s="1"/>
+    </row>
+    <row r="103" spans="3:15">
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
-      <c r="K103" s="1"/>
-      <c r="L103" s="107"/>
-      <c r="M103" s="50"/>
-      <c r="N103" s="1"/>
-    </row>
-    <row r="104" spans="3:14">
-      <c r="E104" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="L103" s="1"/>
+      <c r="M103" s="107"/>
+      <c r="N103" s="50"/>
+      <c r="O103" s="1"/>
+    </row>
+    <row r="104" spans="3:15">
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
-      <c r="K104" s="1"/>
-      <c r="L104" s="107"/>
-      <c r="M104" s="50"/>
-      <c r="N104" s="1"/>
-    </row>
-    <row r="105" spans="3:14">
-      <c r="E105" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="L104" s="1"/>
+      <c r="M104" s="107"/>
+      <c r="N104" s="50"/>
+      <c r="O104" s="1"/>
+    </row>
+    <row r="105" spans="3:15">
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
-      <c r="K105" s="1"/>
-      <c r="L105" s="107"/>
-      <c r="M105" s="50"/>
-      <c r="N105" s="1"/>
-    </row>
-    <row r="106" spans="3:14">
-      <c r="E106" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="L105" s="1"/>
+      <c r="M105" s="107"/>
+      <c r="N105" s="50"/>
+      <c r="O105" s="1"/>
+    </row>
+    <row r="106" spans="3:15">
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
-      <c r="K106" s="1"/>
-      <c r="L106" s="107"/>
-      <c r="M106" s="50"/>
-      <c r="N106" s="1"/>
-    </row>
-    <row r="107" spans="3:14">
-      <c r="E107" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="L106" s="1"/>
+      <c r="M106" s="107"/>
+      <c r="N106" s="50"/>
+      <c r="O106" s="1"/>
+    </row>
+    <row r="107" spans="3:15">
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
-      <c r="K107" s="1"/>
-      <c r="L107" s="107"/>
-      <c r="M107" s="50"/>
-      <c r="N107" s="1"/>
-    </row>
-    <row r="108" spans="3:14">
+      <c r="H107" s="1"/>
+      <c r="L107" s="1"/>
+      <c r="M107" s="107"/>
+      <c r="N107" s="50"/>
+      <c r="O107" s="1"/>
+    </row>
+    <row r="108" spans="3:15">
       <c r="C108" s="56"/>
-      <c r="E108" s="1"/>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
-      <c r="K108" s="1"/>
-      <c r="L108" s="107"/>
-      <c r="M108" s="50"/>
-      <c r="N108" s="1"/>
-    </row>
-    <row r="109" spans="3:14">
-      <c r="E109" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="L108" s="1"/>
+      <c r="M108" s="107"/>
+      <c r="N108" s="50"/>
+      <c r="O108" s="1"/>
+    </row>
+    <row r="109" spans="3:15">
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
-      <c r="K109" s="1"/>
-      <c r="L109" s="107"/>
-      <c r="M109" s="50"/>
-      <c r="N109" s="1"/>
-    </row>
-    <row r="110" spans="3:14">
-      <c r="E110" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="L109" s="1"/>
+      <c r="M109" s="107"/>
+      <c r="N109" s="50"/>
+      <c r="O109" s="1"/>
+    </row>
+    <row r="110" spans="3:15">
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
-      <c r="K110" s="1"/>
-      <c r="M110" s="50"/>
-      <c r="N110" s="1"/>
-    </row>
-    <row r="111" spans="3:14">
+      <c r="H110" s="1"/>
+      <c r="L110" s="1"/>
+      <c r="N110" s="50"/>
+      <c r="O110" s="1"/>
+    </row>
+    <row r="111" spans="3:15">
       <c r="D111" s="143"/>
-      <c r="E111" s="1"/>
+      <c r="E111" s="143"/>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
-      <c r="K111" s="1"/>
-      <c r="M111" s="50"/>
-      <c r="N111" s="1"/>
-    </row>
-    <row r="112" spans="3:14">
+      <c r="H111" s="1"/>
+      <c r="L111" s="1"/>
+      <c r="N111" s="50"/>
+      <c r="O111" s="1"/>
+    </row>
+    <row r="112" spans="3:15">
       <c r="D112" s="143"/>
-      <c r="E112" s="1"/>
+      <c r="E112" s="143"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
-      <c r="K112" s="1"/>
-      <c r="M112" s="50"/>
-      <c r="N112" s="1"/>
-    </row>
-    <row r="113" spans="5:14">
-      <c r="E113" s="1"/>
+      <c r="H112" s="1"/>
+      <c r="L112" s="1"/>
+      <c r="N112" s="50"/>
+      <c r="O112" s="1"/>
+    </row>
+    <row r="113" spans="6:15">
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
-      <c r="K113" s="1"/>
-      <c r="M113" s="50"/>
-      <c r="N113" s="1"/>
-    </row>
-    <row r="114" spans="5:14">
-      <c r="E114" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="L113" s="1"/>
+      <c r="N113" s="50"/>
+      <c r="O113" s="1"/>
+    </row>
+    <row r="114" spans="6:15">
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
-      <c r="K114" s="1"/>
-      <c r="M114" s="50"/>
-      <c r="N114" s="1"/>
-    </row>
-    <row r="115" spans="5:14">
-      <c r="E115" s="1"/>
+      <c r="H114" s="1"/>
+      <c r="L114" s="1"/>
+      <c r="N114" s="50"/>
+      <c r="O114" s="1"/>
+    </row>
+    <row r="115" spans="6:15">
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
-      <c r="K115" s="1"/>
-      <c r="M115" s="50"/>
-      <c r="N115" s="1"/>
-    </row>
-    <row r="116" spans="5:14">
-      <c r="E116" s="1"/>
+      <c r="H115" s="1"/>
+      <c r="L115" s="1"/>
+      <c r="N115" s="50"/>
+      <c r="O115" s="1"/>
+    </row>
+    <row r="116" spans="6:15">
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
-      <c r="K116" s="1"/>
-      <c r="N116" s="1"/>
-    </row>
-    <row r="117" spans="5:14">
-      <c r="E117" s="1"/>
+      <c r="H116" s="1"/>
+      <c r="L116" s="1"/>
+      <c r="O116" s="1"/>
+    </row>
+    <row r="117" spans="6:15">
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
-      <c r="K117" s="1"/>
-      <c r="L117" s="107"/>
-      <c r="M117" s="50"/>
-      <c r="N117" s="1"/>
-    </row>
-    <row r="118" spans="5:14">
-      <c r="E118" s="1"/>
+      <c r="H117" s="1"/>
+      <c r="L117" s="1"/>
+      <c r="M117" s="107"/>
+      <c r="N117" s="50"/>
+      <c r="O117" s="1"/>
+    </row>
+    <row r="118" spans="6:15">
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
-      <c r="K118" s="1"/>
-      <c r="M118" s="50"/>
-      <c r="N118" s="1"/>
-    </row>
-    <row r="119" spans="5:14">
-      <c r="E119" s="1"/>
+      <c r="H118" s="1"/>
+      <c r="L118" s="1"/>
+      <c r="N118" s="50"/>
+      <c r="O118" s="1"/>
+    </row>
+    <row r="119" spans="6:15">
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
-      <c r="K119" s="1"/>
-      <c r="M119" s="50"/>
-      <c r="N119" s="1"/>
-    </row>
-    <row r="120" spans="5:14">
-      <c r="E120" s="1"/>
+      <c r="H119" s="1"/>
+      <c r="L119" s="1"/>
+      <c r="N119" s="50"/>
+      <c r="O119" s="1"/>
+    </row>
+    <row r="120" spans="6:15">
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
-      <c r="K120" s="1"/>
-      <c r="L120" s="110"/>
-      <c r="N120" s="1"/>
-    </row>
-    <row r="121" spans="5:14">
-      <c r="E121" s="1"/>
+      <c r="H120" s="1"/>
+      <c r="L120" s="1"/>
+      <c r="M120" s="110"/>
+      <c r="O120" s="1"/>
+    </row>
+    <row r="121" spans="6:15">
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
-      <c r="K121" s="1"/>
-      <c r="N121" s="1"/>
-    </row>
-    <row r="122" spans="5:14">
-      <c r="E122" s="1"/>
+      <c r="H121" s="1"/>
+      <c r="L121" s="1"/>
+      <c r="O121" s="1"/>
+    </row>
+    <row r="122" spans="6:15">
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
-      <c r="K122" s="1"/>
-      <c r="N122" s="1"/>
-    </row>
-    <row r="123" spans="5:14">
-      <c r="E123" s="1"/>
+      <c r="H122" s="1"/>
+      <c r="L122" s="1"/>
+      <c r="O122" s="1"/>
+    </row>
+    <row r="123" spans="6:15">
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
-      <c r="K123" s="1"/>
-      <c r="N123" s="1"/>
-    </row>
-    <row r="124" spans="5:14">
-      <c r="E124" s="1"/>
+      <c r="H123" s="1"/>
+      <c r="L123" s="1"/>
+      <c r="O123" s="1"/>
+    </row>
+    <row r="124" spans="6:15">
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
-      <c r="K124" s="1"/>
-      <c r="N124" s="1"/>
-    </row>
-    <row r="125" spans="5:14">
-      <c r="E125" s="1"/>
+      <c r="H124" s="1"/>
+      <c r="L124" s="1"/>
+      <c r="O124" s="1"/>
+    </row>
+    <row r="125" spans="6:15">
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
-      <c r="K125" s="1"/>
-      <c r="N125" s="1"/>
-    </row>
-    <row r="126" spans="5:14">
-      <c r="E126" s="1"/>
+      <c r="H125" s="1"/>
+      <c r="L125" s="1"/>
+      <c r="O125" s="1"/>
+    </row>
+    <row r="126" spans="6:15">
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
-      <c r="K126" s="1"/>
-      <c r="L126" s="107"/>
-      <c r="N126" s="1"/>
-    </row>
-    <row r="127" spans="5:14">
-      <c r="E127" s="1"/>
+      <c r="H126" s="1"/>
+      <c r="L126" s="1"/>
+      <c r="M126" s="107"/>
+      <c r="O126" s="1"/>
+    </row>
+    <row r="127" spans="6:15">
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
-      <c r="K127" s="1"/>
-      <c r="N127" s="1"/>
-    </row>
-    <row r="128" spans="5:14">
-      <c r="E128" s="1"/>
+      <c r="H127" s="1"/>
+      <c r="L127" s="1"/>
+      <c r="O127" s="1"/>
+    </row>
+    <row r="128" spans="6:15">
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
-      <c r="K128" s="1"/>
-      <c r="N128" s="1"/>
-    </row>
-    <row r="129" spans="2:14">
-      <c r="E129" s="1"/>
+      <c r="H128" s="1"/>
+      <c r="L128" s="1"/>
+      <c r="O128" s="1"/>
+    </row>
+    <row r="129" spans="2:15">
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
-      <c r="K129" s="1"/>
-      <c r="N129" s="1"/>
-    </row>
-    <row r="130" spans="2:14">
-      <c r="E130" s="1"/>
+      <c r="H129" s="1"/>
+      <c r="L129" s="1"/>
+      <c r="O129" s="1"/>
+    </row>
+    <row r="130" spans="2:15">
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
-      <c r="K130" s="1"/>
-      <c r="N130" s="1"/>
-    </row>
-    <row r="131" spans="2:14">
-      <c r="E131" s="1"/>
+      <c r="H130" s="1"/>
+      <c r="L130" s="1"/>
+      <c r="O130" s="1"/>
+    </row>
+    <row r="131" spans="2:15">
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
-      <c r="K131" s="1"/>
-      <c r="N131" s="1"/>
-    </row>
-    <row r="132" spans="2:14">
-      <c r="E132" s="1"/>
+      <c r="H131" s="1"/>
+      <c r="L131" s="1"/>
+      <c r="O131" s="1"/>
+    </row>
+    <row r="132" spans="2:15">
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
-      <c r="K132" s="1"/>
-      <c r="N132" s="1"/>
-    </row>
-    <row r="133" spans="2:14">
-      <c r="E133" s="1"/>
+      <c r="H132" s="1"/>
+      <c r="L132" s="1"/>
+      <c r="O132" s="1"/>
+    </row>
+    <row r="133" spans="2:15">
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
-      <c r="K133" s="1"/>
-      <c r="N133" s="1"/>
-    </row>
-    <row r="134" spans="2:14">
-      <c r="E134" s="1"/>
+      <c r="H133" s="1"/>
+      <c r="L133" s="1"/>
+      <c r="O133" s="1"/>
+    </row>
+    <row r="134" spans="2:15">
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
-      <c r="K134" s="1"/>
-      <c r="N134" s="1"/>
-    </row>
-    <row r="135" spans="2:14">
+      <c r="H134" s="1"/>
+      <c r="L134" s="1"/>
+      <c r="O134" s="1"/>
+    </row>
+    <row r="135" spans="2:15">
       <c r="B135" s="36"/>
-      <c r="E135" s="1"/>
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
-      <c r="K135" s="1"/>
-      <c r="N135" s="1"/>
-    </row>
-    <row r="136" spans="2:14">
+      <c r="H135" s="1"/>
+      <c r="L135" s="1"/>
+      <c r="O135" s="1"/>
+    </row>
+    <row r="136" spans="2:15">
       <c r="B136" s="36"/>
-      <c r="E136" s="1"/>
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
-      <c r="K136" s="1"/>
-      <c r="N136" s="1"/>
-    </row>
-    <row r="137" spans="2:14">
+      <c r="H136" s="1"/>
+      <c r="L136" s="1"/>
+      <c r="O136" s="1"/>
+    </row>
+    <row r="137" spans="2:15">
       <c r="B137" s="36"/>
       <c r="C137" s="36"/>
-      <c r="E137" s="1"/>
       <c r="F137" s="1"/>
       <c r="G137" s="1"/>
-      <c r="K137" s="1"/>
-      <c r="N137" s="1"/>
-    </row>
-    <row r="138" spans="2:14">
-      <c r="E138" s="1"/>
+      <c r="H137" s="1"/>
+      <c r="L137" s="1"/>
+      <c r="O137" s="1"/>
+    </row>
+    <row r="138" spans="2:15">
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
-      <c r="K138" s="1"/>
-      <c r="N138" s="1"/>
-    </row>
-    <row r="139" spans="2:14">
-      <c r="E139" s="1"/>
+      <c r="H138" s="1"/>
+      <c r="L138" s="1"/>
+      <c r="O138" s="1"/>
+    </row>
+    <row r="139" spans="2:15">
       <c r="F139" s="1"/>
       <c r="G139" s="1"/>
-      <c r="K139" s="1"/>
-      <c r="N139" s="1"/>
-    </row>
-    <row r="140" spans="2:14">
+      <c r="H139" s="1"/>
+      <c r="L139" s="1"/>
+      <c r="O139" s="1"/>
+    </row>
+    <row r="140" spans="2:15">
       <c r="C140" s="36"/>
-      <c r="E140" s="1"/>
       <c r="F140" s="1"/>
       <c r="G140" s="1"/>
-      <c r="K140" s="1"/>
-      <c r="N140" s="1"/>
-    </row>
-    <row r="141" spans="2:14">
+      <c r="H140" s="1"/>
+      <c r="L140" s="1"/>
+      <c r="O140" s="1"/>
+    </row>
+    <row r="141" spans="2:15">
       <c r="C141" s="36"/>
-      <c r="E141" s="1"/>
       <c r="F141" s="1"/>
       <c r="G141" s="1"/>
-      <c r="K141" s="1"/>
-      <c r="N141" s="1"/>
-    </row>
-    <row r="142" spans="2:14">
-      <c r="E142" s="1"/>
+      <c r="H141" s="1"/>
+      <c r="L141" s="1"/>
+      <c r="O141" s="1"/>
+    </row>
+    <row r="142" spans="2:15">
       <c r="F142" s="1"/>
       <c r="G142" s="1"/>
-      <c r="K142" s="1"/>
-      <c r="N142" s="1"/>
-    </row>
-    <row r="143" spans="2:14">
+      <c r="H142" s="1"/>
+      <c r="L142" s="1"/>
+      <c r="O142" s="1"/>
+    </row>
+    <row r="143" spans="2:15">
       <c r="B143" s="36"/>
       <c r="C143" s="36"/>
-      <c r="E143" s="1"/>
       <c r="F143" s="1"/>
       <c r="G143" s="1"/>
-      <c r="K143" s="1"/>
-      <c r="N143" s="1"/>
-    </row>
-    <row r="144" spans="2:14">
+      <c r="H143" s="1"/>
+      <c r="L143" s="1"/>
+      <c r="O143" s="1"/>
+    </row>
+    <row r="144" spans="2:15">
       <c r="B144" s="36"/>
       <c r="C144" s="36"/>
-      <c r="E144" s="1"/>
       <c r="F144" s="1"/>
       <c r="G144" s="1"/>
-      <c r="K144" s="1"/>
-      <c r="N144" s="1"/>
-    </row>
-    <row r="145" spans="2:14">
+      <c r="H144" s="1"/>
+      <c r="L144" s="1"/>
+      <c r="O144" s="1"/>
+    </row>
+    <row r="145" spans="2:15">
       <c r="B145" s="36"/>
       <c r="C145" s="36"/>
-      <c r="E145" s="1"/>
       <c r="F145" s="1"/>
       <c r="G145" s="1"/>
-      <c r="K145" s="1"/>
-      <c r="N145" s="1"/>
-    </row>
-    <row r="146" spans="2:14">
-      <c r="E146" s="1"/>
+      <c r="H145" s="1"/>
+      <c r="L145" s="1"/>
+      <c r="O145" s="1"/>
+    </row>
+    <row r="146" spans="2:15">
       <c r="F146" s="1"/>
       <c r="G146" s="1"/>
-      <c r="K146" s="1"/>
-      <c r="M146" s="50"/>
-      <c r="N146" s="1"/>
-    </row>
-    <row r="147" spans="2:14">
-      <c r="E147" s="1"/>
+      <c r="H146" s="1"/>
+      <c r="L146" s="1"/>
+      <c r="N146" s="50"/>
+      <c r="O146" s="1"/>
+    </row>
+    <row r="147" spans="2:15">
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
-      <c r="K147" s="1"/>
-      <c r="M147" s="50"/>
-      <c r="N147" s="1"/>
-    </row>
-    <row r="148" spans="2:14">
-      <c r="E148" s="1"/>
+      <c r="H147" s="1"/>
+      <c r="L147" s="1"/>
+      <c r="N147" s="50"/>
+      <c r="O147" s="1"/>
+    </row>
+    <row r="148" spans="2:15">
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
-      <c r="K148" s="1"/>
-      <c r="M148" s="50"/>
-      <c r="N148" s="1"/>
-    </row>
-    <row r="149" spans="2:14">
-      <c r="E149" s="1"/>
+      <c r="H148" s="1"/>
+      <c r="L148" s="1"/>
+      <c r="N148" s="50"/>
+      <c r="O148" s="1"/>
+    </row>
+    <row r="149" spans="2:15">
       <c r="F149" s="1"/>
       <c r="G149" s="1"/>
-      <c r="K149" s="1"/>
-      <c r="M149" s="50"/>
-      <c r="N149" s="1"/>
-    </row>
-    <row r="150" spans="2:14">
-      <c r="E150" s="1"/>
+      <c r="H149" s="1"/>
+      <c r="L149" s="1"/>
+      <c r="N149" s="50"/>
+      <c r="O149" s="1"/>
+    </row>
+    <row r="150" spans="2:15">
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
-      <c r="K150" s="1"/>
-      <c r="M150" s="50"/>
-      <c r="N150" s="1"/>
-    </row>
-    <row r="151" spans="2:14">
-      <c r="E151" s="1"/>
+      <c r="H150" s="1"/>
+      <c r="L150" s="1"/>
+      <c r="N150" s="50"/>
+      <c r="O150" s="1"/>
+    </row>
+    <row r="151" spans="2:15">
       <c r="F151" s="1"/>
       <c r="G151" s="1"/>
-      <c r="K151" s="1"/>
-      <c r="M151" s="50"/>
-      <c r="N151" s="1"/>
-    </row>
-    <row r="152" spans="2:14">
-      <c r="E152" s="1"/>
+      <c r="H151" s="1"/>
+      <c r="L151" s="1"/>
+      <c r="N151" s="50"/>
+      <c r="O151" s="1"/>
+    </row>
+    <row r="152" spans="2:15">
       <c r="F152" s="1"/>
       <c r="G152" s="1"/>
-      <c r="K152" s="1"/>
-      <c r="N152" s="1"/>
-    </row>
-    <row r="153" spans="2:14">
-      <c r="E153" s="1"/>
+      <c r="H152" s="1"/>
+      <c r="L152" s="1"/>
+      <c r="O152" s="1"/>
+    </row>
+    <row r="153" spans="2:15">
       <c r="F153" s="1"/>
       <c r="G153" s="1"/>
-      <c r="K153" s="1"/>
-      <c r="N153" s="1"/>
-    </row>
-    <row r="154" spans="2:14">
-      <c r="E154" s="1"/>
+      <c r="H153" s="1"/>
+      <c r="L153" s="1"/>
+      <c r="O153" s="1"/>
+    </row>
+    <row r="154" spans="2:15">
       <c r="F154" s="1"/>
       <c r="G154" s="1"/>
-      <c r="K154" s="1"/>
-      <c r="N154" s="1"/>
-    </row>
-    <row r="155" spans="2:14">
-      <c r="E155" s="1"/>
+      <c r="H154" s="1"/>
+      <c r="L154" s="1"/>
+      <c r="O154" s="1"/>
+    </row>
+    <row r="155" spans="2:15">
       <c r="F155" s="1"/>
       <c r="G155" s="1"/>
-      <c r="K155" s="1"/>
-      <c r="N155" s="1"/>
-    </row>
-    <row r="156" spans="2:14">
-      <c r="E156" s="1"/>
+      <c r="H155" s="1"/>
+      <c r="L155" s="1"/>
+      <c r="O155" s="1"/>
+    </row>
+    <row r="156" spans="2:15">
       <c r="F156" s="1"/>
       <c r="G156" s="1"/>
-      <c r="K156" s="1"/>
-      <c r="N156" s="1"/>
-    </row>
-    <row r="157" spans="2:14">
-      <c r="E157" s="1"/>
+      <c r="H156" s="1"/>
+      <c r="L156" s="1"/>
+      <c r="O156" s="1"/>
+    </row>
+    <row r="157" spans="2:15">
       <c r="F157" s="1"/>
       <c r="G157" s="1"/>
-      <c r="K157" s="1"/>
-      <c r="N157" s="1"/>
-    </row>
-    <row r="158" spans="2:14">
-      <c r="E158" s="1"/>
+      <c r="H157" s="1"/>
+      <c r="L157" s="1"/>
+      <c r="O157" s="1"/>
+    </row>
+    <row r="158" spans="2:15">
       <c r="F158" s="1"/>
       <c r="G158" s="1"/>
-      <c r="K158" s="1"/>
-      <c r="N158" s="1"/>
-    </row>
-    <row r="159" spans="2:14">
-      <c r="E159" s="1"/>
+      <c r="H158" s="1"/>
+      <c r="L158" s="1"/>
+      <c r="O158" s="1"/>
+    </row>
+    <row r="159" spans="2:15">
       <c r="F159" s="1"/>
       <c r="G159" s="1"/>
-      <c r="K159" s="1"/>
-      <c r="N159" s="1"/>
-    </row>
-    <row r="160" spans="2:14">
-      <c r="E160" s="1"/>
+      <c r="H159" s="1"/>
+      <c r="L159" s="1"/>
+      <c r="O159" s="1"/>
+    </row>
+    <row r="160" spans="2:15">
       <c r="F160" s="1"/>
       <c r="G160" s="1"/>
-      <c r="K160" s="1"/>
-      <c r="N160" s="1"/>
-    </row>
-    <row r="161" spans="5:14">
-      <c r="E161" s="1"/>
+      <c r="H160" s="1"/>
+      <c r="L160" s="1"/>
+      <c r="O160" s="1"/>
+    </row>
+    <row r="161" spans="6:15">
       <c r="F161" s="1"/>
       <c r="G161" s="1"/>
-      <c r="K161" s="1"/>
-      <c r="N161" s="1"/>
-    </row>
-    <row r="162" spans="5:14">
-      <c r="E162" s="1"/>
+      <c r="H161" s="1"/>
+      <c r="L161" s="1"/>
+      <c r="O161" s="1"/>
+    </row>
+    <row r="162" spans="6:15">
       <c r="F162" s="1"/>
       <c r="G162" s="1"/>
-      <c r="K162" s="1"/>
-      <c r="N162" s="1"/>
-    </row>
-    <row r="163" spans="5:14">
-      <c r="E163" s="1"/>
+      <c r="H162" s="1"/>
+      <c r="L162" s="1"/>
+      <c r="O162" s="1"/>
+    </row>
+    <row r="163" spans="6:15">
       <c r="F163" s="1"/>
       <c r="G163" s="1"/>
-      <c r="K163" s="1"/>
-      <c r="N163" s="1"/>
-    </row>
-    <row r="164" spans="5:14">
-      <c r="E164" s="1"/>
+      <c r="H163" s="1"/>
+      <c r="L163" s="1"/>
+      <c r="O163" s="1"/>
+    </row>
+    <row r="164" spans="6:15">
       <c r="F164" s="1"/>
       <c r="G164" s="1"/>
-      <c r="K164" s="1"/>
-      <c r="N164" s="1"/>
-    </row>
-    <row r="165" spans="5:14">
-      <c r="E165" s="1"/>
+      <c r="H164" s="1"/>
+      <c r="L164" s="1"/>
+      <c r="O164" s="1"/>
+    </row>
+    <row r="165" spans="6:15">
       <c r="F165" s="1"/>
       <c r="G165" s="1"/>
-      <c r="K165" s="1"/>
-      <c r="L165" s="107"/>
-      <c r="N165" s="1"/>
-    </row>
-    <row r="166" spans="5:14">
-      <c r="E166" s="1"/>
+      <c r="H165" s="1"/>
+      <c r="L165" s="1"/>
+      <c r="M165" s="107"/>
+      <c r="O165" s="1"/>
+    </row>
+    <row r="166" spans="6:15">
       <c r="F166" s="1"/>
       <c r="G166" s="1"/>
-      <c r="K166" s="1"/>
-      <c r="N166" s="1"/>
-    </row>
-    <row r="167" spans="5:14">
-      <c r="E167" s="1"/>
+      <c r="H166" s="1"/>
+      <c r="L166" s="1"/>
+      <c r="O166" s="1"/>
+    </row>
+    <row r="167" spans="6:15">
       <c r="F167" s="1"/>
       <c r="G167" s="1"/>
-      <c r="K167" s="1"/>
-      <c r="N167" s="1"/>
-    </row>
-    <row r="168" spans="5:14">
-      <c r="E168" s="1"/>
+      <c r="H167" s="1"/>
+      <c r="L167" s="1"/>
+      <c r="O167" s="1"/>
+    </row>
+    <row r="168" spans="6:15">
       <c r="F168" s="1"/>
       <c r="G168" s="1"/>
-      <c r="K168" s="1"/>
-      <c r="N168" s="1"/>
-    </row>
-    <row r="169" spans="5:14">
-      <c r="E169" s="1"/>
+      <c r="H168" s="1"/>
+      <c r="L168" s="1"/>
+      <c r="O168" s="1"/>
+    </row>
+    <row r="169" spans="6:15">
       <c r="F169" s="1"/>
       <c r="G169" s="1"/>
-      <c r="K169" s="1"/>
-      <c r="N169" s="1"/>
-    </row>
-    <row r="170" spans="5:14">
-      <c r="E170" s="1"/>
+      <c r="H169" s="1"/>
+      <c r="L169" s="1"/>
+      <c r="O169" s="1"/>
+    </row>
+    <row r="170" spans="6:15">
       <c r="F170" s="1"/>
       <c r="G170" s="1"/>
-      <c r="K170" s="1"/>
-      <c r="N170" s="1"/>
-    </row>
-    <row r="171" spans="5:14">
-      <c r="E171" s="1"/>
+      <c r="H170" s="1"/>
+      <c r="L170" s="1"/>
+      <c r="O170" s="1"/>
+    </row>
+    <row r="171" spans="6:15">
       <c r="F171" s="1"/>
       <c r="G171" s="1"/>
-      <c r="K171" s="1"/>
-      <c r="N171" s="1"/>
-    </row>
-    <row r="172" spans="5:14">
-      <c r="E172" s="1"/>
+      <c r="H171" s="1"/>
+      <c r="L171" s="1"/>
+      <c r="O171" s="1"/>
+    </row>
+    <row r="172" spans="6:15">
       <c r="F172" s="1"/>
       <c r="G172" s="1"/>
-      <c r="K172" s="1"/>
-      <c r="L172" s="107"/>
-      <c r="N172" s="1"/>
-    </row>
-    <row r="173" spans="5:14">
-      <c r="E173" s="1"/>
+      <c r="H172" s="1"/>
+      <c r="L172" s="1"/>
+      <c r="M172" s="107"/>
+      <c r="O172" s="1"/>
+    </row>
+    <row r="173" spans="6:15">
       <c r="F173" s="1"/>
       <c r="G173" s="1"/>
-      <c r="K173" s="1"/>
-      <c r="L173" s="107"/>
-      <c r="N173" s="1"/>
-    </row>
-    <row r="174" spans="5:14">
-      <c r="E174" s="1"/>
+      <c r="H173" s="1"/>
+      <c r="L173" s="1"/>
+      <c r="M173" s="107"/>
+      <c r="O173" s="1"/>
+    </row>
+    <row r="174" spans="6:15">
       <c r="F174" s="1"/>
       <c r="G174" s="1"/>
-      <c r="K174" s="1"/>
-      <c r="L174" s="41"/>
-      <c r="N174" s="1"/>
-    </row>
-    <row r="175" spans="5:14">
-      <c r="E175" s="1"/>
+      <c r="H174" s="1"/>
+      <c r="L174" s="1"/>
+      <c r="M174" s="41"/>
+      <c r="O174" s="1"/>
+    </row>
+    <row r="175" spans="6:15">
       <c r="F175" s="1"/>
       <c r="G175" s="1"/>
-      <c r="K175" s="1"/>
-      <c r="L175" s="41"/>
-      <c r="N175" s="1"/>
-    </row>
-    <row r="176" spans="5:14">
-      <c r="E176" s="1"/>
+      <c r="H175" s="1"/>
+      <c r="L175" s="1"/>
+      <c r="M175" s="41"/>
+      <c r="O175" s="1"/>
+    </row>
+    <row r="176" spans="6:15">
       <c r="F176" s="1"/>
       <c r="G176" s="1"/>
-      <c r="K176" s="1"/>
-      <c r="L176" s="41"/>
-      <c r="N176" s="1"/>
-    </row>
-    <row r="177" spans="4:14">
-      <c r="E177" s="1"/>
+      <c r="H176" s="1"/>
+      <c r="L176" s="1"/>
+      <c r="M176" s="41"/>
+      <c r="O176" s="1"/>
+    </row>
+    <row r="177" spans="4:15">
       <c r="F177" s="1"/>
       <c r="G177" s="1"/>
-      <c r="K177" s="1"/>
-      <c r="L177" s="41"/>
-      <c r="N177" s="1"/>
-    </row>
-    <row r="178" spans="4:14">
-      <c r="E178" s="1"/>
+      <c r="H177" s="1"/>
+      <c r="L177" s="1"/>
+      <c r="M177" s="41"/>
+      <c r="O177" s="1"/>
+    </row>
+    <row r="178" spans="4:15">
       <c r="F178" s="1"/>
       <c r="G178" s="1"/>
-      <c r="K178" s="1"/>
-      <c r="L178" s="41"/>
-      <c r="N178" s="1"/>
-    </row>
-    <row r="179" spans="4:14">
-      <c r="E179" s="1"/>
+      <c r="H178" s="1"/>
+      <c r="L178" s="1"/>
+      <c r="M178" s="41"/>
+      <c r="O178" s="1"/>
+    </row>
+    <row r="179" spans="4:15">
       <c r="F179" s="1"/>
       <c r="G179" s="1"/>
-      <c r="K179" s="1"/>
-      <c r="L179" s="41"/>
-      <c r="N179" s="1"/>
-    </row>
-    <row r="180" spans="4:14">
-      <c r="E180" s="1"/>
+      <c r="H179" s="1"/>
+      <c r="L179" s="1"/>
+      <c r="M179" s="41"/>
+      <c r="O179" s="1"/>
+    </row>
+    <row r="180" spans="4:15">
       <c r="F180" s="1"/>
       <c r="G180" s="1"/>
-      <c r="K180" s="1"/>
-      <c r="L180" s="41"/>
-      <c r="N180" s="1"/>
-    </row>
-    <row r="181" spans="4:14">
-      <c r="E181" s="1"/>
+      <c r="H180" s="1"/>
+      <c r="L180" s="1"/>
+      <c r="M180" s="41"/>
+      <c r="O180" s="1"/>
+    </row>
+    <row r="181" spans="4:15">
       <c r="F181" s="1"/>
       <c r="G181" s="1"/>
-      <c r="K181" s="1"/>
-      <c r="N181" s="1"/>
-    </row>
-    <row r="182" spans="4:14">
-      <c r="E182" s="1"/>
+      <c r="H181" s="1"/>
+      <c r="L181" s="1"/>
+      <c r="O181" s="1"/>
+    </row>
+    <row r="182" spans="4:15">
       <c r="F182" s="1"/>
       <c r="G182" s="1"/>
-      <c r="K182" s="1"/>
-      <c r="N182" s="1"/>
-    </row>
-    <row r="183" spans="4:14">
-      <c r="E183" s="1"/>
+      <c r="H182" s="1"/>
+      <c r="L182" s="1"/>
+      <c r="O182" s="1"/>
+    </row>
+    <row r="183" spans="4:15">
       <c r="F183" s="1"/>
       <c r="G183" s="1"/>
-      <c r="K183" s="1"/>
-      <c r="N183" s="1"/>
-    </row>
-    <row r="184" spans="4:14">
-      <c r="E184" s="1"/>
+      <c r="H183" s="1"/>
+      <c r="L183" s="1"/>
+      <c r="O183" s="1"/>
+    </row>
+    <row r="184" spans="4:15">
       <c r="F184" s="1"/>
       <c r="G184" s="1"/>
-      <c r="K184" s="1"/>
-      <c r="N184" s="1"/>
-    </row>
-    <row r="185" spans="4:14">
-      <c r="E185" s="1"/>
+      <c r="H184" s="1"/>
+      <c r="L184" s="1"/>
+      <c r="O184" s="1"/>
+    </row>
+    <row r="185" spans="4:15">
       <c r="F185" s="1"/>
       <c r="G185" s="1"/>
-      <c r="K185" s="1"/>
-      <c r="N185" s="1"/>
-    </row>
-    <row r="186" spans="4:14">
-      <c r="E186" s="1"/>
+      <c r="H185" s="1"/>
+      <c r="L185" s="1"/>
+      <c r="O185" s="1"/>
+    </row>
+    <row r="186" spans="4:15">
       <c r="F186" s="1"/>
       <c r="G186" s="1"/>
-      <c r="K186" s="1"/>
-      <c r="N186" s="1"/>
-    </row>
-    <row r="187" spans="4:14">
+      <c r="H186" s="1"/>
+      <c r="L186" s="1"/>
+      <c r="O186" s="1"/>
+    </row>
+    <row r="187" spans="4:15">
       <c r="D187" s="108"/>
-      <c r="E187" s="1"/>
+      <c r="E187" s="108"/>
       <c r="F187" s="1"/>
       <c r="G187" s="1"/>
-      <c r="K187" s="1"/>
-      <c r="N187" s="1"/>
-    </row>
-    <row r="188" spans="4:14">
+      <c r="H187" s="1"/>
+      <c r="L187" s="1"/>
+      <c r="O187" s="1"/>
+    </row>
+    <row r="188" spans="4:15">
       <c r="D188" s="108"/>
-      <c r="E188" s="1"/>
+      <c r="E188" s="108"/>
       <c r="F188" s="1"/>
       <c r="G188" s="1"/>
-      <c r="K188" s="1"/>
-      <c r="N188" s="1"/>
-    </row>
-    <row r="189" spans="4:14">
+      <c r="H188" s="1"/>
+      <c r="L188" s="1"/>
+      <c r="O188" s="1"/>
+    </row>
+    <row r="189" spans="4:15">
       <c r="D189" s="108"/>
-      <c r="E189" s="1"/>
+      <c r="E189" s="108"/>
       <c r="F189" s="1"/>
       <c r="G189" s="1"/>
-      <c r="K189" s="1"/>
-      <c r="N189" s="1"/>
-    </row>
-    <row r="190" spans="4:14">
+      <c r="H189" s="1"/>
+      <c r="L189" s="1"/>
+      <c r="O189" s="1"/>
+    </row>
+    <row r="190" spans="4:15">
       <c r="D190" s="108"/>
-      <c r="E190" s="1"/>
+      <c r="E190" s="108"/>
       <c r="F190" s="1"/>
       <c r="G190" s="1"/>
-      <c r="K190" s="1"/>
-      <c r="N190" s="1"/>
-    </row>
-    <row r="191" spans="4:14">
+      <c r="H190" s="1"/>
+      <c r="L190" s="1"/>
+      <c r="O190" s="1"/>
+    </row>
+    <row r="191" spans="4:15">
       <c r="D191" s="108"/>
-      <c r="E191" s="1"/>
+      <c r="E191" s="108"/>
       <c r="F191" s="1"/>
       <c r="G191" s="1"/>
-      <c r="K191" s="1"/>
-      <c r="N191" s="1"/>
-    </row>
-    <row r="192" spans="4:14">
+      <c r="H191" s="1"/>
+      <c r="L191" s="1"/>
+      <c r="O191" s="1"/>
+    </row>
+    <row r="192" spans="4:15">
       <c r="D192" s="108"/>
-      <c r="E192" s="1"/>
+      <c r="E192" s="108"/>
       <c r="F192" s="1"/>
       <c r="G192" s="1"/>
-      <c r="K192" s="1"/>
-      <c r="N192" s="1"/>
-    </row>
-    <row r="193" spans="3:14">
+      <c r="H192" s="1"/>
+      <c r="L192" s="1"/>
+      <c r="O192" s="1"/>
+    </row>
+    <row r="193" spans="3:15">
       <c r="D193" s="108"/>
-      <c r="E193" s="1"/>
+      <c r="E193" s="108"/>
       <c r="F193" s="1"/>
       <c r="G193" s="1"/>
-      <c r="K193" s="1"/>
-      <c r="N193" s="1"/>
-    </row>
-    <row r="194" spans="3:14">
+      <c r="H193" s="1"/>
+      <c r="L193" s="1"/>
+      <c r="O193" s="1"/>
+    </row>
+    <row r="194" spans="3:15">
       <c r="C194" s="36"/>
       <c r="D194" s="108"/>
-      <c r="E194" s="1"/>
+      <c r="E194" s="108"/>
       <c r="F194" s="1"/>
       <c r="G194" s="1"/>
-      <c r="K194" s="1"/>
-      <c r="L194" s="107"/>
-      <c r="N194" s="1"/>
-    </row>
-    <row r="195" spans="3:14">
-      <c r="E195" s="1"/>
+      <c r="H194" s="1"/>
+      <c r="L194" s="1"/>
+      <c r="M194" s="107"/>
+      <c r="O194" s="1"/>
+    </row>
+    <row r="195" spans="3:15">
       <c r="F195" s="1"/>
       <c r="G195" s="1"/>
-      <c r="K195" s="1"/>
-      <c r="L195" s="141"/>
-      <c r="N195" s="1"/>
-    </row>
-    <row r="196" spans="3:14">
-      <c r="E196" s="1"/>
+      <c r="H195" s="1"/>
+      <c r="L195" s="1"/>
+      <c r="M195" s="141"/>
+      <c r="O195" s="1"/>
+    </row>
+    <row r="196" spans="3:15">
       <c r="F196" s="1"/>
       <c r="G196" s="1"/>
-      <c r="K196" s="1"/>
-      <c r="N196" s="1"/>
-    </row>
-    <row r="197" spans="3:14">
-      <c r="E197" s="1"/>
+      <c r="H196" s="1"/>
+      <c r="L196" s="1"/>
+      <c r="O196" s="1"/>
+    </row>
+    <row r="197" spans="3:15">
       <c r="F197" s="1"/>
       <c r="G197" s="1"/>
-      <c r="H197" s="201"/>
-      <c r="K197" s="1"/>
-      <c r="N197" s="1"/>
-    </row>
-    <row r="198" spans="3:14">
-      <c r="E198" s="1"/>
+      <c r="H197" s="1"/>
+      <c r="I197" s="201"/>
+      <c r="L197" s="1"/>
+      <c r="O197" s="1"/>
+    </row>
+    <row r="198" spans="3:15">
       <c r="F198" s="1"/>
       <c r="G198" s="1"/>
-      <c r="K198" s="1"/>
-      <c r="N198" s="1"/>
-    </row>
-    <row r="199" spans="3:14">
-      <c r="E199" s="1"/>
+      <c r="H198" s="1"/>
+      <c r="L198" s="1"/>
+      <c r="O198" s="1"/>
+    </row>
+    <row r="199" spans="3:15">
       <c r="F199" s="1"/>
       <c r="G199" s="1"/>
-      <c r="K199" s="1"/>
-      <c r="N199" s="1"/>
-    </row>
-    <row r="200" spans="3:14">
-      <c r="E200" s="1"/>
+      <c r="H199" s="1"/>
+      <c r="L199" s="1"/>
+      <c r="O199" s="1"/>
+    </row>
+    <row r="200" spans="3:15">
       <c r="F200" s="1"/>
       <c r="G200" s="1"/>
-      <c r="K200" s="1"/>
-      <c r="N200" s="1"/>
-    </row>
-    <row r="201" spans="3:14">
-      <c r="E201" s="1"/>
+      <c r="H200" s="1"/>
+      <c r="L200" s="1"/>
+      <c r="O200" s="1"/>
+    </row>
+    <row r="201" spans="3:15">
       <c r="F201" s="1"/>
       <c r="G201" s="1"/>
-      <c r="K201" s="1"/>
-      <c r="N201" s="1"/>
-    </row>
-    <row r="202" spans="3:14">
-      <c r="E202" s="1"/>
+      <c r="H201" s="1"/>
+      <c r="L201" s="1"/>
+      <c r="O201" s="1"/>
+    </row>
+    <row r="202" spans="3:15">
       <c r="F202" s="1"/>
       <c r="G202" s="1"/>
-      <c r="K202" s="1"/>
-      <c r="N202" s="1"/>
-    </row>
-    <row r="203" spans="3:14">
-      <c r="E203" s="1"/>
+      <c r="H202" s="1"/>
+      <c r="L202" s="1"/>
+      <c r="O202" s="1"/>
+    </row>
+    <row r="203" spans="3:15">
       <c r="F203" s="1"/>
       <c r="G203" s="1"/>
-      <c r="K203" s="1"/>
-      <c r="N203" s="1"/>
-    </row>
-    <row r="204" spans="3:14">
-      <c r="E204" s="1"/>
+      <c r="H203" s="1"/>
+      <c r="L203" s="1"/>
+      <c r="O203" s="1"/>
+    </row>
+    <row r="204" spans="3:15">
       <c r="F204" s="1"/>
       <c r="G204" s="1"/>
-      <c r="K204" s="1"/>
-      <c r="L204" s="107"/>
-      <c r="N204" s="1"/>
-    </row>
-    <row r="205" spans="3:14">
+      <c r="H204" s="1"/>
+      <c r="L204" s="1"/>
+      <c r="M204" s="107"/>
+      <c r="O204" s="1"/>
+    </row>
+    <row r="205" spans="3:15">
       <c r="C205" s="36"/>
-      <c r="E205" s="1"/>
       <c r="F205" s="1"/>
       <c r="G205" s="1"/>
-      <c r="K205" s="1"/>
-      <c r="L205" s="107"/>
-      <c r="N205" s="1"/>
-    </row>
-    <row r="206" spans="3:14">
+      <c r="H205" s="1"/>
+      <c r="L205" s="1"/>
+      <c r="M205" s="107"/>
+      <c r="O205" s="1"/>
+    </row>
+    <row r="206" spans="3:15">
       <c r="C206" s="36"/>
-      <c r="E206" s="1"/>
       <c r="F206" s="1"/>
       <c r="G206" s="1"/>
-      <c r="I206" s="36"/>
+      <c r="H206" s="1"/>
       <c r="J206" s="36"/>
-      <c r="K206" s="1"/>
-      <c r="L206" s="107"/>
-      <c r="N206" s="1"/>
-    </row>
-    <row r="207" spans="3:14">
+      <c r="K206" s="36"/>
+      <c r="L206" s="1"/>
+      <c r="M206" s="107"/>
+      <c r="O206" s="1"/>
+    </row>
+    <row r="207" spans="3:15">
       <c r="C207" s="36"/>
-      <c r="E207" s="1"/>
       <c r="F207" s="1"/>
       <c r="G207" s="1"/>
-      <c r="K207" s="1"/>
-      <c r="L207" s="107"/>
-      <c r="N207" s="1"/>
-    </row>
-    <row r="208" spans="3:14">
+      <c r="H207" s="1"/>
+      <c r="L207" s="1"/>
+      <c r="M207" s="107"/>
+      <c r="O207" s="1"/>
+    </row>
+    <row r="208" spans="3:15">
       <c r="C208" s="36"/>
-      <c r="E208" s="1"/>
       <c r="F208" s="1"/>
       <c r="G208" s="1"/>
-      <c r="K208" s="1"/>
-      <c r="L208" s="107"/>
-      <c r="N208" s="1"/>
-    </row>
-    <row r="209" spans="2:14">
+      <c r="H208" s="1"/>
+      <c r="L208" s="1"/>
+      <c r="M208" s="107"/>
+      <c r="O208" s="1"/>
+    </row>
+    <row r="209" spans="2:15">
       <c r="C209" s="36"/>
-      <c r="E209" s="1"/>
       <c r="F209" s="1"/>
       <c r="G209" s="1"/>
-      <c r="K209" s="1"/>
-      <c r="L209" s="107"/>
-      <c r="N209" s="1"/>
-    </row>
-    <row r="210" spans="2:14">
+      <c r="H209" s="1"/>
+      <c r="L209" s="1"/>
+      <c r="M209" s="107"/>
+      <c r="O209" s="1"/>
+    </row>
+    <row r="210" spans="2:15">
       <c r="C210" s="36"/>
-      <c r="E210" s="1"/>
       <c r="F210" s="1"/>
       <c r="G210" s="1"/>
-      <c r="I210" s="36"/>
+      <c r="H210" s="1"/>
       <c r="J210" s="36"/>
-      <c r="K210" s="1"/>
-      <c r="L210" s="107"/>
-      <c r="N210" s="1"/>
-    </row>
-    <row r="211" spans="2:14">
+      <c r="K210" s="36"/>
+      <c r="L210" s="1"/>
+      <c r="M210" s="107"/>
+      <c r="O210" s="1"/>
+    </row>
+    <row r="211" spans="2:15">
       <c r="C211" s="36"/>
-      <c r="E211" s="1"/>
       <c r="F211" s="1"/>
       <c r="G211" s="1"/>
-      <c r="I211" s="36"/>
+      <c r="H211" s="1"/>
       <c r="J211" s="36"/>
-      <c r="K211" s="1"/>
-      <c r="L211" s="107"/>
-      <c r="N211" s="1"/>
-    </row>
-    <row r="212" spans="2:14">
-      <c r="E212" s="1"/>
+      <c r="K211" s="36"/>
+      <c r="L211" s="1"/>
+      <c r="M211" s="107"/>
+      <c r="O211" s="1"/>
+    </row>
+    <row r="212" spans="2:15">
       <c r="F212" s="1"/>
       <c r="G212" s="1"/>
-      <c r="K212" s="1"/>
-      <c r="N212" s="1"/>
-    </row>
-    <row r="213" spans="2:14">
+      <c r="H212" s="1"/>
+      <c r="L212" s="1"/>
+      <c r="O212" s="1"/>
+    </row>
+    <row r="213" spans="2:15">
       <c r="C213" s="36"/>
       <c r="D213" s="108"/>
-      <c r="E213" s="1"/>
+      <c r="E213" s="108"/>
       <c r="F213" s="1"/>
       <c r="G213" s="1"/>
-      <c r="K213" s="1"/>
-      <c r="N213" s="1"/>
-    </row>
-    <row r="214" spans="2:14">
+      <c r="H213" s="1"/>
+      <c r="L213" s="1"/>
+      <c r="O213" s="1"/>
+    </row>
+    <row r="214" spans="2:15">
       <c r="D214" s="108"/>
-      <c r="E214" s="1"/>
+      <c r="E214" s="108"/>
       <c r="F214" s="1"/>
       <c r="G214" s="1"/>
-      <c r="K214" s="1"/>
-      <c r="N214" s="1"/>
-    </row>
-    <row r="215" spans="2:14">
+      <c r="H214" s="1"/>
+      <c r="L214" s="1"/>
+      <c r="O214" s="1"/>
+    </row>
+    <row r="215" spans="2:15">
       <c r="D215" s="108"/>
-      <c r="E215" s="1"/>
+      <c r="E215" s="108"/>
       <c r="F215" s="1"/>
       <c r="G215" s="1"/>
-      <c r="K215" s="1"/>
-      <c r="N215" s="1"/>
-    </row>
-    <row r="216" spans="2:14">
+      <c r="H215" s="1"/>
+      <c r="L215" s="1"/>
+      <c r="O215" s="1"/>
+    </row>
+    <row r="216" spans="2:15">
       <c r="D216" s="108"/>
-      <c r="E216" s="1"/>
+      <c r="E216" s="108"/>
       <c r="F216" s="1"/>
       <c r="G216" s="1"/>
-      <c r="K216" s="1"/>
-      <c r="N216" s="1"/>
-    </row>
-    <row r="217" spans="2:14">
+      <c r="H216" s="1"/>
+      <c r="L216" s="1"/>
+      <c r="O216" s="1"/>
+    </row>
+    <row r="217" spans="2:15">
       <c r="D217" s="108"/>
-      <c r="E217" s="1"/>
+      <c r="E217" s="108"/>
       <c r="F217" s="1"/>
       <c r="G217" s="1"/>
-      <c r="K217" s="1"/>
-      <c r="N217" s="1"/>
-    </row>
-    <row r="218" spans="2:14">
+      <c r="H217" s="1"/>
+      <c r="L217" s="1"/>
+      <c r="O217" s="1"/>
+    </row>
+    <row r="218" spans="2:15">
       <c r="D218" s="108"/>
-      <c r="E218" s="1"/>
+      <c r="E218" s="108"/>
       <c r="F218" s="1"/>
       <c r="G218" s="1"/>
-      <c r="K218" s="1"/>
-      <c r="L218" s="107"/>
-      <c r="N218" s="1"/>
-    </row>
-    <row r="219" spans="2:14">
+      <c r="H218" s="1"/>
+      <c r="L218" s="1"/>
+      <c r="M218" s="107"/>
+      <c r="O218" s="1"/>
+    </row>
+    <row r="219" spans="2:15">
       <c r="D219" s="108"/>
-      <c r="E219" s="1"/>
+      <c r="E219" s="108"/>
       <c r="F219" s="1"/>
       <c r="G219" s="1"/>
-      <c r="K219" s="1"/>
-      <c r="N219" s="1"/>
-    </row>
-    <row r="220" spans="2:14">
+      <c r="H219" s="1"/>
+      <c r="L219" s="1"/>
+      <c r="O219" s="1"/>
+    </row>
+    <row r="220" spans="2:15">
       <c r="D220" s="108"/>
-      <c r="E220" s="1"/>
+      <c r="E220" s="108"/>
       <c r="F220" s="1"/>
       <c r="G220" s="1"/>
-      <c r="K220" s="1"/>
-      <c r="L220" s="107"/>
-      <c r="N220" s="1"/>
-    </row>
-    <row r="221" spans="2:14">
+      <c r="H220" s="1"/>
+      <c r="L220" s="1"/>
+      <c r="M220" s="107"/>
+      <c r="O220" s="1"/>
+    </row>
+    <row r="221" spans="2:15">
       <c r="B221" s="36"/>
       <c r="C221" s="36"/>
-      <c r="E221" s="1"/>
       <c r="F221" s="1"/>
       <c r="G221" s="1"/>
-      <c r="K221" s="1"/>
-      <c r="N221" s="1"/>
-    </row>
-    <row r="222" spans="2:14">
+      <c r="H221" s="1"/>
+      <c r="L221" s="1"/>
+      <c r="O221" s="1"/>
+    </row>
+    <row r="222" spans="2:15">
       <c r="B222" s="36"/>
       <c r="C222" s="36"/>
-      <c r="E222" s="1"/>
       <c r="F222" s="1"/>
       <c r="G222" s="1"/>
-      <c r="K222" s="1"/>
-      <c r="N222" s="1"/>
-    </row>
-    <row r="223" spans="2:14">
-      <c r="E223" s="1"/>
+      <c r="H222" s="1"/>
+      <c r="L222" s="1"/>
+      <c r="O222" s="1"/>
+    </row>
+    <row r="223" spans="2:15">
       <c r="F223" s="1"/>
       <c r="G223" s="1"/>
-      <c r="K223" s="1"/>
-      <c r="N223" s="1"/>
-    </row>
-    <row r="224" spans="2:14">
-      <c r="E224" s="1"/>
+      <c r="H223" s="1"/>
+      <c r="L223" s="1"/>
+      <c r="O223" s="1"/>
+    </row>
+    <row r="224" spans="2:15">
       <c r="F224" s="1"/>
       <c r="G224" s="1"/>
-      <c r="K224" s="1"/>
-      <c r="L224" s="107"/>
-      <c r="N224" s="1"/>
-    </row>
-    <row r="225" spans="3:14">
-      <c r="E225" s="1"/>
+      <c r="H224" s="1"/>
+      <c r="L224" s="1"/>
+      <c r="M224" s="107"/>
+      <c r="O224" s="1"/>
+    </row>
+    <row r="225" spans="3:15">
       <c r="F225" s="1"/>
       <c r="G225" s="1"/>
-      <c r="K225" s="1"/>
-      <c r="N225" s="1"/>
-    </row>
-    <row r="226" spans="3:14">
-      <c r="E226" s="1"/>
+      <c r="H225" s="1"/>
+      <c r="L225" s="1"/>
+      <c r="O225" s="1"/>
+    </row>
+    <row r="226" spans="3:15">
       <c r="F226" s="1"/>
       <c r="G226" s="1"/>
-      <c r="K226" s="1"/>
-      <c r="N226" s="1"/>
-    </row>
-    <row r="227" spans="3:14">
-      <c r="E227" s="1"/>
+      <c r="H226" s="1"/>
+      <c r="L226" s="1"/>
+      <c r="O226" s="1"/>
+    </row>
+    <row r="227" spans="3:15">
       <c r="F227" s="1"/>
       <c r="G227" s="1"/>
-      <c r="K227" s="1"/>
-      <c r="N227" s="1"/>
-    </row>
-    <row r="228" spans="3:14">
-      <c r="E228" s="1"/>
+      <c r="H227" s="1"/>
+      <c r="L227" s="1"/>
+      <c r="O227" s="1"/>
+    </row>
+    <row r="228" spans="3:15">
       <c r="F228" s="1"/>
       <c r="G228" s="1"/>
-      <c r="K228" s="1"/>
-      <c r="N228" s="1"/>
-    </row>
-    <row r="229" spans="3:14">
-      <c r="E229" s="1"/>
+      <c r="H228" s="1"/>
+      <c r="L228" s="1"/>
+      <c r="O228" s="1"/>
+    </row>
+    <row r="229" spans="3:15">
       <c r="F229" s="1"/>
       <c r="G229" s="1"/>
-      <c r="K229" s="1"/>
-      <c r="N229" s="1"/>
-    </row>
-    <row r="230" spans="3:14">
-      <c r="E230" s="1"/>
+      <c r="H229" s="1"/>
+      <c r="L229" s="1"/>
+      <c r="O229" s="1"/>
+    </row>
+    <row r="230" spans="3:15">
       <c r="F230" s="1"/>
       <c r="G230" s="1"/>
-      <c r="K230" s="1"/>
-      <c r="N230" s="1"/>
-    </row>
-    <row r="231" spans="3:14">
-      <c r="E231" s="1"/>
+      <c r="H230" s="1"/>
+      <c r="L230" s="1"/>
+      <c r="O230" s="1"/>
+    </row>
+    <row r="231" spans="3:15">
       <c r="F231" s="1"/>
       <c r="G231" s="1"/>
-      <c r="K231" s="1"/>
-      <c r="N231" s="1"/>
-    </row>
-    <row r="232" spans="3:14">
-      <c r="E232" s="1"/>
+      <c r="H231" s="1"/>
+      <c r="L231" s="1"/>
+      <c r="O231" s="1"/>
+    </row>
+    <row r="232" spans="3:15">
       <c r="F232" s="1"/>
       <c r="G232" s="1"/>
-      <c r="H232" s="36"/>
+      <c r="H232" s="1"/>
       <c r="I232" s="36"/>
       <c r="J232" s="36"/>
-      <c r="K232" s="1"/>
-      <c r="N232" s="1"/>
-    </row>
-    <row r="233" spans="3:14">
-      <c r="E233" s="1"/>
+      <c r="K232" s="36"/>
+      <c r="L232" s="1"/>
+      <c r="O232" s="1"/>
+    </row>
+    <row r="233" spans="3:15">
       <c r="F233" s="1"/>
       <c r="G233" s="1"/>
-      <c r="H233" s="36"/>
+      <c r="H233" s="1"/>
       <c r="I233" s="36"/>
       <c r="J233" s="36"/>
-      <c r="K233" s="1"/>
-      <c r="N233" s="1"/>
-    </row>
-    <row r="234" spans="3:14">
-      <c r="E234" s="1"/>
+      <c r="K233" s="36"/>
+      <c r="L233" s="1"/>
+      <c r="O233" s="1"/>
+    </row>
+    <row r="234" spans="3:15">
       <c r="F234" s="1"/>
       <c r="G234" s="1"/>
-      <c r="H234" s="36"/>
+      <c r="H234" s="1"/>
       <c r="I234" s="36"/>
       <c r="J234" s="36"/>
-      <c r="K234" s="1"/>
-      <c r="N234" s="1"/>
-    </row>
-    <row r="235" spans="3:14">
-      <c r="E235" s="1"/>
+      <c r="K234" s="36"/>
+      <c r="L234" s="1"/>
+      <c r="O234" s="1"/>
+    </row>
+    <row r="235" spans="3:15">
       <c r="F235" s="1"/>
       <c r="G235" s="1"/>
-      <c r="H235" s="36"/>
+      <c r="H235" s="1"/>
       <c r="I235" s="36"/>
       <c r="J235" s="36"/>
-      <c r="K235" s="1"/>
-      <c r="N235" s="1"/>
-    </row>
-    <row r="236" spans="3:14">
+      <c r="K235" s="36"/>
+      <c r="L235" s="1"/>
+      <c r="O235" s="1"/>
+    </row>
+    <row r="236" spans="3:15">
       <c r="C236" s="36"/>
-      <c r="E236" s="1"/>
       <c r="F236" s="1"/>
       <c r="G236" s="1"/>
-      <c r="H236" s="36"/>
+      <c r="H236" s="1"/>
       <c r="I236" s="36"/>
       <c r="J236" s="36"/>
-      <c r="K236" s="1"/>
-      <c r="N236" s="1"/>
-    </row>
-    <row r="237" spans="3:14">
+      <c r="K236" s="36"/>
+      <c r="L236" s="1"/>
+      <c r="O236" s="1"/>
+    </row>
+    <row r="237" spans="3:15">
       <c r="C237" s="36"/>
-      <c r="E237" s="1"/>
       <c r="F237" s="1"/>
       <c r="G237" s="1"/>
-      <c r="H237" s="36"/>
+      <c r="H237" s="1"/>
       <c r="I237" s="36"/>
       <c r="J237" s="36"/>
-      <c r="K237" s="1"/>
-      <c r="N237" s="1"/>
-    </row>
-    <row r="238" spans="3:14">
+      <c r="K237" s="36"/>
+      <c r="L237" s="1"/>
+      <c r="O237" s="1"/>
+    </row>
+    <row r="238" spans="3:15">
       <c r="C238" s="36"/>
-      <c r="E238" s="1"/>
       <c r="F238" s="1"/>
       <c r="G238" s="1"/>
-      <c r="H238" s="36"/>
+      <c r="H238" s="1"/>
       <c r="I238" s="36"/>
       <c r="J238" s="36"/>
-      <c r="K238" s="1"/>
-      <c r="N238" s="1"/>
-    </row>
-    <row r="239" spans="3:14">
+      <c r="K238" s="36"/>
+      <c r="L238" s="1"/>
+      <c r="O238" s="1"/>
+    </row>
+    <row r="239" spans="3:15">
       <c r="C239" s="36"/>
-      <c r="E239" s="1"/>
       <c r="F239" s="1"/>
       <c r="G239" s="1"/>
-      <c r="H239" s="36"/>
+      <c r="H239" s="1"/>
       <c r="I239" s="36"/>
       <c r="J239" s="36"/>
-      <c r="K239" s="1"/>
-      <c r="N239" s="1"/>
-    </row>
-    <row r="240" spans="3:14">
-      <c r="E240" s="1"/>
+      <c r="K239" s="36"/>
+      <c r="L239" s="1"/>
+      <c r="O239" s="1"/>
+    </row>
+    <row r="240" spans="3:15">
       <c r="F240" s="1"/>
       <c r="G240" s="1"/>
-      <c r="K240" s="1"/>
-      <c r="L240" s="107"/>
-      <c r="N240" s="1"/>
+      <c r="H240" s="1"/>
+      <c r="L240" s="1"/>
+      <c r="M240" s="107"/>
+      <c r="O240" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:P231" xr:uid="{93D30021-67EF-EE48-BE7B-4A9D77B3B997}"/>
+  <autoFilter ref="A3:Q231" xr:uid="{93D30021-67EF-EE48-BE7B-4A9D77B3B997}"/>
   <phoneticPr fontId="49" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Implement Searchable column in template
Signed-off-by: Harpreet Jhita <harpreet.jhita@justice.gov.uk>
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\fergusoshea\et-ccd-definitions-scotland\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harpreet.jhita/Projects/et-ccd-definitions-scotland/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AB373C-FADA-40DE-80E8-9D866EFAA00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912F4E59-2B5D-5B4B-A4A5-8E0EFDDD2D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20625" tabRatio="500" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20620" tabRatio="500" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchParty" sheetId="36" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="390">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1321,6 +1321,12 @@
   </si>
   <si>
     <t>Publish</t>
+  </si>
+  <si>
+    <t>Seachable</t>
+  </si>
+  <si>
+    <t>Searchable</t>
   </si>
 </sst>
 </file>
@@ -2863,9 +2869,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2903,7 +2909,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3009,7 +3015,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3151,7 +3157,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3165,11 +3171,11 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" style="291" customWidth="1"/>
-    <col min="3" max="1025" width="11.140625" style="287" customWidth="1"/>
-    <col min="1026" max="16384" width="8.85546875" style="287"/>
+    <col min="1" max="2" width="10.6640625" style="291" customWidth="1"/>
+    <col min="3" max="1025" width="11.1640625" style="287" customWidth="1"/>
+    <col min="1026" max="16384" width="8.83203125" style="287"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18">
@@ -3186,7 +3192,7 @@
       <c r="I1" s="299"/>
       <c r="J1" s="298"/>
     </row>
-    <row r="2" spans="1:10" ht="409.5">
+    <row r="2" spans="1:10" ht="409.6">
       <c r="A2" s="296" t="s">
         <v>353</v>
       </c>
@@ -3260,26 +3266,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:U206"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="33.42578125" customWidth="1"/>
-    <col min="12" max="17" width="8.42578125" customWidth="1"/>
-    <col min="18" max="21" width="6.28515625" customWidth="1"/>
-    <col min="22" max="1023" width="8.28515625" customWidth="1"/>
+    <col min="10" max="10" width="26.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="33.5" customWidth="1"/>
+    <col min="12" max="17" width="8.5" customWidth="1"/>
+    <col min="18" max="21" width="6.33203125" customWidth="1"/>
+    <col min="22" max="1023" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18">
@@ -3389,7 +3395,9 @@
       <c r="K3" s="27" t="s">
         <v>378</v>
       </c>
-      <c r="L3" s="51"/>
+      <c r="L3" s="51" t="s">
+        <v>389</v>
+      </c>
       <c r="M3" s="51"/>
       <c r="N3" s="51"/>
       <c r="O3" s="51"/>
@@ -4475,7 +4483,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:5" ht="18">
       <c r="A1" s="35" t="s">
@@ -4487,7 +4495,7 @@
       <c r="D1" s="36"/>
       <c r="E1" s="36"/>
     </row>
-    <row r="2" spans="1:5" ht="63.75">
+    <row r="2" spans="1:5" ht="70">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
@@ -4504,7 +4512,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="25.5">
+    <row r="3" spans="1:5" ht="14">
       <c r="A3" s="303" t="s">
         <v>32</v>
       </c>
@@ -4534,20 +4542,20 @@
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" style="246" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="246"/>
-    <col min="3" max="3" width="54.7109375" style="246" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="246" customWidth="1"/>
-    <col min="5" max="6" width="12.7109375" style="246" customWidth="1"/>
-    <col min="7" max="7" width="44.28515625" style="246" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="246" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" style="246" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="246"/>
+    <col min="3" max="3" width="54.6640625" style="246" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="246" customWidth="1"/>
+    <col min="5" max="6" width="12.6640625" style="246" customWidth="1"/>
+    <col min="7" max="7" width="44.33203125" style="246" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" style="246" customWidth="1"/>
     <col min="9" max="9" width="37" style="246" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" style="246" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" style="246" customWidth="1"/>
-    <col min="12" max="1025" width="10.85546875" style="246"/>
-    <col min="1026" max="16384" width="10.85546875" style="245"/>
+    <col min="10" max="10" width="43.6640625" style="246" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" style="246" customWidth="1"/>
+    <col min="12" max="1025" width="10.83203125" style="246"/>
+    <col min="1026" max="16384" width="10.83203125" style="245"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18">
@@ -4573,7 +4581,7 @@
       <c r="L1" s="247"/>
       <c r="M1" s="247"/>
     </row>
-    <row r="2" spans="1:13" ht="63.75">
+    <row r="2" spans="1:13" ht="56">
       <c r="A2" s="258" t="s">
         <v>4</v>
       </c>
@@ -4608,7 +4616,7 @@
       <c r="L2" s="254"/>
       <c r="M2" s="254"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75">
+    <row r="3" spans="1:13" ht="16">
       <c r="A3" s="253" t="s">
         <v>9</v>
       </c>
@@ -4729,30 +4737,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:W649"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="31.5" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" style="52" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" style="41" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="41" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="52" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" style="41" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="41" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="53" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="53" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" customWidth="1"/>
-    <col min="14" max="14" width="33.5703125" customWidth="1"/>
-    <col min="15" max="15" width="28.28515625" customWidth="1"/>
-    <col min="16" max="23" width="6.28515625" customWidth="1"/>
-    <col min="24" max="1023" width="8.28515625" customWidth="1"/>
-    <col min="1024" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" style="53" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" style="53" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" customWidth="1"/>
+    <col min="14" max="14" width="33.5" customWidth="1"/>
+    <col min="15" max="15" width="28.33203125" customWidth="1"/>
+    <col min="16" max="23" width="6.33203125" customWidth="1"/>
+    <col min="24" max="1023" width="8.33203125" customWidth="1"/>
+    <col min="1024" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="18" customHeight="1">
@@ -4780,7 +4788,7 @@
       <c r="P1" s="36"/>
       <c r="Q1" s="36"/>
     </row>
-    <row r="2" spans="1:23" ht="65.099999999999994" customHeight="1">
+    <row r="2" spans="1:23" ht="65" customHeight="1">
       <c r="A2" s="25" t="s">
         <v>113</v>
       </c>
@@ -4823,7 +4831,7 @@
       <c r="P2" s="10"/>
       <c r="Q2" s="10"/>
     </row>
-    <row r="3" spans="1:23" s="2" customFormat="1" ht="33.6" customHeight="1">
+    <row r="3" spans="1:23" s="2" customFormat="1" ht="33.5" customHeight="1">
       <c r="A3" s="27" t="s">
         <v>11</v>
       </c>
@@ -4866,7 +4874,9 @@
       <c r="N3" s="27" t="s">
         <v>378</v>
       </c>
-      <c r="O3" s="51"/>
+      <c r="O3" s="51" t="s">
+        <v>388</v>
+      </c>
       <c r="P3" s="51"/>
       <c r="Q3" s="51"/>
       <c r="R3" s="51"/>
@@ -6968,7 +6978,7 @@
       <c r="I278"/>
       <c r="J278"/>
     </row>
-    <row r="279" spans="1:10" ht="13.5">
+    <row r="279" spans="1:10">
       <c r="B279" s="231"/>
       <c r="E279"/>
       <c r="F279" s="108"/>
@@ -8507,7 +8517,7 @@
       <c r="G488" s="219"/>
       <c r="H488" s="193"/>
     </row>
-    <row r="489" spans="1:8" ht="13.5">
+    <row r="489" spans="1:8">
       <c r="A489" s="56"/>
       <c r="B489" s="231"/>
       <c r="C489" s="56"/>
@@ -8517,7 +8527,7 @@
       <c r="G489" s="219"/>
       <c r="H489" s="193"/>
     </row>
-    <row r="490" spans="1:8" ht="13.5">
+    <row r="490" spans="1:8">
       <c r="A490" s="56"/>
       <c r="B490" s="231"/>
       <c r="C490" s="56"/>
@@ -8527,7 +8537,7 @@
       <c r="G490" s="219"/>
       <c r="H490" s="193"/>
     </row>
-    <row r="491" spans="1:8" ht="13.5">
+    <row r="491" spans="1:8">
       <c r="A491" s="56"/>
       <c r="B491" s="231"/>
       <c r="C491" s="56"/>
@@ -9357,21 +9367,21 @@
       <selection pane="bottomLeft" activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.42578125" customWidth="1"/>
-    <col min="6" max="6" width="50.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.5" customWidth="1"/>
+    <col min="6" max="6" width="50.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="39.950000000000003" customHeight="1">
+    <row r="1" spans="1:12" ht="40" customHeight="1">
       <c r="A1" s="282" t="s">
         <v>120</v>
       </c>
@@ -9390,7 +9400,7 @@
       <c r="H1" s="278"/>
       <c r="I1" s="277"/>
     </row>
-    <row r="2" spans="1:12" ht="66.95" customHeight="1">
+    <row r="2" spans="1:12" ht="67" customHeight="1">
       <c r="A2" s="275" t="s">
         <v>121</v>
       </c>
@@ -15585,13 +15595,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18">
@@ -15605,7 +15615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="165.75">
+    <row r="2" spans="1:5" ht="154">
       <c r="A2" s="300" t="s">
         <v>4</v>
       </c>
@@ -16386,22 +16396,22 @@
   </sheetPr>
   <dimension ref="A1:K650"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD650"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" style="151" customWidth="1"/>
-    <col min="2" max="2" width="61.7109375" style="171" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" style="151" customWidth="1"/>
+    <col min="2" max="2" width="61.6640625" style="171" customWidth="1"/>
     <col min="3" max="3" width="65" style="151" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="151" customWidth="1"/>
-    <col min="5" max="6" width="8.7109375" style="151"/>
+    <col min="4" max="4" width="14.6640625" style="151" customWidth="1"/>
+    <col min="5" max="6" width="8.6640625" style="151"/>
     <col min="7" max="7" width="13" style="151" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="151" customWidth="1"/>
-    <col min="9" max="12" width="8.7109375" style="151"/>
-    <col min="13" max="13" width="16.28515625" style="151" customWidth="1"/>
-    <col min="14" max="16384" width="8.7109375" style="151"/>
+    <col min="8" max="8" width="11.5" style="151" customWidth="1"/>
+    <col min="9" max="12" width="8.6640625" style="151"/>
+    <col min="13" max="13" width="16.33203125" style="151" customWidth="1"/>
+    <col min="14" max="16384" width="8.6640625" style="151"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18">
@@ -16418,7 +16428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="51">
+    <row r="2" spans="1:11" ht="56">
       <c r="A2" s="152" t="s">
         <v>129</v>
       </c>
@@ -19283,22 +19293,22 @@
       <selection activeCell="A4" sqref="A4:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="32.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" customWidth="1"/>
-    <col min="7" max="7" width="43.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" customWidth="1"/>
-    <col min="9" max="9" width="31.42578125" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" customWidth="1"/>
-    <col min="12" max="1025" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="32.5" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="43.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" customWidth="1"/>
+    <col min="9" max="9" width="31.5" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" customWidth="1"/>
+    <col min="12" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="36">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="19">
       <c r="A1" s="69" t="s">
         <v>134</v>
       </c>
@@ -19316,7 +19326,7 @@
       <c r="G1" s="73"/>
       <c r="H1" s="186"/>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="75">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="71">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
@@ -19546,20 +19556,20 @@
       <selection activeCell="A4" sqref="A4:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" customWidth="1"/>
-    <col min="9" max="1023" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.5" customWidth="1"/>
+    <col min="9" max="1023" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75">
+    <row r="1" spans="1:8" ht="19">
       <c r="A1" s="80" t="s">
         <v>142</v>
       </c>
@@ -19574,7 +19584,7 @@
       </c>
       <c r="E1" s="84"/>
     </row>
-    <row r="2" spans="1:8" ht="89.25">
+    <row r="2" spans="1:8" ht="84">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
@@ -19634,7 +19644,7 @@
       <c r="E5" s="1"/>
       <c r="G5" s="68"/>
     </row>
-    <row r="6" spans="1:8" ht="14.25">
+    <row r="6" spans="1:8" ht="14">
       <c r="D6" s="112"/>
       <c r="E6" s="1"/>
     </row>
@@ -19643,7 +19653,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="187"/>
     </row>
-    <row r="8" spans="1:8" ht="14.25">
+    <row r="8" spans="1:8" ht="14">
       <c r="B8" s="108"/>
       <c r="D8" s="112"/>
       <c r="E8" s="1"/>
@@ -19678,19 +19688,19 @@
       <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.5" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1"/>
-    <col min="8" max="1023" width="11.42578125"/>
+    <col min="6" max="6" width="28.33203125" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" customWidth="1"/>
+    <col min="8" max="1023" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36">
+    <row r="1" spans="1:15" ht="19">
       <c r="A1" s="69" t="s">
         <v>138</v>
       </c>
@@ -19710,7 +19720,7 @@
       <c r="I1" s="39"/>
       <c r="J1" s="39"/>
     </row>
-    <row r="2" spans="1:15" ht="90">
+    <row r="2" spans="1:15" ht="80">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
@@ -19816,11 +19826,11 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" style="291" customWidth="1"/>
-    <col min="3" max="1025" width="11.140625" style="287" customWidth="1"/>
-    <col min="1026" max="16384" width="8.85546875" style="287"/>
+    <col min="1" max="2" width="10.6640625" style="291" customWidth="1"/>
+    <col min="3" max="1025" width="11.1640625" style="287" customWidth="1"/>
+    <col min="1026" max="16384" width="8.83203125" style="287"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -19831,7 +19841,7 @@
       <c r="C1" s="285"/>
       <c r="D1" s="286"/>
     </row>
-    <row r="2" spans="1:4" ht="102.75">
+    <row r="2" spans="1:4" ht="99">
       <c r="A2" s="288" t="s">
         <v>353</v>
       </c>
@@ -19876,17 +19886,17 @@
       <selection activeCell="A4" sqref="A4:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" style="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="50" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" customWidth="1"/>
-    <col min="8" max="14" width="6.28515625" customWidth="1"/>
-    <col min="15" max="1023" width="8.28515625" customWidth="1"/>
+    <col min="7" max="7" width="25.5" customWidth="1"/>
+    <col min="8" max="14" width="6.33203125" customWidth="1"/>
+    <col min="15" max="1023" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18">
@@ -19908,7 +19918,7 @@
       <c r="H1" s="36"/>
       <c r="I1" s="36"/>
     </row>
-    <row r="2" spans="1:14" ht="105">
+    <row r="2" spans="1:14" ht="96">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
@@ -20013,18 +20023,18 @@
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="133" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="133" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" style="133" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="133" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="133" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="133" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" style="133" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="133" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="133" customWidth="1"/>
-    <col min="10" max="16384" width="10.7109375" style="133"/>
+    <col min="1" max="1" width="13.33203125" style="133" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="133" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="133" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="133" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="133" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="133" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" style="133" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="133" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="133" customWidth="1"/>
+    <col min="10" max="16384" width="10.6640625" style="133"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18">
@@ -20046,7 +20056,7 @@
       <c r="H1" s="132"/>
       <c r="I1" s="132"/>
     </row>
-    <row r="2" spans="1:9" ht="38.25">
+    <row r="2" spans="1:9" ht="42">
       <c r="A2" s="134"/>
       <c r="B2" s="134"/>
       <c r="C2" s="135" t="s">
@@ -20176,14 +20186,14 @@
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="2" width="11.42578125"/>
-    <col min="3" max="3" width="35.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="1" max="2" width="11.5"/>
+    <col min="3" max="3" width="35.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="1025" width="11.42578125"/>
+    <col min="7" max="1025" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18">
@@ -20207,7 +20217,7 @@
       <c r="J1" s="36"/>
       <c r="K1" s="36"/>
     </row>
-    <row r="2" spans="1:11" ht="63.75">
+    <row r="2" spans="1:11" ht="70">
       <c r="A2" s="23" t="s">
         <v>4</v>
       </c>
@@ -20230,7 +20240,7 @@
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
     </row>
-    <row r="3" spans="1:11" ht="38.25">
+    <row r="3" spans="1:11" ht="28">
       <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
@@ -20273,15 +20283,15 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="50.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="45.7109375" customWidth="1"/>
-    <col min="7" max="1025" width="8.28515625" customWidth="1"/>
+    <col min="4" max="4" width="50.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="45.6640625" customWidth="1"/>
+    <col min="7" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:255" ht="18" customHeight="1">
@@ -20549,7 +20559,7 @@
       <c r="IT1" s="36"/>
       <c r="IU1" s="36"/>
     </row>
-    <row r="2" spans="1:255" ht="191.25">
+    <row r="2" spans="1:255" ht="196">
       <c r="A2" s="23"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24" t="s">
@@ -21326,14 +21336,14 @@
       <selection activeCell="A4" sqref="A4:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="50.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
-    <col min="6" max="1025" width="8.28515625" customWidth="1"/>
+    <col min="4" max="4" width="50.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="1" customWidth="1"/>
+    <col min="6" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:255" ht="18" customHeight="1">
@@ -21601,7 +21611,7 @@
       <c r="IT1" s="36"/>
       <c r="IU1" s="36"/>
     </row>
-    <row r="2" spans="1:255" ht="89.25">
+    <row r="2" spans="1:255" ht="84">
       <c r="A2" s="23" t="s">
         <v>4</v>
       </c>
@@ -21939,14 +21949,14 @@
       <selection activeCell="A4" sqref="A4:XFD518"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" style="1" customWidth="1"/>
-    <col min="5" max="1011" width="8.28515625" customWidth="1"/>
-    <col min="1012" max="1016" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" style="1" customWidth="1"/>
+    <col min="5" max="1011" width="8.33203125" customWidth="1"/>
+    <col min="1012" max="1016" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -21963,7 +21973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="51">
+    <row r="2" spans="1:4" ht="56">
       <c r="A2" s="24" t="s">
         <v>153</v>
       </c>
@@ -23683,12 +23693,12 @@
       <selection activeCell="A4" sqref="A4:XFD115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -23705,7 +23715,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="63.75">
+    <row r="2" spans="1:4" ht="56">
       <c r="A2" s="24" t="s">
         <v>160</v>
       </c>
@@ -24112,12 +24122,12 @@
       <selection activeCell="A4" sqref="A4:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="53.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="53.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
@@ -24134,7 +24144,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="51">
+    <row r="2" spans="1:4" ht="56">
       <c r="A2" s="24" t="s">
         <v>153</v>
       </c>
@@ -24312,17 +24322,17 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="133" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="133" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" style="133" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" style="133" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="133" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="133" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" style="133" customWidth="1"/>
-    <col min="8" max="1025" width="8.85546875" style="133" customWidth="1"/>
-    <col min="1026" max="16384" width="8.85546875" style="133"/>
+    <col min="1" max="1" width="16.1640625" style="133" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" style="133" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="133" customWidth="1"/>
+    <col min="4" max="4" width="28.5" style="133" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" style="133" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" style="133" customWidth="1"/>
+    <col min="7" max="7" width="24.5" style="133" customWidth="1"/>
+    <col min="8" max="1025" width="8.83203125" style="133" customWidth="1"/>
+    <col min="1026" max="16384" width="8.83203125" style="133"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25.5" customHeight="1">
@@ -24341,7 +24351,7 @@
       <c r="E1" s="240"/>
       <c r="F1" s="240"/>
     </row>
-    <row r="2" spans="1:6" s="236" customFormat="1" ht="38.25">
+    <row r="2" spans="1:6" s="236" customFormat="1" ht="42">
       <c r="A2" s="239" t="s">
         <v>4</v>
       </c>
@@ -24361,7 +24371,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.7" customHeight="1">
+    <row r="3" spans="1:6" ht="13.75" customHeight="1">
       <c r="A3" s="233" t="s">
         <v>9</v>
       </c>
@@ -24381,28 +24391,28 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.7" customHeight="1">
+    <row r="4" spans="1:6" ht="13.75" customHeight="1">
       <c r="A4" s="232"/>
       <c r="B4" s="232"/>
     </row>
-    <row r="5" spans="1:6" ht="13.7" customHeight="1">
+    <row r="5" spans="1:6" ht="13.75" customHeight="1">
       <c r="A5" s="232"/>
       <c r="B5" s="232"/>
     </row>
-    <row r="6" spans="1:6" ht="13.7" customHeight="1">
+    <row r="6" spans="1:6" ht="13.75" customHeight="1">
       <c r="A6" s="232"/>
       <c r="B6" s="232"/>
     </row>
-    <row r="7" spans="1:6" ht="13.7" customHeight="1">
+    <row r="7" spans="1:6" ht="13.75" customHeight="1">
       <c r="A7" s="232"/>
       <c r="B7" s="232"/>
     </row>
-    <row r="8" spans="1:6" ht="13.7" customHeight="1">
+    <row r="8" spans="1:6" ht="13.75" customHeight="1">
       <c r="A8" s="232"/>
       <c r="B8" s="232"/>
     </row>
-    <row r="9" spans="1:6" ht="13.7" customHeight="1"/>
-    <row r="10" spans="1:6" ht="13.7" customHeight="1"/>
+    <row r="9" spans="1:6" ht="13.75" customHeight="1"/>
+    <row r="10" spans="1:6" ht="13.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -24420,11 +24430,11 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="2" width="11.42578125"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="1024" width="11.42578125"/>
+    <col min="1" max="2" width="11.5"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="4" max="1024" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18">
@@ -24442,7 +24452,7 @@
       </c>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:14" ht="127.5">
+    <row r="2" spans="1:14" ht="126">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -24521,14 +24531,14 @@
       <selection activeCell="A4" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="2" width="11.42578125"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="1" max="2" width="11.5"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
     <col min="4" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="61.28515625" customWidth="1"/>
-    <col min="8" max="1025" width="11.42578125"/>
+    <col min="7" max="7" width="61.33203125" customWidth="1"/>
+    <col min="8" max="1025" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18">
@@ -24555,7 +24565,7 @@
       <c r="M1" s="22"/>
       <c r="N1" s="22"/>
     </row>
-    <row r="2" spans="1:19" ht="178.5">
+    <row r="2" spans="1:19" ht="196">
       <c r="A2" s="23" t="s">
         <v>4</v>
       </c>
@@ -24589,7 +24599,7 @@
       <c r="M2" s="26"/>
       <c r="N2" s="26"/>
     </row>
-    <row r="3" spans="1:19" ht="38.25">
+    <row r="3" spans="1:19" ht="42">
       <c r="A3" s="27" t="s">
         <v>9</v>
       </c>
@@ -24669,14 +24679,14 @@
       <selection activeCell="A4" sqref="A4:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="3" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="2" max="3" width="21.33203125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125"/>
-    <col min="6" max="6" width="35.28515625" customWidth="1"/>
-    <col min="7" max="1023" width="11.42578125"/>
+    <col min="5" max="5" width="11.5"/>
+    <col min="6" max="6" width="35.33203125" customWidth="1"/>
+    <col min="7" max="1023" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18">
@@ -24701,7 +24711,7 @@
       <c r="K1" s="22"/>
       <c r="L1" s="22"/>
     </row>
-    <row r="2" spans="1:17" ht="89.25">
+    <row r="2" spans="1:17" ht="98">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
@@ -24727,7 +24737,7 @@
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
     </row>
-    <row r="3" spans="1:17" ht="25.5">
+    <row r="3" spans="1:17" ht="28">
       <c r="A3" s="28" t="s">
         <v>32</v>
       </c>
@@ -24829,19 +24839,19 @@
       <selection activeCell="A4" sqref="A4:XFD98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
     <col min="9" max="9" width="31" customWidth="1"/>
-    <col min="10" max="10" width="26.28515625" customWidth="1"/>
-    <col min="11" max="1023" width="8.7109375" customWidth="1"/>
+    <col min="10" max="10" width="26.33203125" customWidth="1"/>
+    <col min="11" max="1023" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18">
@@ -24899,7 +24909,7 @@
       <c r="K2" s="36"/>
       <c r="L2" s="36"/>
     </row>
-    <row r="3" spans="1:16" ht="38.25">
+    <row r="3" spans="1:16" ht="42">
       <c r="A3" s="40" t="s">
         <v>32</v>
       </c>
@@ -25479,29 +25489,29 @@
       <selection activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="42.28515625" customWidth="1"/>
-    <col min="8" max="8" width="74.7109375" customWidth="1"/>
-    <col min="9" max="9" width="83.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="79.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="88.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="23.28515625" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" customWidth="1"/>
-    <col min="18" max="18" width="20.42578125" customWidth="1"/>
-    <col min="19" max="19" width="17.7109375" customWidth="1"/>
-    <col min="20" max="30" width="8.42578125" customWidth="1"/>
-    <col min="31" max="1024" width="8.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="42.33203125" customWidth="1"/>
+    <col min="8" max="8" width="74.6640625" customWidth="1"/>
+    <col min="9" max="9" width="83.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="79.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="88.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="23.33203125" customWidth="1"/>
+    <col min="14" max="14" width="8.5" customWidth="1"/>
+    <col min="15" max="15" width="18.5" customWidth="1"/>
+    <col min="16" max="16" width="18.5" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" customWidth="1"/>
+    <col min="18" max="18" width="20.5" customWidth="1"/>
+    <col min="19" max="19" width="17.6640625" customWidth="1"/>
+    <col min="20" max="30" width="8.5" customWidth="1"/>
+    <col min="31" max="1024" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">
@@ -25533,7 +25543,7 @@
       <c r="R1" s="39"/>
       <c r="S1" s="39"/>
     </row>
-    <row r="2" spans="1:26" ht="127.5">
+    <row r="2" spans="1:26" ht="126">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
@@ -25577,7 +25587,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="38.25">
+    <row r="3" spans="1:26" ht="42">
       <c r="A3" s="40" t="s">
         <v>32</v>
       </c>
@@ -25645,14 +25655,14 @@
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
     </row>
-    <row r="4" spans="1:26" ht="14.25">
+    <row r="4" spans="1:26" ht="14">
       <c r="I4" s="107"/>
       <c r="L4" s="36"/>
       <c r="M4" s="46"/>
       <c r="R4" s="109"/>
       <c r="S4" s="109"/>
     </row>
-    <row r="5" spans="1:26" ht="14.25">
+    <row r="5" spans="1:26" ht="14">
       <c r="F5" s="2"/>
       <c r="J5" s="107"/>
       <c r="K5" s="36"/>
@@ -25661,7 +25671,7 @@
       <c r="R5" s="109"/>
       <c r="S5" s="109"/>
     </row>
-    <row r="6" spans="1:26" ht="14.25">
+    <row r="6" spans="1:26" ht="14">
       <c r="F6" s="2"/>
       <c r="G6" s="143"/>
       <c r="I6" s="188"/>
@@ -25671,7 +25681,7 @@
       <c r="R6" s="109"/>
       <c r="S6" s="109"/>
     </row>
-    <row r="7" spans="1:26" ht="14.25">
+    <row r="7" spans="1:26" ht="14">
       <c r="F7" s="2"/>
       <c r="G7" s="218"/>
       <c r="H7" s="2"/>
@@ -25682,7 +25692,7 @@
       <c r="R7" s="109"/>
       <c r="S7" s="109"/>
     </row>
-    <row r="8" spans="1:26" ht="14.25">
+    <row r="8" spans="1:26" ht="14">
       <c r="F8" s="2"/>
       <c r="G8" s="218"/>
       <c r="H8" s="2"/>
@@ -25693,7 +25703,7 @@
       <c r="R8" s="109"/>
       <c r="S8" s="109"/>
     </row>
-    <row r="9" spans="1:26" ht="14.25">
+    <row r="9" spans="1:26" ht="14">
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -25705,7 +25715,7 @@
       <c r="R9" s="109"/>
       <c r="S9" s="109"/>
     </row>
-    <row r="10" spans="1:26" ht="14.25">
+    <row r="10" spans="1:26" ht="14">
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -25717,7 +25727,7 @@
       <c r="R10" s="109"/>
       <c r="S10" s="109"/>
     </row>
-    <row r="11" spans="1:26" ht="14.25">
+    <row r="11" spans="1:26" ht="14">
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -25729,7 +25739,7 @@
       <c r="R11" s="109"/>
       <c r="S11" s="109"/>
     </row>
-    <row r="12" spans="1:26" ht="14.25">
+    <row r="12" spans="1:26" ht="14">
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -25741,7 +25751,7 @@
       <c r="R12" s="109"/>
       <c r="S12" s="109"/>
     </row>
-    <row r="13" spans="1:26" ht="14.25">
+    <row r="13" spans="1:26" ht="14">
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -25753,7 +25763,7 @@
       <c r="R13" s="109"/>
       <c r="S13" s="109"/>
     </row>
-    <row r="14" spans="1:26" ht="14.25">
+    <row r="14" spans="1:26" ht="14">
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -25765,7 +25775,7 @@
       <c r="R14" s="109"/>
       <c r="S14" s="109"/>
     </row>
-    <row r="15" spans="1:26" ht="14.25">
+    <row r="15" spans="1:26" ht="14">
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -25777,7 +25787,7 @@
       <c r="R15" s="109"/>
       <c r="S15" s="109"/>
     </row>
-    <row r="16" spans="1:26" ht="14.25">
+    <row r="16" spans="1:26" ht="14">
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -25789,7 +25799,7 @@
       <c r="R16" s="109"/>
       <c r="S16" s="109"/>
     </row>
-    <row r="17" spans="6:19" ht="14.25">
+    <row r="17" spans="6:19" ht="14">
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -25801,7 +25811,7 @@
       <c r="R17" s="109"/>
       <c r="S17" s="109"/>
     </row>
-    <row r="18" spans="6:19" ht="14.25">
+    <row r="18" spans="6:19" ht="14">
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -25812,7 +25822,7 @@
       <c r="R18" s="109"/>
       <c r="S18" s="109"/>
     </row>
-    <row r="19" spans="6:19" ht="14.25">
+    <row r="19" spans="6:19" ht="14">
       <c r="F19" s="2"/>
       <c r="I19" s="115"/>
       <c r="J19" s="141"/>
@@ -25822,7 +25832,7 @@
       <c r="R19" s="109"/>
       <c r="S19" s="109"/>
     </row>
-    <row r="20" spans="6:19" ht="14.25">
+    <row r="20" spans="6:19" ht="14">
       <c r="F20" s="2"/>
       <c r="I20" s="107"/>
       <c r="J20" s="107"/>
@@ -25831,7 +25841,7 @@
       <c r="R20" s="109"/>
       <c r="S20" s="109"/>
     </row>
-    <row r="21" spans="6:19" ht="14.25">
+    <row r="21" spans="6:19" ht="14">
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -25842,7 +25852,7 @@
       <c r="R21" s="109"/>
       <c r="S21" s="109"/>
     </row>
-    <row r="22" spans="6:19" ht="14.25">
+    <row r="22" spans="6:19" ht="14">
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -25854,7 +25864,7 @@
       <c r="R22" s="109"/>
       <c r="S22" s="109"/>
     </row>
-    <row r="23" spans="6:19" ht="14.25">
+    <row r="23" spans="6:19" ht="14">
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -25866,7 +25876,7 @@
       <c r="R23" s="109"/>
       <c r="S23" s="109"/>
     </row>
-    <row r="24" spans="6:19" ht="14.25">
+    <row r="24" spans="6:19" ht="14">
       <c r="J24" s="33"/>
       <c r="L24" s="36"/>
       <c r="M24" s="46"/>
@@ -25874,7 +25884,7 @@
       <c r="R24" s="109"/>
       <c r="S24" s="109"/>
     </row>
-    <row r="25" spans="6:19" ht="14.25">
+    <row r="25" spans="6:19" ht="14">
       <c r="F25" s="2"/>
       <c r="I25" s="107"/>
       <c r="J25" s="107"/>
@@ -25885,7 +25895,7 @@
       <c r="R25" s="109"/>
       <c r="S25" s="109"/>
     </row>
-    <row r="26" spans="6:19" ht="14.25">
+    <row r="26" spans="6:19" ht="14">
       <c r="F26" s="2"/>
       <c r="J26" s="107"/>
       <c r="K26" s="107"/>
@@ -25895,7 +25905,7 @@
       <c r="R26" s="109"/>
       <c r="S26" s="109"/>
     </row>
-    <row r="27" spans="6:19" ht="14.25">
+    <row r="27" spans="6:19" ht="14">
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="I27" s="107"/>
@@ -25906,7 +25916,7 @@
       <c r="R27" s="109"/>
       <c r="S27" s="109"/>
     </row>
-    <row r="28" spans="6:19" ht="14.25">
+    <row r="28" spans="6:19" ht="14">
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="I28" s="107"/>
@@ -25917,7 +25927,7 @@
       <c r="R28" s="109"/>
       <c r="S28" s="109"/>
     </row>
-    <row r="29" spans="6:19" ht="14.25">
+    <row r="29" spans="6:19" ht="14">
       <c r="F29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="107"/>
@@ -25928,7 +25938,7 @@
       <c r="R29" s="109"/>
       <c r="S29" s="109"/>
     </row>
-    <row r="30" spans="6:19" ht="14.25">
+    <row r="30" spans="6:19" ht="14">
       <c r="G30" s="2"/>
       <c r="I30" s="188"/>
       <c r="J30" s="107"/>
@@ -25938,7 +25948,7 @@
       <c r="R30" s="109"/>
       <c r="S30" s="109"/>
     </row>
-    <row r="31" spans="6:19" ht="14.25">
+    <row r="31" spans="6:19" ht="14">
       <c r="J31" s="107"/>
       <c r="K31" s="107"/>
       <c r="L31" s="36"/>
@@ -25947,7 +25957,7 @@
       <c r="R31" s="109"/>
       <c r="S31" s="109"/>
     </row>
-    <row r="32" spans="6:19" ht="14.25">
+    <row r="32" spans="6:19" ht="14">
       <c r="G32" s="2"/>
       <c r="J32" s="107"/>
       <c r="K32" s="107"/>
@@ -25957,7 +25967,7 @@
       <c r="R32" s="109"/>
       <c r="S32" s="109"/>
     </row>
-    <row r="33" spans="1:19" ht="14.25">
+    <row r="33" spans="1:19" ht="14">
       <c r="H33" s="145"/>
       <c r="I33" s="107"/>
       <c r="J33" s="110"/>
@@ -25967,7 +25977,7 @@
       <c r="R33" s="36"/>
       <c r="S33" s="36"/>
     </row>
-    <row r="34" spans="1:19" ht="14.25">
+    <row r="34" spans="1:19" ht="14">
       <c r="I34" s="107"/>
       <c r="J34" s="107"/>
       <c r="L34" s="36"/>
@@ -26071,7 +26081,7 @@
       <c r="R45" s="109"/>
       <c r="S45" s="32"/>
     </row>
-    <row r="46" spans="1:19" ht="14.25">
+    <row r="46" spans="1:19" ht="14">
       <c r="A46" s="120"/>
       <c r="F46" s="111"/>
       <c r="I46" s="107"/>
@@ -26166,21 +26176,21 @@
       <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
     <col min="4" max="5" width="18" customWidth="1"/>
-    <col min="6" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" customWidth="1"/>
+    <col min="6" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="9" width="28.6640625" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="90.28515625" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" customWidth="1"/>
-    <col min="15" max="17" width="8.7109375" customWidth="1"/>
-    <col min="19" max="1011" width="8.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="90.33203125" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" customWidth="1"/>
+    <col min="15" max="17" width="8.6640625" customWidth="1"/>
+    <col min="19" max="1011" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18">
@@ -26262,7 +26272,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="51">
+    <row r="3" spans="1:18" ht="56">
       <c r="A3" s="28" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
ttl related changes added (#856)
* ttl related changes added

* missing columns added to the base template

* pr feedback changes

* ttl added to ET1Repped

* ttl is added for submitEt1Draft

* retain and dispose changes separated out

* ttl-related changes separated out in to non-prod variants

* retain and dispose changes separated out to nonprod files

* Update Auths

* Update CaseEvent with TTL

---------

Co-authored-by: Harpreet Jhita <harpreet.jhita@justice.gov.uk>
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harpreet.jhita/Projects/et-ccd-definitions-scotland/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tensaybulcha/Documents/GitHub/Reformed-ET/et-ccd-definitions-scotland/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC27FCF-15AA-0848-9701-6F6A0CE968CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC4C04A-FD68-494F-9313-B06A081DBDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20620" tabRatio="500" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31700" yWindow="960" windowWidth="39760" windowHeight="15800" tabRatio="500" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SearchParty" sheetId="36" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="25" hidden="1">AuthorisationCaseEvent!$A$3:$D$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">AuthorisationCaseField!$A$1:$D$517</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="26" hidden="1">AuthorisationCaseState!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEvent!$A$3:$Z$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEvent!$A$3:$AB$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseEventToFields!$A$3:$Q$231</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">CaseField!$A$3:$U$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CaseRoles!$A$3:$F$3</definedName>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="394">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1324,6 +1324,21 @@
   </si>
   <si>
     <t>Searchable</t>
+  </si>
+  <si>
+    <t>Marker field for Case deletion when its Time to Live(TTL) value expires</t>
+  </si>
+  <si>
+    <t>EnableForDeletion</t>
+  </si>
+  <si>
+    <t>Magnitude in number of days that a Time to Live(TTL) value is incremented by</t>
+  </si>
+  <si>
+    <t>SignificantEvent</t>
+  </si>
+  <si>
+    <t>TTLIncrement</t>
   </si>
 </sst>
 </file>
@@ -1784,7 +1799,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1807,6 +1822,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF0432FF"/>
         <bgColor rgb="FF0000FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2074,7 +2101,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="304">
+  <cellXfs count="306">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2666,6 +2693,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -4734,7 +4767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:W649"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
@@ -24525,7 +24558,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD6"/>
+      <selection activeCell="J2" sqref="J2:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
@@ -24535,7 +24568,9 @@
     <col min="4" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="61.33203125" customWidth="1"/>
-    <col min="8" max="1025" width="11.5"/>
+    <col min="8" max="9" width="11.5"/>
+    <col min="10" max="10" width="17.1640625" customWidth="1"/>
+    <col min="11" max="1025" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18">
@@ -24590,7 +24625,9 @@
       <c r="I2" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="26"/>
+      <c r="J2" s="25" t="s">
+        <v>389</v>
+      </c>
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
       <c r="M2" s="26"/>
@@ -24624,7 +24661,9 @@
       <c r="I3" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="14"/>
+      <c r="J3" s="304" t="s">
+        <v>390</v>
+      </c>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
       <c r="M3" s="14"/>
@@ -25480,10 +25519,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Z54"/>
+  <dimension ref="A1:AB54"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T1048576"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13"/>
@@ -25503,15 +25542,15 @@
     <col min="13" max="13" width="23.33203125" customWidth="1"/>
     <col min="14" max="14" width="8.5" customWidth="1"/>
     <col min="15" max="15" width="18.5" customWidth="1"/>
-    <col min="16" max="16" width="18.5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.33203125" customWidth="1"/>
-    <col min="18" max="18" width="20.5" customWidth="1"/>
-    <col min="19" max="19" width="17.6640625" customWidth="1"/>
-    <col min="20" max="30" width="8.5" customWidth="1"/>
-    <col min="31" max="1024" width="8.33203125" customWidth="1"/>
+    <col min="16" max="18" width="18.5" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.33203125" customWidth="1"/>
+    <col min="20" max="20" width="20.5" customWidth="1"/>
+    <col min="21" max="21" width="17.6640625" customWidth="1"/>
+    <col min="22" max="32" width="8.5" customWidth="1"/>
+    <col min="33" max="1026" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18" customHeight="1">
+    <row r="1" spans="1:28" ht="18" customHeight="1">
       <c r="A1" s="35" t="s">
         <v>54</v>
       </c>
@@ -25536,11 +25575,13 @@
       <c r="N1" s="36"/>
       <c r="O1" s="36"/>
       <c r="P1" s="36"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
       <c r="S1" s="39"/>
-    </row>
-    <row r="2" spans="1:26" ht="126">
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+    </row>
+    <row r="2" spans="1:28" ht="126">
       <c r="A2" s="24" t="s">
         <v>26</v>
       </c>
@@ -25577,14 +25618,20 @@
       <c r="P2" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
+      <c r="Q2" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="R2" s="23" t="s">
+        <v>391</v>
+      </c>
       <c r="S2" s="25"/>
-      <c r="T2" s="23" t="s">
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="23" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="42">
+    <row r="3" spans="1:28" ht="42">
       <c r="A3" s="40" t="s">
         <v>32</v>
       </c>
@@ -25633,52 +25680,60 @@
       <c r="P3" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="Q3" s="27" t="s">
+      <c r="Q3" s="305" t="s">
+        <v>392</v>
+      </c>
+      <c r="R3" s="305" t="s">
+        <v>393</v>
+      </c>
+      <c r="S3" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="R3" s="27" t="s">
+      <c r="T3" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="S3" s="27" t="s">
+      <c r="U3" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="T3" s="42" t="s">
+      <c r="V3" s="42" t="s">
         <v>387</v>
       </c>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
       <c r="W3" s="14"/>
       <c r="X3" s="14"/>
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
-    </row>
-    <row r="4" spans="1:26" ht="14">
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
+    </row>
+    <row r="4" spans="1:28" ht="14">
       <c r="I4" s="107"/>
       <c r="L4" s="36"/>
       <c r="M4" s="46"/>
-      <c r="R4" s="109"/>
-      <c r="S4" s="109"/>
-    </row>
-    <row r="5" spans="1:26" ht="14">
+      <c r="T4" s="109"/>
+      <c r="U4" s="109"/>
+    </row>
+    <row r="5" spans="1:28" ht="14">
       <c r="F5" s="2"/>
       <c r="J5" s="107"/>
       <c r="K5" s="36"/>
       <c r="L5" s="36"/>
       <c r="M5" s="46"/>
-      <c r="R5" s="109"/>
-      <c r="S5" s="109"/>
-    </row>
-    <row r="6" spans="1:26" ht="14">
+      <c r="T5" s="109"/>
+      <c r="U5" s="109"/>
+    </row>
+    <row r="6" spans="1:28" ht="14">
       <c r="F6" s="2"/>
       <c r="G6" s="143"/>
       <c r="I6" s="188"/>
       <c r="L6" s="36"/>
       <c r="M6" s="46"/>
       <c r="P6" s="46"/>
-      <c r="R6" s="109"/>
-      <c r="S6" s="109"/>
-    </row>
-    <row r="7" spans="1:26" ht="14">
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+      <c r="T6" s="109"/>
+      <c r="U6" s="109"/>
+    </row>
+    <row r="7" spans="1:28" ht="14">
       <c r="F7" s="2"/>
       <c r="G7" s="218"/>
       <c r="H7" s="2"/>
@@ -25686,10 +25741,10 @@
       <c r="J7" s="33"/>
       <c r="L7" s="36"/>
       <c r="M7" s="46"/>
-      <c r="R7" s="109"/>
-      <c r="S7" s="109"/>
-    </row>
-    <row r="8" spans="1:26" ht="14">
+      <c r="T7" s="109"/>
+      <c r="U7" s="109"/>
+    </row>
+    <row r="8" spans="1:28" ht="14">
       <c r="F8" s="2"/>
       <c r="G8" s="218"/>
       <c r="H8" s="2"/>
@@ -25697,10 +25752,10 @@
       <c r="J8" s="33"/>
       <c r="L8" s="36"/>
       <c r="M8" s="46"/>
-      <c r="R8" s="109"/>
-      <c r="S8" s="109"/>
-    </row>
-    <row r="9" spans="1:26" ht="14">
+      <c r="T8" s="109"/>
+      <c r="U8" s="109"/>
+    </row>
+    <row r="9" spans="1:28" ht="14">
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -25709,10 +25764,10 @@
       <c r="K9" s="36"/>
       <c r="L9" s="36"/>
       <c r="M9" s="46"/>
-      <c r="R9" s="109"/>
-      <c r="S9" s="109"/>
-    </row>
-    <row r="10" spans="1:26" ht="14">
+      <c r="T9" s="109"/>
+      <c r="U9" s="109"/>
+    </row>
+    <row r="10" spans="1:28" ht="14">
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -25721,10 +25776,10 @@
       <c r="K10" s="36"/>
       <c r="L10" s="36"/>
       <c r="M10" s="46"/>
-      <c r="R10" s="109"/>
-      <c r="S10" s="109"/>
-    </row>
-    <row r="11" spans="1:26" ht="14">
+      <c r="T10" s="109"/>
+      <c r="U10" s="109"/>
+    </row>
+    <row r="11" spans="1:28" ht="14">
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -25733,10 +25788,10 @@
       <c r="K11" s="36"/>
       <c r="L11" s="36"/>
       <c r="M11" s="46"/>
-      <c r="R11" s="109"/>
-      <c r="S11" s="109"/>
-    </row>
-    <row r="12" spans="1:26" ht="14">
+      <c r="T11" s="109"/>
+      <c r="U11" s="109"/>
+    </row>
+    <row r="12" spans="1:28" ht="14">
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -25745,10 +25800,10 @@
       <c r="K12" s="36"/>
       <c r="L12" s="36"/>
       <c r="M12" s="46"/>
-      <c r="R12" s="109"/>
-      <c r="S12" s="109"/>
-    </row>
-    <row r="13" spans="1:26" ht="14">
+      <c r="T12" s="109"/>
+      <c r="U12" s="109"/>
+    </row>
+    <row r="13" spans="1:28" ht="14">
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -25757,10 +25812,10 @@
       <c r="K13" s="36"/>
       <c r="L13" s="36"/>
       <c r="M13" s="46"/>
-      <c r="R13" s="109"/>
-      <c r="S13" s="109"/>
-    </row>
-    <row r="14" spans="1:26" ht="14">
+      <c r="T13" s="109"/>
+      <c r="U13" s="109"/>
+    </row>
+    <row r="14" spans="1:28" ht="14">
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -25769,10 +25824,10 @@
       <c r="K14" s="36"/>
       <c r="L14" s="36"/>
       <c r="M14" s="46"/>
-      <c r="R14" s="109"/>
-      <c r="S14" s="109"/>
-    </row>
-    <row r="15" spans="1:26" ht="14">
+      <c r="T14" s="109"/>
+      <c r="U14" s="109"/>
+    </row>
+    <row r="15" spans="1:28" ht="14">
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -25781,10 +25836,10 @@
       <c r="K15" s="36"/>
       <c r="L15" s="36"/>
       <c r="M15" s="46"/>
-      <c r="R15" s="109"/>
-      <c r="S15" s="109"/>
-    </row>
-    <row r="16" spans="1:26" ht="14">
+      <c r="T15" s="109"/>
+      <c r="U15" s="109"/>
+    </row>
+    <row r="16" spans="1:28" ht="14">
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -25793,10 +25848,10 @@
       <c r="K16" s="36"/>
       <c r="L16" s="36"/>
       <c r="M16" s="46"/>
-      <c r="R16" s="109"/>
-      <c r="S16" s="109"/>
-    </row>
-    <row r="17" spans="6:19" ht="14">
+      <c r="T16" s="109"/>
+      <c r="U16" s="109"/>
+    </row>
+    <row r="17" spans="6:21" ht="14">
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -25805,10 +25860,10 @@
       <c r="K17" s="36"/>
       <c r="L17" s="36"/>
       <c r="M17" s="46"/>
-      <c r="R17" s="109"/>
-      <c r="S17" s="109"/>
-    </row>
-    <row r="18" spans="6:19" ht="14">
+      <c r="T17" s="109"/>
+      <c r="U17" s="109"/>
+    </row>
+    <row r="18" spans="6:21" ht="14">
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -25816,29 +25871,29 @@
       <c r="J18" s="107"/>
       <c r="L18" s="36"/>
       <c r="M18" s="46"/>
-      <c r="R18" s="109"/>
-      <c r="S18" s="109"/>
-    </row>
-    <row r="19" spans="6:19" ht="14">
+      <c r="T18" s="109"/>
+      <c r="U18" s="109"/>
+    </row>
+    <row r="19" spans="6:21" ht="14">
       <c r="F19" s="2"/>
       <c r="I19" s="115"/>
       <c r="J19" s="141"/>
       <c r="K19" s="36"/>
       <c r="L19" s="36"/>
       <c r="M19" s="46"/>
-      <c r="R19" s="109"/>
-      <c r="S19" s="109"/>
-    </row>
-    <row r="20" spans="6:19" ht="14">
+      <c r="T19" s="109"/>
+      <c r="U19" s="109"/>
+    </row>
+    <row r="20" spans="6:21" ht="14">
       <c r="F20" s="2"/>
       <c r="I20" s="107"/>
       <c r="J20" s="107"/>
       <c r="L20" s="36"/>
       <c r="M20" s="46"/>
-      <c r="R20" s="109"/>
-      <c r="S20" s="109"/>
-    </row>
-    <row r="21" spans="6:19" ht="14">
+      <c r="T20" s="109"/>
+      <c r="U20" s="109"/>
+    </row>
+    <row r="21" spans="6:21" ht="14">
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -25846,10 +25901,10 @@
       <c r="J21" s="109"/>
       <c r="L21" s="36"/>
       <c r="M21" s="46"/>
-      <c r="R21" s="109"/>
-      <c r="S21" s="109"/>
-    </row>
-    <row r="22" spans="6:19" ht="14">
+      <c r="T21" s="109"/>
+      <c r="U21" s="109"/>
+    </row>
+    <row r="22" spans="6:21" ht="14">
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -25858,10 +25913,10 @@
       <c r="K22" s="36"/>
       <c r="L22" s="36"/>
       <c r="M22" s="46"/>
-      <c r="R22" s="109"/>
-      <c r="S22" s="109"/>
-    </row>
-    <row r="23" spans="6:19" ht="14">
+      <c r="T22" s="109"/>
+      <c r="U22" s="109"/>
+    </row>
+    <row r="23" spans="6:21" ht="14">
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -25870,18 +25925,20 @@
       <c r="K23" s="36"/>
       <c r="L23" s="36"/>
       <c r="M23" s="46"/>
-      <c r="R23" s="109"/>
-      <c r="S23" s="109"/>
-    </row>
-    <row r="24" spans="6:19" ht="14">
+      <c r="T23" s="109"/>
+      <c r="U23" s="109"/>
+    </row>
+    <row r="24" spans="6:21" ht="14">
       <c r="J24" s="33"/>
       <c r="L24" s="36"/>
       <c r="M24" s="46"/>
       <c r="P24" s="46"/>
-      <c r="R24" s="109"/>
-      <c r="S24" s="109"/>
-    </row>
-    <row r="25" spans="6:19" ht="14">
+      <c r="Q24" s="46"/>
+      <c r="R24" s="46"/>
+      <c r="T24" s="109"/>
+      <c r="U24" s="109"/>
+    </row>
+    <row r="25" spans="6:21" ht="14">
       <c r="F25" s="2"/>
       <c r="I25" s="107"/>
       <c r="J25" s="107"/>
@@ -25889,20 +25946,24 @@
       <c r="L25" s="36"/>
       <c r="M25" s="46"/>
       <c r="P25" s="46"/>
-      <c r="R25" s="109"/>
-      <c r="S25" s="109"/>
-    </row>
-    <row r="26" spans="6:19" ht="14">
+      <c r="Q25" s="46"/>
+      <c r="R25" s="46"/>
+      <c r="T25" s="109"/>
+      <c r="U25" s="109"/>
+    </row>
+    <row r="26" spans="6:21" ht="14">
       <c r="F26" s="2"/>
       <c r="J26" s="107"/>
       <c r="K26" s="107"/>
       <c r="L26" s="36"/>
       <c r="M26" s="46"/>
       <c r="P26" s="46"/>
-      <c r="R26" s="109"/>
-      <c r="S26" s="109"/>
-    </row>
-    <row r="27" spans="6:19" ht="14">
+      <c r="Q26" s="46"/>
+      <c r="R26" s="46"/>
+      <c r="T26" s="109"/>
+      <c r="U26" s="109"/>
+    </row>
+    <row r="27" spans="6:21" ht="14">
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="I27" s="107"/>
@@ -25910,10 +25971,12 @@
       <c r="L27" s="36"/>
       <c r="M27" s="46"/>
       <c r="P27" s="46"/>
-      <c r="R27" s="109"/>
-      <c r="S27" s="109"/>
-    </row>
-    <row r="28" spans="6:19" ht="14">
+      <c r="Q27" s="46"/>
+      <c r="R27" s="46"/>
+      <c r="T27" s="109"/>
+      <c r="U27" s="109"/>
+    </row>
+    <row r="28" spans="6:21" ht="14">
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="I28" s="107"/>
@@ -25921,10 +25984,12 @@
       <c r="L28" s="36"/>
       <c r="M28" s="46"/>
       <c r="P28" s="46"/>
-      <c r="R28" s="109"/>
-      <c r="S28" s="109"/>
-    </row>
-    <row r="29" spans="6:19" ht="14">
+      <c r="Q28" s="46"/>
+      <c r="R28" s="46"/>
+      <c r="T28" s="109"/>
+      <c r="U28" s="109"/>
+    </row>
+    <row r="29" spans="6:21" ht="14">
       <c r="F29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="107"/>
@@ -25932,96 +25997,100 @@
       <c r="K29" s="33"/>
       <c r="L29" s="36"/>
       <c r="M29" s="46"/>
-      <c r="R29" s="109"/>
-      <c r="S29" s="109"/>
-    </row>
-    <row r="30" spans="6:19" ht="14">
+      <c r="T29" s="109"/>
+      <c r="U29" s="109"/>
+    </row>
+    <row r="30" spans="6:21" ht="14">
       <c r="G30" s="2"/>
       <c r="I30" s="188"/>
       <c r="J30" s="107"/>
       <c r="K30" s="33"/>
       <c r="L30" s="36"/>
       <c r="M30" s="46"/>
-      <c r="R30" s="109"/>
-      <c r="S30" s="109"/>
-    </row>
-    <row r="31" spans="6:19" ht="14">
+      <c r="T30" s="109"/>
+      <c r="U30" s="109"/>
+    </row>
+    <row r="31" spans="6:21" ht="14">
       <c r="J31" s="107"/>
       <c r="K31" s="107"/>
       <c r="L31" s="36"/>
       <c r="M31" s="46"/>
       <c r="P31" s="46"/>
-      <c r="R31" s="109"/>
-      <c r="S31" s="109"/>
-    </row>
-    <row r="32" spans="6:19" ht="14">
+      <c r="Q31" s="46"/>
+      <c r="R31" s="46"/>
+      <c r="T31" s="109"/>
+      <c r="U31" s="109"/>
+    </row>
+    <row r="32" spans="6:21" ht="14">
       <c r="G32" s="2"/>
       <c r="J32" s="107"/>
       <c r="K32" s="107"/>
       <c r="L32" s="36"/>
       <c r="M32" s="46"/>
       <c r="P32" s="46"/>
-      <c r="R32" s="109"/>
-      <c r="S32" s="109"/>
-    </row>
-    <row r="33" spans="1:19" ht="14">
+      <c r="Q32" s="46"/>
+      <c r="R32" s="46"/>
+      <c r="T32" s="109"/>
+      <c r="U32" s="109"/>
+    </row>
+    <row r="33" spans="1:21" ht="14">
       <c r="H33" s="145"/>
       <c r="I33" s="107"/>
       <c r="J33" s="110"/>
       <c r="L33" s="36"/>
       <c r="M33" s="46"/>
-      <c r="Q33" s="36"/>
-      <c r="R33" s="36"/>
       <c r="S33" s="36"/>
-    </row>
-    <row r="34" spans="1:19" ht="14">
+      <c r="T33" s="36"/>
+      <c r="U33" s="36"/>
+    </row>
+    <row r="34" spans="1:21" ht="14">
       <c r="I34" s="107"/>
       <c r="J34" s="107"/>
       <c r="L34" s="36"/>
       <c r="M34" s="46"/>
-      <c r="Q34" s="36"/>
-      <c r="R34" s="36"/>
       <c r="S34" s="36"/>
-    </row>
-    <row r="35" spans="1:19">
+      <c r="T34" s="36"/>
+      <c r="U34" s="36"/>
+    </row>
+    <row r="35" spans="1:21">
       <c r="J35" s="115"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="1:19">
+    <row r="36" spans="1:21">
       <c r="J36" s="115"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="1:21">
       <c r="I37" s="107"/>
       <c r="J37" s="107"/>
       <c r="K37" s="107"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="1:19">
+    <row r="38" spans="1:21">
       <c r="F38" s="111"/>
       <c r="G38" s="111"/>
       <c r="J38" s="110"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="1:19">
+    <row r="39" spans="1:21">
       <c r="F39" s="111"/>
       <c r="G39" s="111"/>
       <c r="J39" s="107"/>
       <c r="K39" s="107"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="1:19">
+    <row r="40" spans="1:21">
       <c r="A40" s="45"/>
       <c r="I40" s="107"/>
       <c r="J40" s="107"/>
       <c r="K40" s="107"/>
       <c r="L40" s="36"/>
       <c r="M40" s="1"/>
-      <c r="Q40" s="32"/>
-      <c r="R40" s="109"/>
       <c r="S40" s="32"/>
-    </row>
-    <row r="41" spans="1:19">
+      <c r="T40" s="109"/>
+      <c r="U40" s="32"/>
+    </row>
+    <row r="41" spans="1:21">
       <c r="A41" s="47"/>
       <c r="I41" s="107"/>
       <c r="J41" s="107"/>
@@ -26029,44 +26098,46 @@
       <c r="L41" s="36"/>
       <c r="M41" s="48"/>
       <c r="P41" s="48"/>
-      <c r="Q41" s="32"/>
-      <c r="R41" s="109"/>
+      <c r="Q41" s="48"/>
+      <c r="R41" s="48"/>
       <c r="S41" s="32"/>
-    </row>
-    <row r="42" spans="1:19">
+      <c r="T41" s="109"/>
+      <c r="U41" s="32"/>
+    </row>
+    <row r="42" spans="1:21">
       <c r="A42" s="47"/>
       <c r="I42" s="107"/>
       <c r="J42" s="107"/>
       <c r="K42" s="107"/>
       <c r="L42" s="36"/>
       <c r="M42" s="1"/>
-      <c r="Q42" s="32"/>
-      <c r="R42" s="109"/>
       <c r="S42" s="32"/>
-    </row>
-    <row r="43" spans="1:19">
+      <c r="T42" s="109"/>
+      <c r="U42" s="32"/>
+    </row>
+    <row r="43" spans="1:21">
       <c r="A43" s="47"/>
       <c r="I43" s="107"/>
       <c r="J43" s="107"/>
       <c r="K43" s="107"/>
       <c r="L43" s="36"/>
       <c r="M43" s="1"/>
-      <c r="Q43" s="32"/>
-      <c r="R43" s="109"/>
       <c r="S43" s="32"/>
-    </row>
-    <row r="44" spans="1:19">
+      <c r="T43" s="109"/>
+      <c r="U43" s="32"/>
+    </row>
+    <row r="44" spans="1:21">
       <c r="A44" s="47"/>
       <c r="I44" s="107"/>
       <c r="J44" s="107"/>
       <c r="K44" s="107"/>
       <c r="L44" s="36"/>
       <c r="M44" s="1"/>
-      <c r="Q44" s="32"/>
-      <c r="R44" s="109"/>
       <c r="S44" s="32"/>
-    </row>
-    <row r="45" spans="1:19">
+      <c r="T44" s="109"/>
+      <c r="U44" s="32"/>
+    </row>
+    <row r="45" spans="1:21">
       <c r="A45" s="120"/>
       <c r="I45" s="107"/>
       <c r="J45" s="107"/>
@@ -26074,11 +26145,13 @@
       <c r="L45" s="36"/>
       <c r="M45" s="48"/>
       <c r="P45" s="48"/>
-      <c r="Q45" s="32"/>
-      <c r="R45" s="109"/>
+      <c r="Q45" s="48"/>
+      <c r="R45" s="48"/>
       <c r="S45" s="32"/>
-    </row>
-    <row r="46" spans="1:19" ht="14">
+      <c r="T45" s="109"/>
+      <c r="U45" s="32"/>
+    </row>
+    <row r="46" spans="1:21" ht="14">
       <c r="A46" s="120"/>
       <c r="F46" s="111"/>
       <c r="I46" s="107"/>
@@ -26086,11 +26159,11 @@
       <c r="K46" s="107"/>
       <c r="L46" s="36"/>
       <c r="M46" s="46"/>
-      <c r="Q46" s="109"/>
-      <c r="R46" s="107"/>
       <c r="S46" s="109"/>
-    </row>
-    <row r="47" spans="1:19">
+      <c r="T46" s="107"/>
+      <c r="U46" s="109"/>
+    </row>
+    <row r="47" spans="1:21">
       <c r="A47" s="120"/>
       <c r="F47" s="111"/>
       <c r="I47" s="107"/>
@@ -26098,9 +26171,9 @@
       <c r="K47" s="107"/>
       <c r="L47" s="36"/>
       <c r="M47" s="48"/>
-      <c r="Q47" s="32"/>
-    </row>
-    <row r="48" spans="1:19">
+      <c r="S47" s="32"/>
+    </row>
+    <row r="48" spans="1:21">
       <c r="A48" s="120"/>
       <c r="C48" s="143"/>
       <c r="F48" s="111"/>
@@ -26110,7 +26183,7 @@
       <c r="L48" s="36"/>
       <c r="M48" s="48"/>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:18">
       <c r="A49" s="120"/>
       <c r="F49" s="111"/>
       <c r="I49" s="107"/>
@@ -26119,7 +26192,7 @@
       <c r="L49" s="36"/>
       <c r="M49" s="48"/>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:18">
       <c r="A50" s="120"/>
       <c r="I50" s="107"/>
       <c r="J50" s="141"/>
@@ -26127,7 +26200,7 @@
       <c r="L50" s="36"/>
       <c r="M50" s="48"/>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:18">
       <c r="A51" s="120"/>
       <c r="I51" s="107"/>
       <c r="J51" s="107"/>
@@ -26135,14 +26208,14 @@
       <c r="L51" s="36"/>
       <c r="M51" s="48"/>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:18">
       <c r="I52" s="107"/>
       <c r="J52" s="107"/>
       <c r="K52" s="107"/>
       <c r="L52" s="36"/>
       <c r="M52" s="48"/>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:18">
       <c r="A53" s="120"/>
       <c r="I53" s="41"/>
       <c r="J53" s="107"/>
@@ -26150,11 +26223,13 @@
       <c r="L53" s="36"/>
       <c r="M53" s="1"/>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:18">
       <c r="J54" s="107"/>
       <c r="L54" s="36"/>
       <c r="M54" s="48"/>
       <c r="P54"/>
+      <c r="Q54"/>
+      <c r="R54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>